<commit_message>
Add moscow, add stavr
</commit_message>
<xml_diff>
--- a/id.xlsx
+++ b/id.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="634">
   <si>
     <t>Aito</t>
   </si>
@@ -1923,6 +1923,12 @@
   </si>
   <si>
     <t>T9</t>
+  </si>
+  <si>
+    <t>JS3 New</t>
+  </si>
+  <si>
+    <t>H9 New</t>
   </si>
 </sst>
 </file>
@@ -1935,14 +1941,7 @@
     <numFmt numFmtId="178" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2398,28 +2397,31 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2428,118 +2430,115 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2891,10 +2890,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C583"/>
+  <dimension ref="A1:C585"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A564" workbookViewId="0">
-      <selection activeCell="F580" sqref="F580"/>
+      <selection activeCell="M579" sqref="M579"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -9312,6 +9311,28 @@
         <v>631</v>
       </c>
     </row>
+    <row r="584" spans="1:3">
+      <c r="A584">
+        <v>683</v>
+      </c>
+      <c r="B584" t="s">
+        <v>258</v>
+      </c>
+      <c r="C584" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="585" spans="1:3">
+      <c r="A585">
+        <v>684</v>
+      </c>
+      <c r="B585" t="s">
+        <v>207</v>
+      </c>
+      <c r="C585" t="s">
+        <v>633</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add json vlg, chelyaba, cheboksari
</commit_message>
<xml_diff>
--- a/id.xlsx
+++ b/id.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="649">
   <si>
     <t>Aito</t>
   </si>
@@ -1169,7 +1169,7 @@
     <t>Largus 7 мест</t>
   </si>
   <si>
-    <t>Фургон New</t>
+    <t>Largus Фургон New</t>
   </si>
   <si>
     <t>Lifan</t>
@@ -1929,6 +1929,51 @@
   </si>
   <si>
     <t>H9 New</t>
+  </si>
+  <si>
+    <t>ASX</t>
+  </si>
+  <si>
+    <t>Largus CNG</t>
+  </si>
+  <si>
+    <t>Largus Cross CNG</t>
+  </si>
+  <si>
+    <t>Largus Фургон CNG</t>
+  </si>
+  <si>
+    <t>M6 New</t>
+  </si>
+  <si>
+    <t>Jimny</t>
+  </si>
+  <si>
+    <t>DFM AX7</t>
+  </si>
+  <si>
+    <t>Vesta Sedan New NG</t>
+  </si>
+  <si>
+    <t>3909 Бортовой грузовик</t>
+  </si>
+  <si>
+    <t>3909 Микроавтобус</t>
+  </si>
+  <si>
+    <t>3909 Скорая помощь</t>
+  </si>
+  <si>
+    <t>3909 Цельнометаллический фургон</t>
+  </si>
+  <si>
+    <t>Профи</t>
+  </si>
+  <si>
+    <t>ВИС</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4x4 3 двери </t>
   </si>
 </sst>
 </file>
@@ -2890,10 +2935,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C585"/>
+  <dimension ref="A1:C602"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A564" workbookViewId="0">
-      <selection activeCell="M579" sqref="M579"/>
+    <sheetView tabSelected="1" topLeftCell="A587" workbookViewId="0">
+      <selection activeCell="K604" sqref="K604"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -9333,6 +9378,193 @@
         <v>633</v>
       </c>
     </row>
+    <row r="586" spans="1:3">
+      <c r="A586">
+        <v>685</v>
+      </c>
+      <c r="B586" t="s">
+        <v>424</v>
+      </c>
+      <c r="C586" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="587" spans="1:3">
+      <c r="A587">
+        <v>686</v>
+      </c>
+      <c r="B587" t="s">
+        <v>327</v>
+      </c>
+      <c r="C587" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="588" spans="1:3">
+      <c r="A588">
+        <v>687</v>
+      </c>
+      <c r="B588" t="s">
+        <v>327</v>
+      </c>
+      <c r="C588" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="589" spans="1:3">
+      <c r="A589">
+        <v>688</v>
+      </c>
+      <c r="B589" t="s">
+        <v>327</v>
+      </c>
+      <c r="C589" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="590" spans="1:3">
+      <c r="A590">
+        <v>689</v>
+      </c>
+      <c r="B590" t="s">
+        <v>207</v>
+      </c>
+      <c r="C590" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="591" spans="1:3">
+      <c r="A591">
+        <v>690</v>
+      </c>
+      <c r="B591" t="s">
+        <v>543</v>
+      </c>
+      <c r="C591" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="592" spans="1:3">
+      <c r="A592">
+        <v>691</v>
+      </c>
+      <c r="B592" t="s">
+        <v>192</v>
+      </c>
+      <c r="C592" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="593" spans="1:3">
+      <c r="A593">
+        <v>692</v>
+      </c>
+      <c r="B593" t="s">
+        <v>97</v>
+      </c>
+      <c r="C593" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="594" spans="1:3">
+      <c r="A594">
+        <v>693</v>
+      </c>
+      <c r="B594" t="s">
+        <v>327</v>
+      </c>
+      <c r="C594" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="595" spans="1:3">
+      <c r="A595">
+        <v>694</v>
+      </c>
+      <c r="B595" t="s">
+        <v>575</v>
+      </c>
+      <c r="C595">
+        <v>3909</v>
+      </c>
+    </row>
+    <row r="596" spans="1:3">
+      <c r="A596">
+        <v>695</v>
+      </c>
+      <c r="B596" t="s">
+        <v>575</v>
+      </c>
+      <c r="C596" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="597" spans="1:3">
+      <c r="A597">
+        <v>696</v>
+      </c>
+      <c r="B597" t="s">
+        <v>575</v>
+      </c>
+      <c r="C597" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="598" spans="1:3">
+      <c r="A598">
+        <v>697</v>
+      </c>
+      <c r="B598" t="s">
+        <v>575</v>
+      </c>
+      <c r="C598" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="599" spans="1:3">
+      <c r="A599">
+        <v>698</v>
+      </c>
+      <c r="B599" t="s">
+        <v>575</v>
+      </c>
+      <c r="C599" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="600" spans="1:3">
+      <c r="A600">
+        <v>699</v>
+      </c>
+      <c r="B600" t="s">
+        <v>575</v>
+      </c>
+      <c r="C600" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="601" spans="1:3">
+      <c r="A601">
+        <v>700</v>
+      </c>
+      <c r="B601" t="s">
+        <v>327</v>
+      </c>
+      <c r="C601" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="602" spans="1:3">
+      <c r="A602">
+        <v>701</v>
+      </c>
+      <c r="B602" t="s">
+        <v>327</v>
+      </c>
+      <c r="C602" t="s">
+        <v>648</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add h9 new, preface new
</commit_message>
<xml_diff>
--- a/id.xlsx
+++ b/id.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="691">
   <si>
     <t>Aito</t>
   </si>
@@ -2097,6 +2097,9 @@
   </si>
   <si>
     <t>U5 Plus CNG</t>
+  </si>
+  <si>
+    <t>Preface New</t>
   </si>
 </sst>
 </file>
@@ -3058,7 +3061,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C643"/>
+  <dimension ref="A1:C644"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A620" workbookViewId="0">
       <selection activeCell="H640" sqref="H640"/>
@@ -10139,6 +10142,17 @@
         <v>689</v>
       </c>
     </row>
+    <row r="644" spans="1:3">
+      <c r="A644">
+        <v>743</v>
+      </c>
+      <c r="B644" t="s">
+        <v>168</v>
+      </c>
+      <c r="C644" t="s">
+        <v>690</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add 6 sites, del 5 sites, add 1 car
</commit_message>
<xml_diff>
--- a/id.xlsx
+++ b/id.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9000"/>
+    <workbookView windowWidth="22188" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="733">
   <si>
     <t>Aito</t>
   </si>
@@ -2214,6 +2214,18 @@
   </si>
   <si>
     <t>01</t>
+  </si>
+  <si>
+    <t>K3</t>
+  </si>
+  <si>
+    <t>Maxus</t>
+  </si>
+  <si>
+    <t>Territory</t>
+  </si>
+  <si>
+    <t>Mega</t>
   </si>
 </sst>
 </file>
@@ -3177,10 +3189,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C690"/>
+  <dimension ref="A1:C693"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A669" workbookViewId="0">
-      <selection activeCell="G686" sqref="G686"/>
+      <selection activeCell="M683" sqref="M683"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -10775,6 +10787,39 @@
         <v>728</v>
       </c>
     </row>
+    <row r="691" spans="1:3">
+      <c r="A691">
+        <v>790</v>
+      </c>
+      <c r="B691" t="s">
+        <v>287</v>
+      </c>
+      <c r="C691" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="692" spans="1:3">
+      <c r="A692">
+        <v>791</v>
+      </c>
+      <c r="B692" t="s">
+        <v>730</v>
+      </c>
+      <c r="C692" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="693" spans="1:3">
+      <c r="A693">
+        <v>792</v>
+      </c>
+      <c r="B693" t="s">
+        <v>392</v>
+      </c>
+      <c r="C693" t="s">
+        <v>732</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add 4 sites - samara(1)
</commit_message>
<xml_diff>
--- a/id.xlsx
+++ b/id.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="768">
   <si>
     <t>Aito</t>
   </si>
@@ -2328,6 +2328,9 @@
   </si>
   <si>
     <t>Granta Sportline Drive Active Liftback</t>
+  </si>
+  <si>
+    <t>Pickup АКПП</t>
   </si>
 </sst>
 </file>
@@ -3291,10 +3294,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C728"/>
+  <dimension ref="A1:C729"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A703" workbookViewId="0">
-      <selection activeCell="H718" sqref="H718"/>
+      <selection activeCell="E722" sqref="E722"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -11307,6 +11310,17 @@
         <v>766</v>
       </c>
     </row>
+    <row r="729" spans="1:3">
+      <c r="A729">
+        <v>828</v>
+      </c>
+      <c r="B729" t="s">
+        <v>575</v>
+      </c>
+      <c r="C729" t="s">
+        <v>767</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Fix 2 sites, add 5 cars
</commit_message>
<xml_diff>
--- a/id.xlsx
+++ b/id.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$C$736</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="772">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="777">
   <si>
     <t>Aito</t>
   </si>
@@ -2343,6 +2346,21 @@
   </si>
   <si>
     <t>Tiggo 9 New</t>
+  </si>
+  <si>
+    <t>Bestune T90 New</t>
+  </si>
+  <si>
+    <t>RX 5</t>
+  </si>
+  <si>
+    <t>Monjaro New</t>
+  </si>
+  <si>
+    <t>i20</t>
+  </si>
+  <si>
+    <t>Carnival New</t>
   </si>
 </sst>
 </file>
@@ -3306,10 +3324,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C733"/>
+  <dimension ref="A1:C738"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A709" workbookViewId="0">
-      <selection activeCell="F719" sqref="F719"/>
+    <sheetView tabSelected="1" topLeftCell="A715" workbookViewId="0">
+      <selection activeCell="H730" sqref="H730"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -11377,7 +11395,65 @@
         <v>771</v>
       </c>
     </row>
+    <row r="734" spans="1:3">
+      <c r="A734">
+        <v>833</v>
+      </c>
+      <c r="B734" t="s">
+        <v>126</v>
+      </c>
+      <c r="C734" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="735" spans="1:3">
+      <c r="A735">
+        <v>834</v>
+      </c>
+      <c r="B735" t="s">
+        <v>417</v>
+      </c>
+      <c r="C735" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="736" spans="1:3">
+      <c r="A736">
+        <v>835</v>
+      </c>
+      <c r="B736" t="s">
+        <v>168</v>
+      </c>
+      <c r="C736" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="737" spans="1:3">
+      <c r="A737">
+        <v>836</v>
+      </c>
+      <c r="B737" t="s">
+        <v>233</v>
+      </c>
+      <c r="C737" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="738" spans="1:3">
+      <c r="A738">
+        <v>837</v>
+      </c>
+      <c r="B738" t="s">
+        <v>287</v>
+      </c>
+      <c r="C738" t="s">
+        <v>776</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:C736" etc:filterBottomFollowUsedRange="0">
+    <extLst/>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Add 5 sites, yaroslavl
</commit_message>
<xml_diff>
--- a/id.xlsx
+++ b/id.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$C$736</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$C$741</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="781">
   <si>
     <t>Aito</t>
   </si>
@@ -2361,6 +2361,18 @@
   </si>
   <si>
     <t>Carnival New</t>
+  </si>
+  <si>
+    <t>Juke New</t>
+  </si>
+  <si>
+    <t>Raeton</t>
+  </si>
+  <si>
+    <t>Besturn B70</t>
+  </si>
+  <si>
+    <t>RX 9</t>
   </si>
 </sst>
 </file>
@@ -3324,10 +3336,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C738"/>
+  <dimension ref="A1:C742"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A715" workbookViewId="0">
-      <selection activeCell="H730" sqref="H730"/>
+      <selection activeCell="O730" sqref="O730"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -11450,8 +11462,52 @@
         <v>776</v>
       </c>
     </row>
+    <row r="739" spans="1:3">
+      <c r="A739">
+        <v>838</v>
+      </c>
+      <c r="B739" t="s">
+        <v>440</v>
+      </c>
+      <c r="C739" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="740" spans="1:3">
+      <c r="A740">
+        <v>839</v>
+      </c>
+      <c r="B740" t="s">
+        <v>20</v>
+      </c>
+      <c r="C740" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="741" spans="1:3">
+      <c r="A741">
+        <v>840</v>
+      </c>
+      <c r="B741" t="s">
+        <v>126</v>
+      </c>
+      <c r="C741" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="742" spans="1:3">
+      <c r="A742">
+        <v>841</v>
+      </c>
+      <c r="B742" t="s">
+        <v>417</v>
+      </c>
+      <c r="C742" t="s">
+        <v>780</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:C736" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:C741" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add 10 cars, Fix ufamasmotors - 40 min
</commit_message>
<xml_diff>
--- a/id.xlsx
+++ b/id.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9060"/>
+    <workbookView windowWidth="22188" windowHeight="8615"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$C$776</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$C$781</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1553" uniqueCount="817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="819">
   <si>
     <t>Aito</t>
   </si>
@@ -2481,6 +2481,12 @@
   </si>
   <si>
     <t>Torres</t>
+  </si>
+  <si>
+    <t>EX5</t>
+  </si>
+  <si>
+    <t>Outlander 7 мест</t>
   </si>
 </sst>
 </file>
@@ -3444,10 +3450,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C781"/>
+  <dimension ref="A1:C783"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A757" workbookViewId="0">
-      <selection activeCell="A783" sqref="A783"/>
+    <sheetView tabSelected="1" topLeftCell="A769" workbookViewId="0">
+      <selection activeCell="E779" sqref="E779"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -12043,8 +12049,30 @@
         <v>816</v>
       </c>
     </row>
+    <row r="782" spans="1:3">
+      <c r="A782">
+        <v>881</v>
+      </c>
+      <c r="B782" t="s">
+        <v>168</v>
+      </c>
+      <c r="C782" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="783" spans="1:3">
+      <c r="A783">
+        <v>882</v>
+      </c>
+      <c r="B783" t="s">
+        <v>581</v>
+      </c>
+      <c r="C783" t="s">
+        <v>818</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:C776" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:C781" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fix kosmos.car, alpha-tank, add 7 cars
</commit_message>
<xml_diff>
--- a/id.xlsx
+++ b/id.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="8615"/>
+    <workbookView windowWidth="22188" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$C$781</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$C$787</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1565" uniqueCount="823">
   <si>
     <t>Aito</t>
   </si>
@@ -2487,6 +2487,18 @@
   </si>
   <si>
     <t>Outlander 7 мест</t>
+  </si>
+  <si>
+    <t>Elantra New Rest</t>
+  </si>
+  <si>
+    <t>Sonata New Rest</t>
+  </si>
+  <si>
+    <t>Soul New Rest</t>
+  </si>
+  <si>
+    <t>HT-i</t>
   </si>
 </sst>
 </file>
@@ -3450,10 +3462,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C783"/>
+  <dimension ref="A1:C787"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A769" workbookViewId="0">
-      <selection activeCell="E779" sqref="E779"/>
+    <sheetView tabSelected="1" topLeftCell="A760" workbookViewId="0">
+      <selection activeCell="C789" sqref="C789"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -12071,8 +12083,52 @@
         <v>818</v>
       </c>
     </row>
+    <row r="784" spans="1:3">
+      <c r="A784">
+        <v>883</v>
+      </c>
+      <c r="B784" t="s">
+        <v>233</v>
+      </c>
+      <c r="C784" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="785" spans="1:3">
+      <c r="A785">
+        <v>884</v>
+      </c>
+      <c r="B785" t="s">
+        <v>233</v>
+      </c>
+      <c r="C785" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="786" spans="1:3">
+      <c r="A786">
+        <v>885</v>
+      </c>
+      <c r="B786" t="s">
+        <v>287</v>
+      </c>
+      <c r="C786" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="787" spans="1:3">
+      <c r="A787">
+        <v>886</v>
+      </c>
+      <c r="B787" t="s">
+        <v>505</v>
+      </c>
+      <c r="C787" t="s">
+        <v>822</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:C781" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:C787" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add kemerovo, del 8 sites
</commit_message>
<xml_diff>
--- a/id.xlsx
+++ b/id.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1565" uniqueCount="823">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1571" uniqueCount="827">
   <si>
     <t>Aito</t>
   </si>
@@ -2499,6 +2499,18 @@
   </si>
   <si>
     <t>HT-i</t>
+  </si>
+  <si>
+    <t>Land Rover</t>
+  </si>
+  <si>
+    <t>Discovery Sport</t>
+  </si>
+  <si>
+    <t>Hiace</t>
+  </si>
+  <si>
+    <t>Land Cruiser 200</t>
   </si>
 </sst>
 </file>
@@ -3462,10 +3474,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C787"/>
+  <dimension ref="A1:C790"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A760" workbookViewId="0">
-      <selection activeCell="C789" sqref="C789"/>
+    <sheetView tabSelected="1" topLeftCell="A772" workbookViewId="0">
+      <selection activeCell="C790" sqref="C790"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -12125,6 +12137,39 @@
       </c>
       <c r="C787" t="s">
         <v>822</v>
+      </c>
+    </row>
+    <row r="788" spans="1:3">
+      <c r="A788">
+        <v>887</v>
+      </c>
+      <c r="B788" t="s">
+        <v>823</v>
+      </c>
+      <c r="C788" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="789" spans="1:3">
+      <c r="A789">
+        <v>888</v>
+      </c>
+      <c r="B789" t="s">
+        <v>557</v>
+      </c>
+      <c r="C789" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="790" spans="1:3">
+      <c r="A790">
+        <v>889</v>
+      </c>
+      <c r="B790" t="s">
+        <v>557</v>
+      </c>
+      <c r="C790" t="s">
+        <v>826</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 2 sites spb, fix omsk, del 3 sites
</commit_message>
<xml_diff>
--- a/id.xlsx
+++ b/id.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$E$876</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$E$878</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Лист2!$A$1:$E$249</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2757" uniqueCount="1041">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2761" uniqueCount="1043">
   <si>
     <t>Aito</t>
   </si>
@@ -2759,6 +2759,12 @@
   </si>
   <si>
     <t>TXL 2</t>
+  </si>
+  <si>
+    <t>500 New</t>
+  </si>
+  <si>
+    <t>GS4</t>
   </si>
   <si>
     <t>Марка</t>
@@ -4145,10 +4151,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F877"/>
+  <dimension ref="A1:F879"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A860" workbookViewId="0">
-      <selection activeCell="G881" sqref="G881"/>
+      <selection activeCell="H866" sqref="H866"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -15240,8 +15246,30 @@
         <v>908</v>
       </c>
     </row>
+    <row r="878" spans="1:3">
+      <c r="A878">
+        <v>977</v>
+      </c>
+      <c r="B878" t="s">
+        <v>555</v>
+      </c>
+      <c r="C878" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="879" spans="1:3">
+      <c r="A879">
+        <v>978</v>
+      </c>
+      <c r="B879" t="s">
+        <v>157</v>
+      </c>
+      <c r="C879" t="s">
+        <v>910</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:E876" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:E878" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15262,19 +15290,19 @@
   <sheetData>
     <row r="1" ht="27.15" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
     </row>
     <row r="2" ht="40.35" hidden="1" spans="1:5">
@@ -15282,13 +15310,13 @@
         <v>328</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E2" s="2">
         <v>1239900</v>
@@ -15302,10 +15330,10 @@
         <v>364</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E3" s="2">
         <v>1759000</v>
@@ -15319,10 +15347,10 @@
         <v>370</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E4" s="2">
         <v>1655000</v>
@@ -15336,10 +15364,10 @@
         <v>372</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E5" s="2">
         <v>1879000</v>
@@ -15350,13 +15378,13 @@
         <v>328</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E6" s="2">
         <v>1077000</v>
@@ -15370,10 +15398,10 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="E7" s="2">
         <v>1408000</v>
@@ -15384,13 +15412,13 @@
         <v>328</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E8" s="2">
         <v>749900</v>
@@ -15404,10 +15432,10 @@
         <v>330</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E9" s="2">
         <v>1175000</v>
@@ -15421,10 +15449,10 @@
         <v>242</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
       <c r="E10" s="2">
         <v>2149000</v>
@@ -15438,10 +15466,10 @@
         <v>346</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E11" s="2">
         <v>1660000</v>
@@ -15455,10 +15483,10 @@
         <v>347</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E12" s="2">
         <v>2020000</v>
@@ -15472,10 +15500,10 @@
         <v>236</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="E13" s="2">
         <v>1859000</v>
@@ -15489,10 +15517,10 @@
         <v>300</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E14" s="2">
         <v>1334900</v>
@@ -15503,13 +15531,13 @@
         <v>169</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E15" s="2">
         <v>3512990</v>
@@ -15526,7 +15554,7 @@
         <v>402</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E16" s="2">
         <v>2836990</v>
@@ -15543,7 +15571,7 @@
         <v>402</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="E17" s="2">
         <v>1850000</v>
@@ -15557,10 +15585,10 @@
         <v>256</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="E18" s="2">
         <v>2749000</v>
@@ -15574,10 +15602,10 @@
         <v>180</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E19" s="2">
         <v>2179990</v>
@@ -15588,13 +15616,13 @@
         <v>169</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E20" s="2">
         <v>2794990</v>
@@ -15608,10 +15636,10 @@
         <v>190</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E21" s="2">
         <v>3959990</v>
@@ -15619,7 +15647,7 @@
     </row>
     <row r="22" ht="27.15" hidden="1" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="B22" s="2">
         <v>300</v>
@@ -15628,7 +15656,7 @@
         <v>402</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E22" s="2">
         <v>4499000</v>
@@ -15636,7 +15664,7 @@
     </row>
     <row r="23" ht="27.15" hidden="1" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="B23" s="2">
         <v>500</v>
@@ -15645,7 +15673,7 @@
         <v>402</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E23" s="2">
         <v>6799000</v>
@@ -15656,13 +15684,13 @@
         <v>328</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E24" s="2">
         <v>778500</v>
@@ -15673,13 +15701,13 @@
         <v>328</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E25" s="2">
         <v>719300</v>
@@ -15690,13 +15718,13 @@
         <v>328</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E26" s="2">
         <v>950900</v>
@@ -15710,10 +15738,10 @@
         <v>363</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E27" s="2">
         <v>1316900</v>
@@ -15724,13 +15752,13 @@
         <v>234</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="E28" s="2">
         <v>2769000</v>
@@ -15744,10 +15772,10 @@
         <v>290</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E29" s="2">
         <v>2244900</v>
@@ -15761,10 +15789,10 @@
         <v>305</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="E30" s="2">
         <v>1574900</v>
@@ -15778,10 +15806,10 @@
         <v>303</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="E31" s="2">
         <v>1434900</v>
@@ -15792,13 +15820,13 @@
         <v>328</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E32" s="2">
         <v>1059000</v>
@@ -15812,10 +15840,10 @@
         <v>249</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
       <c r="E33" s="2">
         <v>3969000</v>
@@ -15832,7 +15860,7 @@
         <v>402</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="E34" s="2">
         <v>1314000</v>
@@ -15843,13 +15871,13 @@
         <v>208</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E35" s="2">
         <v>2149000</v>
@@ -15863,10 +15891,10 @@
         <v>224</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="E36" s="2">
         <v>2599000</v>
@@ -15877,13 +15905,13 @@
         <v>208</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="E37" s="2">
         <v>2599000</v>
@@ -15900,7 +15928,7 @@
         <v>402</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E38" s="2">
         <v>5269000</v>
@@ -15914,10 +15942,10 @@
         <v>292</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E39" s="2">
         <v>2314900</v>
@@ -15928,13 +15956,13 @@
         <v>328</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E40" s="2">
         <v>918900</v>
@@ -15948,10 +15976,10 @@
         <v>295</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E41" s="2">
         <v>2159900</v>
@@ -15968,7 +15996,7 @@
         <v>402</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="E42" s="2">
         <v>1106900</v>
@@ -15985,7 +16013,7 @@
         <v>402</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="E43" s="2">
         <v>1249900</v>
@@ -16002,7 +16030,7 @@
         <v>402</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E44" s="2">
         <v>2900000</v>
@@ -16013,13 +16041,13 @@
         <v>20</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E45" s="2">
         <v>2439900</v>
@@ -16033,10 +16061,10 @@
         <v>298</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="E46" s="2">
         <v>2734900</v>
@@ -16050,10 +16078,10 @@
         <v>317</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="E47" s="2">
         <v>1934900</v>
@@ -16070,7 +16098,7 @@
         <v>402</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="E48" s="2">
         <v>2064900</v>
@@ -16084,10 +16112,10 @@
         <v>318</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E49" s="2">
         <v>2849900</v>
@@ -16095,7 +16123,7 @@
     </row>
     <row r="50" ht="27.15" hidden="1" spans="1:5">
       <c r="A50" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>267</v>
@@ -16104,7 +16132,7 @@
         <v>402</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E50" s="2">
         <v>1779000</v>
@@ -16112,7 +16140,7 @@
     </row>
     <row r="51" ht="27.15" hidden="1" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>261</v>
@@ -16121,7 +16149,7 @@
         <v>402</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E51" s="2">
         <v>2150000</v>
@@ -16129,7 +16157,7 @@
     </row>
     <row r="52" ht="27.15" hidden="1" spans="1:5">
       <c r="A52" s="1" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>266</v>
@@ -16138,7 +16166,7 @@
         <v>402</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E52" s="2">
         <v>2129900</v>
@@ -16146,7 +16174,7 @@
     </row>
     <row r="53" ht="27.15" hidden="1" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>456</v>
@@ -16155,7 +16183,7 @@
         <v>402</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E53" s="2">
         <v>2369900</v>
@@ -16172,7 +16200,7 @@
         <v>402</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="E54" s="2">
         <v>1690000</v>
@@ -16189,7 +16217,7 @@
         <v>402</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E55" s="2">
         <v>2869900</v>
@@ -16200,13 +16228,13 @@
         <v>20</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E56" s="2">
         <v>2569900</v>
@@ -16217,13 +16245,13 @@
         <v>20</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E57" s="2">
         <v>2839900</v>
@@ -16237,10 +16265,10 @@
         <v>27</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E58" s="2">
         <v>3969900</v>
@@ -16254,10 +16282,10 @@
         <v>30</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E59" s="2">
         <v>3069900</v>
@@ -16271,10 +16299,10 @@
         <v>33</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E60" s="2">
         <v>3069900</v>
@@ -16285,13 +16313,13 @@
         <v>20</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="E61" s="2">
         <v>2899900</v>
@@ -16299,16 +16327,16 @@
     </row>
     <row r="62" ht="40.35" hidden="1" spans="1:5">
       <c r="A62" s="1" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>128</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E62" s="2">
         <v>2374000</v>
@@ -16316,16 +16344,16 @@
     </row>
     <row r="63" ht="40.35" hidden="1" spans="1:5">
       <c r="A63" s="1" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>129</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E63" s="2">
         <v>2411000</v>
@@ -16333,16 +16361,16 @@
     </row>
     <row r="64" ht="40.35" hidden="1" spans="1:5">
       <c r="A64" s="1" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E64" s="2">
         <v>2024000</v>
@@ -16356,10 +16384,10 @@
         <v>494</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E65" s="2">
         <v>1124000</v>
@@ -16373,10 +16401,10 @@
         <v>519</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E66" s="2">
         <v>1051000</v>
@@ -16390,10 +16418,10 @@
         <v>516</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="E67" s="2">
         <v>1657000</v>
@@ -16407,10 +16435,10 @@
         <v>509</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E68" s="2">
         <v>1705000</v>
@@ -16424,10 +16452,10 @@
         <v>57</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="E69" s="2">
         <v>1699900</v>
@@ -16441,10 +16469,10 @@
         <v>274</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E70" s="2">
         <v>2489900</v>
@@ -16452,16 +16480,16 @@
     </row>
     <row r="71" ht="40.35" hidden="1" spans="1:5">
       <c r="A71" s="1" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>261</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E71" s="2">
         <v>2959900</v>
@@ -16469,16 +16497,16 @@
     </row>
     <row r="72" ht="40.35" hidden="1" spans="1:5">
       <c r="A72" s="1" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="B72" s="2">
         <v>3</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E72" s="2">
         <v>1765000</v>
@@ -16492,10 +16520,10 @@
         <v>447</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="E73" s="2">
         <v>4409000</v>
@@ -16509,10 +16537,10 @@
         <v>452</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="E74" s="2">
         <v>1690000</v>
@@ -16526,10 +16554,10 @@
         <v>79</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E75" s="2">
         <v>950900</v>
@@ -16546,7 +16574,7 @@
         <v>402</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="E76" s="2">
         <v>880900</v>
@@ -16560,10 +16588,10 @@
         <v>77</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E77" s="2">
         <v>953900</v>
@@ -16577,10 +16605,10 @@
         <v>227</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E78" s="2">
         <v>2179000</v>
@@ -16597,7 +16625,7 @@
         <v>402</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="E79" s="2">
         <v>1579000</v>
@@ -16611,10 +16639,10 @@
         <v>220</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="E80" s="2">
         <v>4299000</v>
@@ -16631,7 +16659,7 @@
         <v>402</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="E81" s="2">
         <v>2049000</v>
@@ -16648,7 +16676,7 @@
         <v>402</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E82" s="2">
         <v>3149000</v>
@@ -16662,10 +16690,10 @@
         <v>450</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E83" s="2">
         <v>2337000</v>
@@ -16676,13 +16704,13 @@
         <v>441</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E84" s="2">
         <v>2762000</v>
@@ -16696,10 +16724,10 @@
         <v>489</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E85" s="2">
         <v>1618000</v>
@@ -16713,10 +16741,10 @@
         <v>495</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E86" s="2">
         <v>1301000</v>
@@ -16730,10 +16758,10 @@
         <v>501</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E87" s="2">
         <v>1258000</v>
@@ -16747,10 +16775,10 @@
         <v>502</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E88" s="2">
         <v>1373000</v>
@@ -16764,10 +16792,10 @@
         <v>492</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="E89" s="2">
         <v>1724000</v>
@@ -16784,7 +16812,7 @@
         <v>402</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="E90" s="2">
         <v>1874000</v>
@@ -16798,10 +16826,10 @@
         <v>512</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E91" s="2">
         <v>2057000</v>
@@ -16815,10 +16843,10 @@
         <v>528</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E92" s="2">
         <v>2118900</v>
@@ -16832,10 +16860,10 @@
         <v>529</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E93" s="2">
         <v>3248000</v>
@@ -16849,10 +16877,10 @@
         <v>530</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E94" s="2">
         <v>5378000</v>
@@ -16866,10 +16894,10 @@
         <v>531</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E95" s="2">
         <v>5806000</v>
@@ -16883,10 +16911,10 @@
         <v>523</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="E96" s="2">
         <v>2388000</v>
@@ -16900,10 +16928,10 @@
         <v>524</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="E97" s="2">
         <v>2681000</v>
@@ -16917,10 +16945,10 @@
         <v>595</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="E98" s="2">
         <v>1385900</v>
@@ -16934,10 +16962,10 @@
         <v>279</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E99" s="2">
         <v>1518000</v>
@@ -16951,10 +16979,10 @@
         <v>600</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E100" s="2">
         <v>3375900</v>
@@ -16971,7 +16999,7 @@
         <v>402</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E101" s="2">
         <v>2828900</v>
@@ -16985,10 +17013,10 @@
         <v>32</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="E102" s="2">
         <v>4449900</v>
@@ -17005,7 +17033,7 @@
         <v>402</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="E103" s="2">
         <v>1229000</v>
@@ -17019,10 +17047,10 @@
         <v>580</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E104" s="2">
         <v>2499000</v>
@@ -17030,16 +17058,16 @@
     </row>
     <row r="105" ht="40.35" hidden="1" spans="1:5">
       <c r="A105" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>577</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="E105" s="2">
         <v>1680000</v>
@@ -17047,16 +17075,16 @@
     </row>
     <row r="106" ht="40.35" hidden="1" spans="1:5">
       <c r="A106" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="B106" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>983</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>981</v>
-      </c>
       <c r="D106" s="1" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="E106" s="2">
         <v>1705000</v>
@@ -17064,7 +17092,7 @@
     </row>
     <row r="107" ht="27.15" hidden="1" spans="1:5">
       <c r="A107" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>36</v>
@@ -17073,7 +17101,7 @@
         <v>402</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E107" s="2">
         <v>1510000</v>
@@ -17090,7 +17118,7 @@
         <v>402</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E108" s="2">
         <v>2570000</v>
@@ -17107,7 +17135,7 @@
         <v>402</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E109" s="2">
         <v>3430000</v>
@@ -17118,13 +17146,13 @@
         <v>50</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E110" s="2">
         <v>2770000</v>
@@ -17138,10 +17166,10 @@
         <v>906</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E111" s="2">
         <v>1970000</v>
@@ -17152,13 +17180,13 @@
         <v>50</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E112" s="2">
         <v>3250000</v>
@@ -17169,13 +17197,13 @@
         <v>50</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E113" s="2">
         <v>3370000</v>
@@ -17192,7 +17220,7 @@
         <v>402</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="E114" s="2">
         <v>3759900</v>
@@ -17206,10 +17234,10 @@
         <v>117</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E115" s="2">
         <v>3380000</v>
@@ -17223,10 +17251,10 @@
         <v>115</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E116" s="2">
         <v>3810000</v>
@@ -17243,7 +17271,7 @@
         <v>402</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E117" s="2">
         <v>4910000</v>
@@ -17260,7 +17288,7 @@
         <v>402</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E118" s="2">
         <v>4550000</v>
@@ -17277,7 +17305,7 @@
         <v>402</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E119" s="2">
         <v>2080000</v>
@@ -17294,7 +17322,7 @@
         <v>402</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="E120" s="2">
         <v>2225000</v>
@@ -17311,7 +17339,7 @@
         <v>402</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E121" s="2">
         <v>2970000</v>
@@ -17325,10 +17353,10 @@
         <v>4</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="E122" s="2">
         <v>4350000</v>
@@ -17342,10 +17370,10 @@
         <v>277</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E123" s="2">
         <v>2999900</v>
@@ -17362,7 +17390,7 @@
         <v>402</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E124" s="2">
         <v>3479900</v>
@@ -17376,10 +17404,10 @@
         <v>281</v>
       </c>
       <c r="C125" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="D125" s="1" t="s">
         <v>918</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>916</v>
       </c>
       <c r="E125" s="2">
         <v>1990000</v>
@@ -17393,10 +17421,10 @@
         <v>282</v>
       </c>
       <c r="C126" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="D126" s="1" t="s">
         <v>918</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>916</v>
       </c>
       <c r="E126" s="2">
         <v>2149000</v>
@@ -17413,7 +17441,7 @@
         <v>402</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E127" s="2">
         <v>2115000</v>
@@ -17430,7 +17458,7 @@
         <v>402</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E128" s="2">
         <v>2238000</v>
@@ -17447,7 +17475,7 @@
         <v>402</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E129" s="2">
         <v>2514900</v>
@@ -17464,7 +17492,7 @@
         <v>402</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E130" s="2">
         <v>2997900</v>
@@ -17472,16 +17500,16 @@
     </row>
     <row r="131" ht="27.15" hidden="1" spans="1:5">
       <c r="A131" s="1" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E131" s="2">
         <v>2549900</v>
@@ -17489,16 +17517,16 @@
     </row>
     <row r="132" ht="27.15" hidden="1" spans="1:5">
       <c r="A132" s="1" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E132" s="2">
         <v>2629900</v>
@@ -17506,16 +17534,16 @@
     </row>
     <row r="133" ht="27.15" hidden="1" spans="1:5">
       <c r="A133" s="1" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E133" s="2">
         <v>4100000</v>
@@ -17532,7 +17560,7 @@
         <v>402</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E134" s="2">
         <v>2219900</v>
@@ -17543,13 +17571,13 @@
         <v>20</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E135" s="2">
         <v>2499900</v>
@@ -17557,7 +17585,7 @@
     </row>
     <row r="136" ht="27.15" hidden="1" spans="1:5">
       <c r="A136" s="1" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>138</v>
@@ -17566,7 +17594,7 @@
         <v>402</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E136" s="2">
         <v>1602000</v>
@@ -17574,16 +17602,16 @@
     </row>
     <row r="137" ht="40.35" hidden="1" spans="1:5">
       <c r="A137" s="1" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E137" s="2">
         <v>1508000</v>
@@ -17600,7 +17628,7 @@
         <v>402</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E138" s="2">
         <v>4549990</v>
@@ -17617,7 +17645,7 @@
         <v>402</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E139" s="2">
         <v>2479990</v>
@@ -17634,7 +17662,7 @@
         <v>402</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E140" s="2">
         <v>2075990</v>
@@ -17651,7 +17679,7 @@
         <v>402</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="E141" s="2">
         <v>2080990</v>
@@ -17665,10 +17693,10 @@
         <v>369</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E142" s="2">
         <v>2273000</v>
@@ -17682,10 +17710,10 @@
         <v>651</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E143" s="2">
         <v>2443000</v>
@@ -17699,10 +17727,10 @@
         <v>670</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E144" s="2">
         <v>1341000</v>
@@ -17713,13 +17741,13 @@
         <v>328</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E145" s="2">
         <v>1381000</v>
@@ -17730,13 +17758,13 @@
         <v>328</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E146" s="2">
         <v>1493000</v>
@@ -17747,13 +17775,13 @@
         <v>328</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E147" s="2">
         <v>1533000</v>
@@ -17767,10 +17795,10 @@
         <v>348</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E148" s="2">
         <v>1670000</v>
@@ -17787,7 +17815,7 @@
         <v>402</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E149" s="2">
         <v>1487000</v>
@@ -17798,13 +17826,13 @@
         <v>50</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E150" s="2">
         <v>4850000</v>
@@ -17815,13 +17843,13 @@
         <v>50</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E151" s="2">
         <v>4000000</v>
@@ -17832,13 +17860,13 @@
         <v>50</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E152" s="2">
         <v>4930000</v>
@@ -17852,10 +17880,10 @@
         <v>187</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E153" s="2">
         <v>3692990</v>
@@ -17869,10 +17897,10 @@
         <v>734</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="E154" s="2">
         <v>3979000</v>
@@ -17889,7 +17917,7 @@
         <v>402</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E155" s="2">
         <v>4099000</v>
@@ -17906,7 +17934,7 @@
         <v>402</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E156" s="2">
         <v>3449000</v>
@@ -17923,7 +17951,7 @@
         <v>402</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E157" s="2">
         <v>2799000</v>
@@ -17934,13 +17962,13 @@
         <v>193</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="E158" s="2">
         <v>3549000</v>
@@ -17951,13 +17979,13 @@
         <v>193</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E159" s="2">
         <v>3299000</v>
@@ -17971,10 +17999,10 @@
         <v>315</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E160" s="2">
         <v>7374900</v>
@@ -17988,10 +18016,10 @@
         <v>324</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E161" s="2">
         <v>3789900</v>
@@ -18005,10 +18033,10 @@
         <v>326</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="E162" s="2">
         <v>5829900</v>
@@ -18022,10 +18050,10 @@
         <v>289</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E163" s="2">
         <v>4144900</v>
@@ -18033,16 +18061,16 @@
     </row>
     <row r="164" ht="27.15" hidden="1" spans="1:5">
       <c r="A164" s="1" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E164" s="2">
         <v>1672000</v>
@@ -18059,7 +18087,7 @@
         <v>402</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E165" s="2">
         <v>2040546</v>
@@ -18076,7 +18104,7 @@
         <v>402</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E166" s="2">
         <v>3100000</v>
@@ -18093,7 +18121,7 @@
         <v>402</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E167" s="2">
         <v>2990000</v>
@@ -18107,10 +18135,10 @@
         <v>602</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="E168" s="2">
         <v>8669500</v>
@@ -18124,10 +18152,10 @@
         <v>654</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="E169" s="2">
         <v>4291000</v>
@@ -18141,10 +18169,10 @@
         <v>598</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E170" s="2">
         <v>6146500</v>
@@ -18152,7 +18180,7 @@
     </row>
     <row r="171" ht="27.15" hidden="1" spans="1:5">
       <c r="A171" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>262</v>
@@ -18161,7 +18189,7 @@
         <v>402</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E171" s="2">
         <v>1889000</v>
@@ -18169,7 +18197,7 @@
     </row>
     <row r="172" ht="27.15" hidden="1" spans="1:5">
       <c r="A172" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>264</v>
@@ -18178,7 +18206,7 @@
         <v>402</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E172" s="2">
         <v>2399000</v>
@@ -18186,7 +18214,7 @@
     </row>
     <row r="173" ht="27.15" hidden="1" spans="1:5">
       <c r="A173" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>631</v>
@@ -18195,7 +18223,7 @@
         <v>402</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E173" s="2">
         <v>3059000</v>
@@ -18203,16 +18231,16 @@
     </row>
     <row r="174" ht="27.15" hidden="1" spans="1:5">
       <c r="A174" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E174" s="2">
         <v>3279000</v>
@@ -18220,7 +18248,7 @@
     </row>
     <row r="175" ht="27.15" hidden="1" spans="1:5">
       <c r="A175" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>632</v>
@@ -18229,7 +18257,7 @@
         <v>402</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E175" s="2">
         <v>3599000</v>
@@ -18237,7 +18265,7 @@
     </row>
     <row r="176" ht="27.15" hidden="1" spans="1:5">
       <c r="A176" s="1" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>168</v>
@@ -18246,7 +18274,7 @@
         <v>402</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E176" s="2">
         <v>5499999</v>
@@ -18254,16 +18282,16 @@
     </row>
     <row r="177" ht="27.15" hidden="1" spans="1:5">
       <c r="A177" s="1" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>165</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E177" s="2">
         <v>4099000</v>
@@ -18271,7 +18299,7 @@
     </row>
     <row r="178" ht="27.15" hidden="1" spans="1:5">
       <c r="A178" s="1" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>162</v>
@@ -18280,7 +18308,7 @@
         <v>402</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E178" s="2">
         <v>2449000</v>
@@ -18291,13 +18319,13 @@
         <v>20</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E179" s="2">
         <v>4529900</v>
@@ -18314,7 +18342,7 @@
         <v>402</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E180" s="2">
         <v>3739900</v>
@@ -18325,13 +18353,13 @@
         <v>20</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E181" s="2">
         <v>5219900</v>
@@ -18342,13 +18370,13 @@
         <v>50</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E182" s="2">
         <v>2780000</v>
@@ -18365,7 +18393,7 @@
         <v>402</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E183" s="2">
         <v>2020000</v>
@@ -18382,7 +18410,7 @@
         <v>402</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E184" s="2">
         <v>2650000</v>
@@ -18399,7 +18427,7 @@
         <v>402</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E185" s="2">
         <v>2080000</v>
@@ -18416,7 +18444,7 @@
         <v>402</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E186" s="2">
         <v>2181000</v>
@@ -18430,10 +18458,10 @@
         <v>5</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="E187" s="2">
         <v>2279000</v>
@@ -18447,10 +18475,10 @@
         <v>6</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="E188" s="2">
         <v>2899000</v>
@@ -18464,10 +18492,10 @@
         <v>424</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="E189" s="2">
         <v>2379000</v>
@@ -18475,16 +18503,16 @@
     </row>
     <row r="190" ht="27.15" hidden="1" spans="1:5">
       <c r="A190" s="1" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E190" s="2">
         <v>2499000</v>
@@ -18492,7 +18520,7 @@
     </row>
     <row r="191" ht="27.15" hidden="1" spans="1:5">
       <c r="A191" s="1" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>457</v>
@@ -18501,7 +18529,7 @@
         <v>402</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E191" s="2">
         <v>2479900</v>
@@ -18518,7 +18546,7 @@
         <v>402</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E192" s="2">
         <v>3959000</v>
@@ -18529,13 +18557,13 @@
         <v>114</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E193" s="2">
         <v>2890000</v>
@@ -18546,13 +18574,13 @@
         <v>114</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E194" s="2">
         <v>4080000</v>
@@ -18563,13 +18591,13 @@
         <v>114</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E195" s="2">
         <v>6290000</v>
@@ -18577,7 +18605,7 @@
     </row>
     <row r="196" ht="27.15" hidden="1" spans="1:5">
       <c r="A196" s="1" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="B196" s="2">
         <v>6</v>
@@ -18586,7 +18614,7 @@
         <v>402</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E196" s="2">
         <v>2200000</v>
@@ -18594,7 +18622,7 @@
     </row>
     <row r="197" ht="27.15" hidden="1" spans="1:5">
       <c r="A197" s="1" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>272</v>
@@ -18603,7 +18631,7 @@
         <v>402</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E197" s="2">
         <v>4599000</v>
@@ -18620,7 +18648,7 @@
         <v>402</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E198" s="2">
         <v>2199000</v>
@@ -18631,13 +18659,13 @@
         <v>208</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E199" s="2">
         <v>4599000</v>
@@ -18648,13 +18676,13 @@
         <v>98</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E200" s="2">
         <v>1990000</v>
@@ -18665,13 +18693,13 @@
         <v>98</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E201" s="2">
         <v>3590000</v>
@@ -18688,7 +18716,7 @@
         <v>402</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E202" s="2">
         <v>2650000</v>
@@ -18699,13 +18727,13 @@
         <v>208</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E203" s="2">
         <v>2849000</v>
@@ -18713,7 +18741,7 @@
     </row>
     <row r="204" ht="27.15" hidden="1" spans="1:5">
       <c r="A204" s="1" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>164</v>
@@ -18722,7 +18750,7 @@
         <v>402</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E204" s="2">
         <v>2099000</v>
@@ -18739,7 +18767,7 @@
         <v>402</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="E205" s="2">
         <v>1263000</v>
@@ -18756,7 +18784,7 @@
         <v>402</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E206" s="2">
         <v>1546500</v>
@@ -18773,7 +18801,7 @@
         <v>402</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="E207" s="2">
         <v>883000</v>
@@ -18790,7 +18818,7 @@
         <v>402</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="E208" s="2">
         <v>825000</v>
@@ -18807,7 +18835,7 @@
         <v>402</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="E209" s="2">
         <v>851000</v>
@@ -18818,13 +18846,13 @@
         <v>169</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E210" s="2">
         <v>3357990</v>
@@ -18835,13 +18863,13 @@
         <v>208</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E211" s="2">
         <v>3899000</v>
@@ -18858,7 +18886,7 @@
         <v>402</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E212" s="2">
         <v>1990000</v>
@@ -18875,7 +18903,7 @@
         <v>402</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E213" s="2">
         <v>2199000</v>
@@ -18892,7 +18920,7 @@
         <v>402</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="E214" s="2">
         <v>789900</v>
@@ -18906,10 +18934,10 @@
         <v>388</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="E215" s="2">
         <v>869900</v>
@@ -18926,7 +18954,7 @@
         <v>402</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="E216" s="2">
         <v>1089000</v>
@@ -18943,7 +18971,7 @@
         <v>402</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="E217" s="2">
         <v>999900</v>
@@ -18960,7 +18988,7 @@
         <v>402</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="E218" s="2">
         <v>1455000</v>
@@ -18974,10 +19002,10 @@
         <v>386</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="E219" s="2">
         <v>809900</v>
@@ -18994,7 +19022,7 @@
         <v>402</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="E220" s="2">
         <v>2000000</v>
@@ -19011,7 +19039,7 @@
         <v>402</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="E221" s="2">
         <v>1229900</v>
@@ -19028,7 +19056,7 @@
         <v>402</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E222" s="2">
         <v>2656800</v>
@@ -19039,13 +19067,13 @@
         <v>328</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="E223" s="2">
         <v>824000</v>
@@ -19056,13 +19084,13 @@
         <v>288</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E224" s="2">
         <v>1204900</v>
@@ -19079,7 +19107,7 @@
         <v>402</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="E225" s="2">
         <v>2234900</v>
@@ -19087,16 +19115,16 @@
     </row>
     <row r="226" ht="40.35" hidden="1" spans="1:5">
       <c r="A226" s="1" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="E226" s="2">
         <v>2673000</v>
@@ -19113,7 +19141,7 @@
         <v>402</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>1030</v>
+        <v>1032</v>
       </c>
       <c r="E227" s="2">
         <v>1419990</v>
@@ -19121,7 +19149,7 @@
     </row>
     <row r="228" ht="27.15" hidden="1" spans="1:5">
       <c r="A228" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>265</v>
@@ -19130,7 +19158,7 @@
         <v>402</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="E228" s="2">
         <v>1494000</v>
@@ -19147,7 +19175,7 @@
         <v>402</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E229" s="2">
         <v>2849990</v>
@@ -19161,10 +19189,10 @@
         <v>573</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E230" s="2">
         <v>3173000</v>
@@ -19175,13 +19203,13 @@
         <v>50</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E231" s="2">
         <v>2380000</v>
@@ -19198,7 +19226,7 @@
         <v>402</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E232" s="2">
         <v>2599000</v>
@@ -19206,16 +19234,16 @@
     </row>
     <row r="233" ht="27.15" hidden="1" spans="1:5">
       <c r="A233" s="1" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E233" s="2">
         <v>2999000</v>
@@ -19226,13 +19254,13 @@
         <v>20</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E234" s="2">
         <v>3590000</v>
@@ -19240,16 +19268,16 @@
     </row>
     <row r="235" ht="40.35" hidden="1" spans="1:5">
       <c r="A235" s="1" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E235" s="2">
         <v>2569900</v>
@@ -19266,7 +19294,7 @@
         <v>402</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E236" s="2">
         <v>4750000</v>
@@ -19274,16 +19302,16 @@
     </row>
     <row r="237" ht="40.35" hidden="1" spans="1:5">
       <c r="A237" s="1" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>1037</v>
+        <v>1039</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E237" s="2">
         <v>2499990</v>
@@ -19291,7 +19319,7 @@
     </row>
     <row r="238" ht="27.15" hidden="1" spans="1:5">
       <c r="A238" s="1" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>770</v>
@@ -19300,7 +19328,7 @@
         <v>402</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E238" s="2">
         <v>2779990</v>
@@ -19314,10 +19342,10 @@
         <v>13</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E239" s="2">
         <v>2649000</v>
@@ -19331,10 +19359,10 @@
         <v>580</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E240" s="2">
         <v>1899000</v>
@@ -19351,7 +19379,7 @@
         <v>402</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E241" s="2">
         <v>2825990</v>
@@ -19359,7 +19387,7 @@
     </row>
     <row r="242" ht="27.15" hidden="1" spans="1:5">
       <c r="A242" s="1" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="B242" s="2">
         <v>400</v>
@@ -19368,7 +19396,7 @@
         <v>402</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="E242" s="2">
         <v>5799000</v>
@@ -19376,7 +19404,7 @@
     </row>
     <row r="243" ht="27.15" hidden="1" spans="1:5">
       <c r="A243" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>268</v>
@@ -19385,7 +19413,7 @@
         <v>402</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="E243" s="2">
         <v>2899000</v>
@@ -19402,7 +19430,7 @@
         <v>402</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E244" s="2">
         <v>1887500</v>
@@ -19419,7 +19447,7 @@
         <v>402</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E245" s="2">
         <v>1805000</v>
@@ -19436,7 +19464,7 @@
         <v>402</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E246" s="2">
         <v>1684500</v>
@@ -19444,7 +19472,7 @@
     </row>
     <row r="247" ht="27.15" hidden="1" spans="1:5">
       <c r="A247" s="1" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>762</v>
@@ -19453,7 +19481,7 @@
         <v>402</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E247" s="2">
         <v>3899000</v>
@@ -19461,7 +19489,7 @@
     </row>
     <row r="248" ht="27.15" hidden="1" spans="1:5">
       <c r="A248" s="1" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>761</v>
@@ -19470,7 +19498,7 @@
         <v>402</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E248" s="2">
         <v>3099000</v>
@@ -19478,7 +19506,7 @@
     </row>
     <row r="249" ht="27.15" hidden="1" spans="1:5">
       <c r="A249" s="1" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="B249" s="2">
         <v>1</v>
@@ -19487,7 +19515,7 @@
         <v>402</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E249" s="2">
         <v>4162990</v>

</xml_diff>

<commit_message>
Add dmitrovka, 6 sites
</commit_message>
<xml_diff>
--- a/id.xlsx
+++ b/id.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9060"/>
+    <workbookView windowWidth="22188" windowHeight="8615"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$E$878</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$E$879</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Лист2!$A$1:$E$249</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2761" uniqueCount="1043">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2815" uniqueCount="1072">
   <si>
     <t>Aito</t>
   </si>
@@ -2765,6 +2765,93 @@
   </si>
   <si>
     <t>GS4</t>
+  </si>
+  <si>
+    <t>X-Cross 5</t>
+  </si>
+  <si>
+    <t>Galaxy L7</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>Combo Cargo</t>
+  </si>
+  <si>
+    <t>Vivaro</t>
+  </si>
+  <si>
+    <t>Bestune M9</t>
+  </si>
+  <si>
+    <t>Hunter Экспедиционный</t>
+  </si>
+  <si>
+    <t>3909 Экспедиционный</t>
+  </si>
+  <si>
+    <t>Berlingo</t>
+  </si>
+  <si>
+    <t>Captain-T</t>
+  </si>
+  <si>
+    <t>i-VAN</t>
+  </si>
+  <si>
+    <t>Tunland G7</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>Free Sport Edition</t>
+  </si>
+  <si>
+    <t>FangChengBao Leopard 5</t>
+  </si>
+  <si>
+    <t>Tang</t>
+  </si>
+  <si>
+    <t>Song Pro</t>
+  </si>
+  <si>
+    <t>Yuan Plus</t>
+  </si>
+  <si>
+    <t>Qin Plus</t>
+  </si>
+  <si>
+    <t>EU5</t>
+  </si>
+  <si>
+    <t>T5 HEV</t>
+  </si>
+  <si>
+    <t>HS7</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>M9</t>
+  </si>
+  <si>
+    <t>Avatr</t>
+  </si>
+  <si>
+    <t>JMC</t>
+  </si>
+  <si>
+    <t>Vigus Work</t>
+  </si>
+  <si>
+    <t>Exlantix</t>
+  </si>
+  <si>
+    <t>ET</t>
   </si>
   <si>
     <t>Марка</t>
@@ -4151,10 +4238,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F879"/>
+  <dimension ref="A1:F907"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A860" workbookViewId="0">
-      <selection activeCell="H866" sqref="H866"/>
+    <sheetView tabSelected="1" topLeftCell="A890" workbookViewId="0">
+      <selection activeCell="E901" sqref="E901"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -15268,8 +15355,316 @@
         <v>910</v>
       </c>
     </row>
+    <row r="880" spans="1:3">
+      <c r="A880">
+        <v>979</v>
+      </c>
+      <c r="B880" t="s">
+        <v>328</v>
+      </c>
+      <c r="C880" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="881" spans="1:3">
+      <c r="A881">
+        <v>980</v>
+      </c>
+      <c r="B881" t="s">
+        <v>169</v>
+      </c>
+      <c r="C881" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="882" spans="1:3">
+      <c r="A882">
+        <v>981</v>
+      </c>
+      <c r="B882" t="s">
+        <v>169</v>
+      </c>
+      <c r="C882" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="883" spans="1:3">
+      <c r="A883">
+        <v>982</v>
+      </c>
+      <c r="B883" t="s">
+        <v>458</v>
+      </c>
+      <c r="C883" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="884" spans="1:3">
+      <c r="A884">
+        <v>983</v>
+      </c>
+      <c r="B884" t="s">
+        <v>458</v>
+      </c>
+      <c r="C884" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="885" spans="1:3">
+      <c r="A885">
+        <v>984</v>
+      </c>
+      <c r="B885" t="s">
+        <v>127</v>
+      </c>
+      <c r="C885" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="886" spans="1:3">
+      <c r="A886">
+        <v>985</v>
+      </c>
+      <c r="B886" t="s">
+        <v>576</v>
+      </c>
+      <c r="C886" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="887" spans="1:3">
+      <c r="A887">
+        <v>986</v>
+      </c>
+      <c r="B887" t="s">
+        <v>576</v>
+      </c>
+      <c r="C887" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="888" spans="1:3">
+      <c r="A888">
+        <v>987</v>
+      </c>
+      <c r="B888" t="s">
+        <v>84</v>
+      </c>
+      <c r="C888" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="889" spans="1:3">
+      <c r="A889">
+        <v>988</v>
+      </c>
+      <c r="B889" t="s">
+        <v>98</v>
+      </c>
+      <c r="C889" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="890" spans="1:3">
+      <c r="A890">
+        <v>989</v>
+      </c>
+      <c r="B890" t="s">
+        <v>108</v>
+      </c>
+      <c r="C890" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="891" spans="1:3">
+      <c r="A891">
+        <v>990</v>
+      </c>
+      <c r="B891" t="s">
+        <v>143</v>
+      </c>
+      <c r="C891" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="892" spans="1:3">
+      <c r="A892">
+        <v>991</v>
+      </c>
+      <c r="B892" t="s">
+        <v>616</v>
+      </c>
+      <c r="C892" s="4" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="893" spans="1:3">
+      <c r="A893">
+        <v>992</v>
+      </c>
+      <c r="B893" t="s">
+        <v>610</v>
+      </c>
+      <c r="C893" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="894" spans="1:3">
+      <c r="A894">
+        <v>993</v>
+      </c>
+      <c r="B894" t="s">
+        <v>18</v>
+      </c>
+      <c r="C894" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="895" spans="1:3">
+      <c r="A895">
+        <v>994</v>
+      </c>
+      <c r="B895" t="s">
+        <v>18</v>
+      </c>
+      <c r="C895" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="896" spans="1:3">
+      <c r="A896">
+        <v>995</v>
+      </c>
+      <c r="B896" t="s">
+        <v>18</v>
+      </c>
+      <c r="C896" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="897" spans="1:3">
+      <c r="A897">
+        <v>996</v>
+      </c>
+      <c r="B897" t="s">
+        <v>18</v>
+      </c>
+      <c r="C897" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="898" spans="1:3">
+      <c r="A898">
+        <v>997</v>
+      </c>
+      <c r="B898" t="s">
+        <v>18</v>
+      </c>
+      <c r="C898" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="899" spans="1:3">
+      <c r="A899">
+        <v>998</v>
+      </c>
+      <c r="B899" t="s">
+        <v>3</v>
+      </c>
+      <c r="C899" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="900" spans="1:3">
+      <c r="A900">
+        <v>999</v>
+      </c>
+      <c r="B900" t="s">
+        <v>140</v>
+      </c>
+      <c r="C900" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="901" spans="1:3">
+      <c r="A901">
+        <v>1000</v>
+      </c>
+      <c r="B901" t="s">
+        <v>663</v>
+      </c>
+      <c r="C901" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="902" spans="1:3">
+      <c r="A902">
+        <v>1001</v>
+      </c>
+      <c r="B902" t="s">
+        <v>398</v>
+      </c>
+      <c r="C902" s="4" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="903" spans="1:3">
+      <c r="A903">
+        <v>1002</v>
+      </c>
+      <c r="B903" t="s">
+        <v>0</v>
+      </c>
+      <c r="C903" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="904" spans="1:3">
+      <c r="A904">
+        <v>1003</v>
+      </c>
+      <c r="B904" t="s">
+        <v>935</v>
+      </c>
+      <c r="C904">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="905" spans="1:3">
+      <c r="A905">
+        <v>1004</v>
+      </c>
+      <c r="B905" t="s">
+        <v>935</v>
+      </c>
+      <c r="C905">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="906" spans="1:3">
+      <c r="A906">
+        <v>1005</v>
+      </c>
+      <c r="B906" t="s">
+        <v>936</v>
+      </c>
+      <c r="C906" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="907" spans="1:3">
+      <c r="A907">
+        <v>1006</v>
+      </c>
+      <c r="B907" t="s">
+        <v>938</v>
+      </c>
+      <c r="C907" t="s">
+        <v>939</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:E878" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:E879" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15290,19 +15685,19 @@
   <sheetData>
     <row r="1" ht="27.15" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>911</v>
+        <v>940</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>912</v>
+        <v>941</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>913</v>
+        <v>942</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>914</v>
+        <v>943</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>915</v>
+        <v>944</v>
       </c>
     </row>
     <row r="2" ht="40.35" hidden="1" spans="1:5">
@@ -15310,13 +15705,13 @@
         <v>328</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>916</v>
+        <v>945</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>917</v>
+        <v>946</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E2" s="2">
         <v>1239900</v>
@@ -15330,10 +15725,10 @@
         <v>364</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>917</v>
+        <v>946</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E3" s="2">
         <v>1759000</v>
@@ -15347,10 +15742,10 @@
         <v>370</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>917</v>
+        <v>946</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E4" s="2">
         <v>1655000</v>
@@ -15364,10 +15759,10 @@
         <v>372</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>917</v>
+        <v>946</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E5" s="2">
         <v>1879000</v>
@@ -15378,13 +15773,13 @@
         <v>328</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>919</v>
+        <v>948</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>921</v>
+        <v>950</v>
       </c>
       <c r="E6" s="2">
         <v>1077000</v>
@@ -15398,10 +15793,10 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>922</v>
+        <v>951</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>923</v>
+        <v>952</v>
       </c>
       <c r="E7" s="2">
         <v>1408000</v>
@@ -15412,13 +15807,13 @@
         <v>328</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>924</v>
+        <v>953</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>921</v>
+        <v>950</v>
       </c>
       <c r="E8" s="2">
         <v>749900</v>
@@ -15432,10 +15827,10 @@
         <v>330</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>921</v>
+        <v>950</v>
       </c>
       <c r="E9" s="2">
         <v>1175000</v>
@@ -15449,10 +15844,10 @@
         <v>242</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>925</v>
+        <v>954</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>926</v>
+        <v>955</v>
       </c>
       <c r="E10" s="2">
         <v>2149000</v>
@@ -15466,10 +15861,10 @@
         <v>346</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E11" s="2">
         <v>1660000</v>
@@ -15483,10 +15878,10 @@
         <v>347</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E12" s="2">
         <v>2020000</v>
@@ -15500,10 +15895,10 @@
         <v>236</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>928</v>
+        <v>957</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>929</v>
+        <v>958</v>
       </c>
       <c r="E13" s="2">
         <v>1859000</v>
@@ -15517,10 +15912,10 @@
         <v>300</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>930</v>
+        <v>959</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E14" s="2">
         <v>1334900</v>
@@ -15531,13 +15926,13 @@
         <v>169</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>931</v>
+        <v>960</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>928</v>
+        <v>957</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E15" s="2">
         <v>3512990</v>
@@ -15554,7 +15949,7 @@
         <v>402</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E16" s="2">
         <v>2836990</v>
@@ -15571,7 +15966,7 @@
         <v>402</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>933</v>
+        <v>962</v>
       </c>
       <c r="E17" s="2">
         <v>1850000</v>
@@ -15585,10 +15980,10 @@
         <v>256</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>934</v>
+        <v>963</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>935</v>
+        <v>964</v>
       </c>
       <c r="E18" s="2">
         <v>2749000</v>
@@ -15602,10 +15997,10 @@
         <v>180</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>928</v>
+        <v>957</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E19" s="2">
         <v>2179990</v>
@@ -15616,13 +16011,13 @@
         <v>169</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>936</v>
+        <v>965</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E20" s="2">
         <v>2794990</v>
@@ -15636,10 +16031,10 @@
         <v>190</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E21" s="2">
         <v>3959990</v>
@@ -15647,7 +16042,7 @@
     </row>
     <row r="22" ht="27.15" hidden="1" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>937</v>
+        <v>966</v>
       </c>
       <c r="B22" s="2">
         <v>300</v>
@@ -15656,7 +16051,7 @@
         <v>402</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E22" s="2">
         <v>4499000</v>
@@ -15664,7 +16059,7 @@
     </row>
     <row r="23" ht="27.15" hidden="1" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>937</v>
+        <v>966</v>
       </c>
       <c r="B23" s="2">
         <v>500</v>
@@ -15673,7 +16068,7 @@
         <v>402</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E23" s="2">
         <v>6799000</v>
@@ -15684,13 +16079,13 @@
         <v>328</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>938</v>
+        <v>967</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>921</v>
+        <v>950</v>
       </c>
       <c r="E24" s="2">
         <v>778500</v>
@@ -15701,13 +16096,13 @@
         <v>328</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>939</v>
+        <v>968</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>921</v>
+        <v>950</v>
       </c>
       <c r="E25" s="2">
         <v>719300</v>
@@ -15718,13 +16113,13 @@
         <v>328</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>940</v>
+        <v>969</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>921</v>
+        <v>950</v>
       </c>
       <c r="E26" s="2">
         <v>950900</v>
@@ -15738,10 +16133,10 @@
         <v>363</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>917</v>
+        <v>946</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E27" s="2">
         <v>1316900</v>
@@ -15752,13 +16147,13 @@
         <v>234</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>941</v>
+        <v>970</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>942</v>
+        <v>971</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>943</v>
+        <v>972</v>
       </c>
       <c r="E28" s="2">
         <v>2769000</v>
@@ -15772,10 +16167,10 @@
         <v>290</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>930</v>
+        <v>959</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E29" s="2">
         <v>2244900</v>
@@ -15789,10 +16184,10 @@
         <v>305</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>944</v>
+        <v>973</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>923</v>
+        <v>952</v>
       </c>
       <c r="E30" s="2">
         <v>1574900</v>
@@ -15806,10 +16201,10 @@
         <v>303</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>944</v>
+        <v>973</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>923</v>
+        <v>952</v>
       </c>
       <c r="E31" s="2">
         <v>1434900</v>
@@ -15820,13 +16215,13 @@
         <v>328</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>945</v>
+        <v>974</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E32" s="2">
         <v>1059000</v>
@@ -15840,10 +16235,10 @@
         <v>249</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>944</v>
+        <v>973</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>926</v>
+        <v>955</v>
       </c>
       <c r="E33" s="2">
         <v>3969000</v>
@@ -15860,7 +16255,7 @@
         <v>402</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>947</v>
+        <v>976</v>
       </c>
       <c r="E34" s="2">
         <v>1314000</v>
@@ -15871,13 +16266,13 @@
         <v>208</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>948</v>
+        <v>977</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E35" s="2">
         <v>2149000</v>
@@ -15891,10 +16286,10 @@
         <v>224</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>950</v>
+        <v>979</v>
       </c>
       <c r="E36" s="2">
         <v>2599000</v>
@@ -15905,13 +16300,13 @@
         <v>208</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>951</v>
+        <v>980</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>950</v>
+        <v>979</v>
       </c>
       <c r="E37" s="2">
         <v>2599000</v>
@@ -15928,7 +16323,7 @@
         <v>402</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>952</v>
+        <v>981</v>
       </c>
       <c r="E38" s="2">
         <v>5269000</v>
@@ -15942,10 +16337,10 @@
         <v>292</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>930</v>
+        <v>959</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E39" s="2">
         <v>2314900</v>
@@ -15956,13 +16351,13 @@
         <v>328</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>953</v>
+        <v>982</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E40" s="2">
         <v>918900</v>
@@ -15976,10 +16371,10 @@
         <v>295</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>944</v>
+        <v>973</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E41" s="2">
         <v>2159900</v>
@@ -15996,7 +16391,7 @@
         <v>402</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>954</v>
+        <v>983</v>
       </c>
       <c r="E42" s="2">
         <v>1106900</v>
@@ -16013,7 +16408,7 @@
         <v>402</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>954</v>
+        <v>983</v>
       </c>
       <c r="E43" s="2">
         <v>1249900</v>
@@ -16030,7 +16425,7 @@
         <v>402</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E44" s="2">
         <v>2900000</v>
@@ -16041,13 +16436,13 @@
         <v>20</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>955</v>
+        <v>984</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E45" s="2">
         <v>2439900</v>
@@ -16061,10 +16456,10 @@
         <v>298</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>956</v>
+        <v>985</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>957</v>
+        <v>986</v>
       </c>
       <c r="E46" s="2">
         <v>2734900</v>
@@ -16078,10 +16473,10 @@
         <v>317</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>956</v>
+        <v>985</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>957</v>
+        <v>986</v>
       </c>
       <c r="E47" s="2">
         <v>1934900</v>
@@ -16098,7 +16493,7 @@
         <v>402</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>957</v>
+        <v>986</v>
       </c>
       <c r="E48" s="2">
         <v>2064900</v>
@@ -16112,10 +16507,10 @@
         <v>318</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>958</v>
+        <v>987</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E49" s="2">
         <v>2849900</v>
@@ -16123,7 +16518,7 @@
     </row>
     <row r="50" ht="27.15" hidden="1" spans="1:5">
       <c r="A50" s="1" t="s">
-        <v>959</v>
+        <v>988</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>267</v>
@@ -16132,7 +16527,7 @@
         <v>402</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E50" s="2">
         <v>1779000</v>
@@ -16140,7 +16535,7 @@
     </row>
     <row r="51" ht="27.15" hidden="1" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>959</v>
+        <v>988</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>261</v>
@@ -16149,7 +16544,7 @@
         <v>402</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E51" s="2">
         <v>2150000</v>
@@ -16157,7 +16552,7 @@
     </row>
     <row r="52" ht="27.15" hidden="1" spans="1:5">
       <c r="A52" s="1" t="s">
-        <v>960</v>
+        <v>989</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>266</v>
@@ -16166,7 +16561,7 @@
         <v>402</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E52" s="2">
         <v>2129900</v>
@@ -16174,7 +16569,7 @@
     </row>
     <row r="53" ht="27.15" hidden="1" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>960</v>
+        <v>989</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>456</v>
@@ -16183,7 +16578,7 @@
         <v>402</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E53" s="2">
         <v>2369900</v>
@@ -16200,7 +16595,7 @@
         <v>402</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>957</v>
+        <v>986</v>
       </c>
       <c r="E54" s="2">
         <v>1690000</v>
@@ -16217,7 +16612,7 @@
         <v>402</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E55" s="2">
         <v>2869900</v>
@@ -16228,13 +16623,13 @@
         <v>20</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>961</v>
+        <v>990</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E56" s="2">
         <v>2569900</v>
@@ -16245,13 +16640,13 @@
         <v>20</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>962</v>
+        <v>991</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E57" s="2">
         <v>2839900</v>
@@ -16265,10 +16660,10 @@
         <v>27</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>963</v>
+        <v>992</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E58" s="2">
         <v>3969900</v>
@@ -16282,10 +16677,10 @@
         <v>30</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>963</v>
+        <v>992</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E59" s="2">
         <v>3069900</v>
@@ -16299,10 +16694,10 @@
         <v>33</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>963</v>
+        <v>992</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E60" s="2">
         <v>3069900</v>
@@ -16313,13 +16708,13 @@
         <v>20</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>964</v>
+        <v>993</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>963</v>
+        <v>992</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>965</v>
+        <v>994</v>
       </c>
       <c r="E61" s="2">
         <v>2899900</v>
@@ -16327,16 +16722,16 @@
     </row>
     <row r="62" ht="40.35" hidden="1" spans="1:5">
       <c r="A62" s="1" t="s">
-        <v>966</v>
+        <v>995</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>128</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>963</v>
+        <v>992</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E62" s="2">
         <v>2374000</v>
@@ -16344,16 +16739,16 @@
     </row>
     <row r="63" ht="40.35" hidden="1" spans="1:5">
       <c r="A63" s="1" t="s">
-        <v>966</v>
+        <v>995</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>129</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>963</v>
+        <v>992</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E63" s="2">
         <v>2411000</v>
@@ -16361,16 +16756,16 @@
     </row>
     <row r="64" ht="40.35" hidden="1" spans="1:5">
       <c r="A64" s="1" t="s">
-        <v>966</v>
+        <v>995</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>963</v>
+        <v>992</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>921</v>
+        <v>950</v>
       </c>
       <c r="E64" s="2">
         <v>2024000</v>
@@ -16384,10 +16779,10 @@
         <v>494</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>922</v>
+        <v>951</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>952</v>
+        <v>981</v>
       </c>
       <c r="E65" s="2">
         <v>1124000</v>
@@ -16401,10 +16796,10 @@
         <v>519</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>928</v>
+        <v>957</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E66" s="2">
         <v>1051000</v>
@@ -16418,10 +16813,10 @@
         <v>516</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>967</v>
+        <v>996</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>957</v>
+        <v>986</v>
       </c>
       <c r="E67" s="2">
         <v>1657000</v>
@@ -16435,10 +16830,10 @@
         <v>509</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E68" s="2">
         <v>1705000</v>
@@ -16452,10 +16847,10 @@
         <v>57</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>968</v>
+        <v>997</v>
       </c>
       <c r="E69" s="2">
         <v>1699900</v>
@@ -16469,10 +16864,10 @@
         <v>274</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>963</v>
+        <v>992</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E70" s="2">
         <v>2489900</v>
@@ -16480,16 +16875,16 @@
     </row>
     <row r="71" ht="40.35" hidden="1" spans="1:5">
       <c r="A71" s="1" t="s">
-        <v>969</v>
+        <v>998</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>261</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>963</v>
+        <v>992</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E71" s="2">
         <v>2959900</v>
@@ -16497,16 +16892,16 @@
     </row>
     <row r="72" ht="40.35" hidden="1" spans="1:5">
       <c r="A72" s="1" t="s">
-        <v>970</v>
+        <v>999</v>
       </c>
       <c r="B72" s="2">
         <v>3</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>963</v>
+        <v>992</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E72" s="2">
         <v>1765000</v>
@@ -16520,10 +16915,10 @@
         <v>447</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>971</v>
+        <v>1000</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>972</v>
+        <v>1001</v>
       </c>
       <c r="E73" s="2">
         <v>4409000</v>
@@ -16537,10 +16932,10 @@
         <v>452</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>971</v>
+        <v>1000</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>972</v>
+        <v>1001</v>
       </c>
       <c r="E74" s="2">
         <v>1690000</v>
@@ -16554,10 +16949,10 @@
         <v>79</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>973</v>
+        <v>1002</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E75" s="2">
         <v>950900</v>
@@ -16574,7 +16969,7 @@
         <v>402</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>947</v>
+        <v>976</v>
       </c>
       <c r="E76" s="2">
         <v>880900</v>
@@ -16588,10 +16983,10 @@
         <v>77</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>922</v>
+        <v>951</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E77" s="2">
         <v>953900</v>
@@ -16605,10 +17000,10 @@
         <v>227</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>928</v>
+        <v>957</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E78" s="2">
         <v>2179000</v>
@@ -16625,7 +17020,7 @@
         <v>402</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>974</v>
+        <v>1003</v>
       </c>
       <c r="E79" s="2">
         <v>1579000</v>
@@ -16639,10 +17034,10 @@
         <v>220</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>947</v>
+        <v>976</v>
       </c>
       <c r="E80" s="2">
         <v>4299000</v>
@@ -16659,7 +17054,7 @@
         <v>402</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>975</v>
+        <v>1004</v>
       </c>
       <c r="E81" s="2">
         <v>2049000</v>
@@ -16676,7 +17071,7 @@
         <v>402</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E82" s="2">
         <v>3149000</v>
@@ -16690,10 +17085,10 @@
         <v>450</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>922</v>
+        <v>951</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>976</v>
+        <v>1005</v>
       </c>
       <c r="E83" s="2">
         <v>2337000</v>
@@ -16704,13 +17099,13 @@
         <v>441</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>977</v>
+        <v>1006</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>930</v>
+        <v>959</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>976</v>
+        <v>1005</v>
       </c>
       <c r="E84" s="2">
         <v>2762000</v>
@@ -16724,10 +17119,10 @@
         <v>489</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>928</v>
+        <v>957</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E85" s="2">
         <v>1618000</v>
@@ -16741,10 +17136,10 @@
         <v>495</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>922</v>
+        <v>951</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>952</v>
+        <v>981</v>
       </c>
       <c r="E86" s="2">
         <v>1301000</v>
@@ -16758,10 +17153,10 @@
         <v>501</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>922</v>
+        <v>951</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>952</v>
+        <v>981</v>
       </c>
       <c r="E87" s="2">
         <v>1258000</v>
@@ -16775,10 +17170,10 @@
         <v>502</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>922</v>
+        <v>951</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>952</v>
+        <v>981</v>
       </c>
       <c r="E88" s="2">
         <v>1373000</v>
@@ -16792,10 +17187,10 @@
         <v>492</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>923</v>
+        <v>952</v>
       </c>
       <c r="E89" s="2">
         <v>1724000</v>
@@ -16812,7 +17207,7 @@
         <v>402</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>957</v>
+        <v>986</v>
       </c>
       <c r="E90" s="2">
         <v>1874000</v>
@@ -16826,10 +17221,10 @@
         <v>512</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E91" s="2">
         <v>2057000</v>
@@ -16843,10 +17238,10 @@
         <v>528</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E92" s="2">
         <v>2118900</v>
@@ -16860,10 +17255,10 @@
         <v>529</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E93" s="2">
         <v>3248000</v>
@@ -16877,10 +17272,10 @@
         <v>530</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E94" s="2">
         <v>5378000</v>
@@ -16894,10 +17289,10 @@
         <v>531</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E95" s="2">
         <v>5806000</v>
@@ -16911,10 +17306,10 @@
         <v>523</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>930</v>
+        <v>959</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>957</v>
+        <v>986</v>
       </c>
       <c r="E96" s="2">
         <v>2388000</v>
@@ -16928,10 +17323,10 @@
         <v>524</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>930</v>
+        <v>959</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>957</v>
+        <v>986</v>
       </c>
       <c r="E97" s="2">
         <v>2681000</v>
@@ -16945,10 +17340,10 @@
         <v>595</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>978</v>
+        <v>1007</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>923</v>
+        <v>952</v>
       </c>
       <c r="E98" s="2">
         <v>1385900</v>
@@ -16962,10 +17357,10 @@
         <v>279</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>979</v>
+        <v>1008</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>980</v>
+        <v>1009</v>
       </c>
       <c r="E99" s="2">
         <v>1518000</v>
@@ -16979,10 +17374,10 @@
         <v>600</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>922</v>
+        <v>951</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E100" s="2">
         <v>3375900</v>
@@ -16999,7 +17394,7 @@
         <v>402</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E101" s="2">
         <v>2828900</v>
@@ -17013,10 +17408,10 @@
         <v>32</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>957</v>
+        <v>986</v>
       </c>
       <c r="E102" s="2">
         <v>4449900</v>
@@ -17033,7 +17428,7 @@
         <v>402</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>981</v>
+        <v>1010</v>
       </c>
       <c r="E103" s="2">
         <v>1229000</v>
@@ -17047,10 +17442,10 @@
         <v>580</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>928</v>
+        <v>957</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E104" s="2">
         <v>2499000</v>
@@ -17058,16 +17453,16 @@
     </row>
     <row r="105" ht="40.35" hidden="1" spans="1:5">
       <c r="A105" s="1" t="s">
-        <v>982</v>
+        <v>1011</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>577</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>983</v>
+        <v>1012</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>984</v>
+        <v>1013</v>
       </c>
       <c r="E105" s="2">
         <v>1680000</v>
@@ -17075,16 +17470,16 @@
     </row>
     <row r="106" ht="40.35" hidden="1" spans="1:5">
       <c r="A106" s="1" t="s">
-        <v>982</v>
+        <v>1011</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>985</v>
+        <v>1014</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>983</v>
+        <v>1012</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>984</v>
+        <v>1013</v>
       </c>
       <c r="E106" s="2">
         <v>1705000</v>
@@ -17092,7 +17487,7 @@
     </row>
     <row r="107" ht="27.15" hidden="1" spans="1:5">
       <c r="A107" s="1" t="s">
-        <v>982</v>
+        <v>1011</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>36</v>
@@ -17101,7 +17496,7 @@
         <v>402</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>986</v>
+        <v>1015</v>
       </c>
       <c r="E107" s="2">
         <v>1510000</v>
@@ -17118,7 +17513,7 @@
         <v>402</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E108" s="2">
         <v>2570000</v>
@@ -17135,7 +17530,7 @@
         <v>402</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E109" s="2">
         <v>3430000</v>
@@ -17146,13 +17541,13 @@
         <v>50</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>987</v>
+        <v>1016</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E110" s="2">
         <v>2770000</v>
@@ -17166,10 +17561,10 @@
         <v>906</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E111" s="2">
         <v>1970000</v>
@@ -17180,13 +17575,13 @@
         <v>50</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>988</v>
+        <v>1017</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E112" s="2">
         <v>3250000</v>
@@ -17197,13 +17592,13 @@
         <v>50</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>989</v>
+        <v>1018</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E113" s="2">
         <v>3370000</v>
@@ -17220,7 +17615,7 @@
         <v>402</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>957</v>
+        <v>986</v>
       </c>
       <c r="E114" s="2">
         <v>3759900</v>
@@ -17234,10 +17629,10 @@
         <v>117</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E115" s="2">
         <v>3380000</v>
@@ -17251,10 +17646,10 @@
         <v>115</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E116" s="2">
         <v>3810000</v>
@@ -17271,7 +17666,7 @@
         <v>402</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E117" s="2">
         <v>4910000</v>
@@ -17288,7 +17683,7 @@
         <v>402</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E118" s="2">
         <v>4550000</v>
@@ -17305,7 +17700,7 @@
         <v>402</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E119" s="2">
         <v>2080000</v>
@@ -17322,7 +17717,7 @@
         <v>402</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>957</v>
+        <v>986</v>
       </c>
       <c r="E120" s="2">
         <v>2225000</v>
@@ -17339,7 +17734,7 @@
         <v>402</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E121" s="2">
         <v>2970000</v>
@@ -17353,10 +17748,10 @@
         <v>4</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>957</v>
+        <v>986</v>
       </c>
       <c r="E122" s="2">
         <v>4350000</v>
@@ -17370,10 +17765,10 @@
         <v>277</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E123" s="2">
         <v>2999900</v>
@@ -17390,7 +17785,7 @@
         <v>402</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E124" s="2">
         <v>3479900</v>
@@ -17404,10 +17799,10 @@
         <v>281</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E125" s="2">
         <v>1990000</v>
@@ -17421,10 +17816,10 @@
         <v>282</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E126" s="2">
         <v>2149000</v>
@@ -17441,7 +17836,7 @@
         <v>402</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E127" s="2">
         <v>2115000</v>
@@ -17458,7 +17853,7 @@
         <v>402</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E128" s="2">
         <v>2238000</v>
@@ -17475,7 +17870,7 @@
         <v>402</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E129" s="2">
         <v>2514900</v>
@@ -17492,7 +17887,7 @@
         <v>402</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E130" s="2">
         <v>2997900</v>
@@ -17500,16 +17895,16 @@
     </row>
     <row r="131" ht="27.15" hidden="1" spans="1:5">
       <c r="A131" s="1" t="s">
-        <v>990</v>
+        <v>1019</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>991</v>
+        <v>1020</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E131" s="2">
         <v>2549900</v>
@@ -17517,16 +17912,16 @@
     </row>
     <row r="132" ht="27.15" hidden="1" spans="1:5">
       <c r="A132" s="1" t="s">
-        <v>990</v>
+        <v>1019</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>992</v>
+        <v>1021</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E132" s="2">
         <v>2629900</v>
@@ -17534,16 +17929,16 @@
     </row>
     <row r="133" ht="27.15" hidden="1" spans="1:5">
       <c r="A133" s="1" t="s">
-        <v>970</v>
+        <v>999</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>993</v>
+        <v>1022</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E133" s="2">
         <v>4100000</v>
@@ -17560,7 +17955,7 @@
         <v>402</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>976</v>
+        <v>1005</v>
       </c>
       <c r="E134" s="2">
         <v>2219900</v>
@@ -17571,13 +17966,13 @@
         <v>20</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>994</v>
+        <v>1023</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>921</v>
+        <v>950</v>
       </c>
       <c r="E135" s="2">
         <v>2499900</v>
@@ -17585,7 +17980,7 @@
     </row>
     <row r="136" ht="27.15" hidden="1" spans="1:5">
       <c r="A136" s="1" t="s">
-        <v>966</v>
+        <v>995</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>138</v>
@@ -17594,7 +17989,7 @@
         <v>402</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>995</v>
+        <v>1024</v>
       </c>
       <c r="E136" s="2">
         <v>1602000</v>
@@ -17602,16 +17997,16 @@
     </row>
     <row r="137" ht="40.35" hidden="1" spans="1:5">
       <c r="A137" s="1" t="s">
-        <v>966</v>
+        <v>995</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>952</v>
+        <v>981</v>
       </c>
       <c r="E137" s="2">
         <v>1508000</v>
@@ -17628,7 +18023,7 @@
         <v>402</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E138" s="2">
         <v>4549990</v>
@@ -17645,7 +18040,7 @@
         <v>402</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E139" s="2">
         <v>2479990</v>
@@ -17662,7 +18057,7 @@
         <v>402</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>996</v>
+        <v>1025</v>
       </c>
       <c r="E140" s="2">
         <v>2075990</v>
@@ -17679,7 +18074,7 @@
         <v>402</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>957</v>
+        <v>986</v>
       </c>
       <c r="E141" s="2">
         <v>2080990</v>
@@ -17693,10 +18088,10 @@
         <v>369</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>917</v>
+        <v>946</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E142" s="2">
         <v>2273000</v>
@@ -17710,10 +18105,10 @@
         <v>651</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>917</v>
+        <v>946</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E143" s="2">
         <v>2443000</v>
@@ -17727,10 +18122,10 @@
         <v>670</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>921</v>
+        <v>950</v>
       </c>
       <c r="E144" s="2">
         <v>1341000</v>
@@ -17741,13 +18136,13 @@
         <v>328</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>997</v>
+        <v>1026</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>921</v>
+        <v>950</v>
       </c>
       <c r="E145" s="2">
         <v>1381000</v>
@@ -17758,13 +18153,13 @@
         <v>328</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>998</v>
+        <v>1027</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>921</v>
+        <v>950</v>
       </c>
       <c r="E146" s="2">
         <v>1493000</v>
@@ -17775,13 +18170,13 @@
         <v>328</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>999</v>
+        <v>1028</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>921</v>
+        <v>950</v>
       </c>
       <c r="E147" s="2">
         <v>1533000</v>
@@ -17795,10 +18190,10 @@
         <v>348</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E148" s="2">
         <v>1670000</v>
@@ -17815,7 +18210,7 @@
         <v>402</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E149" s="2">
         <v>1487000</v>
@@ -17826,13 +18221,13 @@
         <v>50</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>1000</v>
+        <v>1029</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E150" s="2">
         <v>4850000</v>
@@ -17843,13 +18238,13 @@
         <v>50</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>1001</v>
+        <v>1030</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E151" s="2">
         <v>4000000</v>
@@ -17860,13 +18255,13 @@
         <v>50</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>1002</v>
+        <v>1031</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E152" s="2">
         <v>4930000</v>
@@ -17880,10 +18275,10 @@
         <v>187</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E153" s="2">
         <v>3692990</v>
@@ -17897,10 +18292,10 @@
         <v>734</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>934</v>
+        <v>963</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>935</v>
+        <v>964</v>
       </c>
       <c r="E154" s="2">
         <v>3979000</v>
@@ -17917,7 +18312,7 @@
         <v>402</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E155" s="2">
         <v>4099000</v>
@@ -17934,7 +18329,7 @@
         <v>402</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E156" s="2">
         <v>3449000</v>
@@ -17951,7 +18346,7 @@
         <v>402</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E157" s="2">
         <v>2799000</v>
@@ -17962,13 +18357,13 @@
         <v>193</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>1003</v>
+        <v>1032</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>957</v>
+        <v>986</v>
       </c>
       <c r="E158" s="2">
         <v>3549000</v>
@@ -17979,13 +18374,13 @@
         <v>193</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>1004</v>
+        <v>1033</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E159" s="2">
         <v>3299000</v>
@@ -17999,10 +18394,10 @@
         <v>315</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>1005</v>
+        <v>1034</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E160" s="2">
         <v>7374900</v>
@@ -18016,10 +18411,10 @@
         <v>324</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>934</v>
+        <v>963</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E161" s="2">
         <v>3789900</v>
@@ -18033,10 +18428,10 @@
         <v>326</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>1006</v>
+        <v>1035</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>957</v>
+        <v>986</v>
       </c>
       <c r="E162" s="2">
         <v>5829900</v>
@@ -18050,10 +18445,10 @@
         <v>289</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>934</v>
+        <v>963</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E163" s="2">
         <v>4144900</v>
@@ -18061,16 +18456,16 @@
     </row>
     <row r="164" ht="27.15" hidden="1" spans="1:5">
       <c r="A164" s="1" t="s">
-        <v>990</v>
+        <v>1019</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>1007</v>
+        <v>1036</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E164" s="2">
         <v>1672000</v>
@@ -18087,7 +18482,7 @@
         <v>402</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E165" s="2">
         <v>2040546</v>
@@ -18104,7 +18499,7 @@
         <v>402</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E166" s="2">
         <v>3100000</v>
@@ -18121,7 +18516,7 @@
         <v>402</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E167" s="2">
         <v>2990000</v>
@@ -18135,10 +18530,10 @@
         <v>602</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>956</v>
+        <v>985</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>968</v>
+        <v>997</v>
       </c>
       <c r="E168" s="2">
         <v>8669500</v>
@@ -18152,10 +18547,10 @@
         <v>654</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>1008</v>
+        <v>1037</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>957</v>
+        <v>986</v>
       </c>
       <c r="E169" s="2">
         <v>4291000</v>
@@ -18169,10 +18564,10 @@
         <v>598</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E170" s="2">
         <v>6146500</v>
@@ -18180,7 +18575,7 @@
     </row>
     <row r="171" ht="27.15" hidden="1" spans="1:5">
       <c r="A171" s="1" t="s">
-        <v>959</v>
+        <v>988</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>262</v>
@@ -18189,7 +18584,7 @@
         <v>402</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E171" s="2">
         <v>1889000</v>
@@ -18197,7 +18592,7 @@
     </row>
     <row r="172" ht="27.15" hidden="1" spans="1:5">
       <c r="A172" s="1" t="s">
-        <v>959</v>
+        <v>988</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>264</v>
@@ -18206,7 +18601,7 @@
         <v>402</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E172" s="2">
         <v>2399000</v>
@@ -18214,7 +18609,7 @@
     </row>
     <row r="173" ht="27.15" hidden="1" spans="1:5">
       <c r="A173" s="1" t="s">
-        <v>959</v>
+        <v>988</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>631</v>
@@ -18223,7 +18618,7 @@
         <v>402</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E173" s="2">
         <v>3059000</v>
@@ -18231,16 +18626,16 @@
     </row>
     <row r="174" ht="27.15" hidden="1" spans="1:5">
       <c r="A174" s="1" t="s">
-        <v>959</v>
+        <v>988</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>1009</v>
+        <v>1038</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E174" s="2">
         <v>3279000</v>
@@ -18248,7 +18643,7 @@
     </row>
     <row r="175" ht="27.15" hidden="1" spans="1:5">
       <c r="A175" s="1" t="s">
-        <v>959</v>
+        <v>988</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>632</v>
@@ -18257,7 +18652,7 @@
         <v>402</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E175" s="2">
         <v>3599000</v>
@@ -18265,7 +18660,7 @@
     </row>
     <row r="176" ht="27.15" hidden="1" spans="1:5">
       <c r="A176" s="1" t="s">
-        <v>1010</v>
+        <v>1039</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>168</v>
@@ -18274,7 +18669,7 @@
         <v>402</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E176" s="2">
         <v>5499999</v>
@@ -18282,16 +18677,16 @@
     </row>
     <row r="177" ht="27.15" hidden="1" spans="1:5">
       <c r="A177" s="1" t="s">
-        <v>1010</v>
+        <v>1039</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>165</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>928</v>
+        <v>957</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E177" s="2">
         <v>4099000</v>
@@ -18299,7 +18694,7 @@
     </row>
     <row r="178" ht="27.15" hidden="1" spans="1:5">
       <c r="A178" s="1" t="s">
-        <v>1010</v>
+        <v>1039</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>162</v>
@@ -18308,7 +18703,7 @@
         <v>402</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E178" s="2">
         <v>2449000</v>
@@ -18319,13 +18714,13 @@
         <v>20</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>1011</v>
+        <v>1040</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>1006</v>
+        <v>1035</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E179" s="2">
         <v>4529900</v>
@@ -18342,7 +18737,7 @@
         <v>402</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E180" s="2">
         <v>3739900</v>
@@ -18353,13 +18748,13 @@
         <v>20</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>1012</v>
+        <v>1041</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>963</v>
+        <v>992</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E181" s="2">
         <v>5219900</v>
@@ -18370,13 +18765,13 @@
         <v>50</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>1013</v>
+        <v>1042</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E182" s="2">
         <v>2780000</v>
@@ -18393,7 +18788,7 @@
         <v>402</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E183" s="2">
         <v>2020000</v>
@@ -18410,7 +18805,7 @@
         <v>402</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E184" s="2">
         <v>2650000</v>
@@ -18427,7 +18822,7 @@
         <v>402</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E185" s="2">
         <v>2080000</v>
@@ -18444,7 +18839,7 @@
         <v>402</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E186" s="2">
         <v>2181000</v>
@@ -18458,10 +18853,10 @@
         <v>5</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>947</v>
+        <v>976</v>
       </c>
       <c r="E187" s="2">
         <v>2279000</v>
@@ -18475,10 +18870,10 @@
         <v>6</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>928</v>
+        <v>957</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>947</v>
+        <v>976</v>
       </c>
       <c r="E188" s="2">
         <v>2899000</v>
@@ -18492,10 +18887,10 @@
         <v>424</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>922</v>
+        <v>951</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>957</v>
+        <v>986</v>
       </c>
       <c r="E189" s="2">
         <v>2379000</v>
@@ -18503,16 +18898,16 @@
     </row>
     <row r="190" ht="27.15" hidden="1" spans="1:5">
       <c r="A190" s="1" t="s">
-        <v>1014</v>
+        <v>1043</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>1015</v>
+        <v>1044</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E190" s="2">
         <v>2499000</v>
@@ -18520,7 +18915,7 @@
     </row>
     <row r="191" ht="27.15" hidden="1" spans="1:5">
       <c r="A191" s="1" t="s">
-        <v>960</v>
+        <v>989</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>457</v>
@@ -18529,7 +18924,7 @@
         <v>402</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E191" s="2">
         <v>2479900</v>
@@ -18546,7 +18941,7 @@
         <v>402</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E192" s="2">
         <v>3959000</v>
@@ -18557,13 +18952,13 @@
         <v>114</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>1016</v>
+        <v>1045</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>1006</v>
+        <v>1035</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E193" s="2">
         <v>2890000</v>
@@ -18574,13 +18969,13 @@
         <v>114</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>1017</v>
+        <v>1046</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>1006</v>
+        <v>1035</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E194" s="2">
         <v>4080000</v>
@@ -18591,13 +18986,13 @@
         <v>114</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>1018</v>
+        <v>1047</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E195" s="2">
         <v>6290000</v>
@@ -18605,7 +19000,7 @@
     </row>
     <row r="196" ht="27.15" hidden="1" spans="1:5">
       <c r="A196" s="1" t="s">
-        <v>970</v>
+        <v>999</v>
       </c>
       <c r="B196" s="2">
         <v>6</v>
@@ -18614,7 +19009,7 @@
         <v>402</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E196" s="2">
         <v>2200000</v>
@@ -18622,7 +19017,7 @@
     </row>
     <row r="197" ht="27.15" hidden="1" spans="1:5">
       <c r="A197" s="1" t="s">
-        <v>969</v>
+        <v>998</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>272</v>
@@ -18631,7 +19026,7 @@
         <v>402</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E197" s="2">
         <v>4599000</v>
@@ -18648,7 +19043,7 @@
         <v>402</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E198" s="2">
         <v>2199000</v>
@@ -18659,13 +19054,13 @@
         <v>208</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>1019</v>
+        <v>1048</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>928</v>
+        <v>957</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E199" s="2">
         <v>4599000</v>
@@ -18676,13 +19071,13 @@
         <v>98</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>1020</v>
+        <v>1049</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E200" s="2">
         <v>1990000</v>
@@ -18693,13 +19088,13 @@
         <v>98</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>1021</v>
+        <v>1050</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E201" s="2">
         <v>3590000</v>
@@ -18716,7 +19111,7 @@
         <v>402</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>918</v>
+        <v>947</v>
       </c>
       <c r="E202" s="2">
         <v>2650000</v>
@@ -18727,13 +19122,13 @@
         <v>208</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>1022</v>
+        <v>1051</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>928</v>
+        <v>957</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E203" s="2">
         <v>2849000</v>
@@ -18741,7 +19136,7 @@
     </row>
     <row r="204" ht="27.15" hidden="1" spans="1:5">
       <c r="A204" s="1" t="s">
-        <v>1010</v>
+        <v>1039</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>164</v>
@@ -18750,7 +19145,7 @@
         <v>402</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E204" s="2">
         <v>2099000</v>
@@ -18767,7 +19162,7 @@
         <v>402</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>1023</v>
+        <v>1052</v>
       </c>
       <c r="E205" s="2">
         <v>1263000</v>
@@ -18784,7 +19179,7 @@
         <v>402</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>921</v>
+        <v>950</v>
       </c>
       <c r="E206" s="2">
         <v>1546500</v>
@@ -18801,7 +19196,7 @@
         <v>402</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>1024</v>
+        <v>1053</v>
       </c>
       <c r="E207" s="2">
         <v>883000</v>
@@ -18818,7 +19213,7 @@
         <v>402</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>1025</v>
+        <v>1054</v>
       </c>
       <c r="E208" s="2">
         <v>825000</v>
@@ -18835,7 +19230,7 @@
         <v>402</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>1024</v>
+        <v>1053</v>
       </c>
       <c r="E209" s="2">
         <v>851000</v>
@@ -18846,13 +19241,13 @@
         <v>169</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>1026</v>
+        <v>1055</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>1006</v>
+        <v>1035</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E210" s="2">
         <v>3357990</v>
@@ -18863,13 +19258,13 @@
         <v>208</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>1027</v>
+        <v>1056</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>928</v>
+        <v>957</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E211" s="2">
         <v>3899000</v>
@@ -18886,7 +19281,7 @@
         <v>402</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E212" s="2">
         <v>1990000</v>
@@ -18903,7 +19298,7 @@
         <v>402</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E213" s="2">
         <v>2199000</v>
@@ -18920,7 +19315,7 @@
         <v>402</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>981</v>
+        <v>1010</v>
       </c>
       <c r="E214" s="2">
         <v>789900</v>
@@ -18934,10 +19329,10 @@
         <v>388</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>1006</v>
+        <v>1035</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>1028</v>
+        <v>1057</v>
       </c>
       <c r="E215" s="2">
         <v>869900</v>
@@ -18954,7 +19349,7 @@
         <v>402</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>1029</v>
+        <v>1058</v>
       </c>
       <c r="E216" s="2">
         <v>1089000</v>
@@ -18971,7 +19366,7 @@
         <v>402</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>1024</v>
+        <v>1053</v>
       </c>
       <c r="E217" s="2">
         <v>999900</v>
@@ -18988,7 +19383,7 @@
         <v>402</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>1025</v>
+        <v>1054</v>
       </c>
       <c r="E218" s="2">
         <v>1455000</v>
@@ -19002,10 +19397,10 @@
         <v>386</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>928</v>
+        <v>957</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>1028</v>
+        <v>1057</v>
       </c>
       <c r="E219" s="2">
         <v>809900</v>
@@ -19022,7 +19417,7 @@
         <v>402</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>935</v>
+        <v>964</v>
       </c>
       <c r="E220" s="2">
         <v>2000000</v>
@@ -19039,7 +19434,7 @@
         <v>402</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>1024</v>
+        <v>1053</v>
       </c>
       <c r="E221" s="2">
         <v>1229900</v>
@@ -19056,7 +19451,7 @@
         <v>402</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>952</v>
+        <v>981</v>
       </c>
       <c r="E222" s="2">
         <v>2656800</v>
@@ -19067,13 +19462,13 @@
         <v>328</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>1030</v>
+        <v>1059</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>974</v>
+        <v>1003</v>
       </c>
       <c r="E223" s="2">
         <v>824000</v>
@@ -19084,13 +19479,13 @@
         <v>288</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>1031</v>
+        <v>1060</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>980</v>
+        <v>1009</v>
       </c>
       <c r="E224" s="2">
         <v>1204900</v>
@@ -19107,7 +19502,7 @@
         <v>402</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>943</v>
+        <v>972</v>
       </c>
       <c r="E225" s="2">
         <v>2234900</v>
@@ -19115,16 +19510,16 @@
     </row>
     <row r="226" ht="40.35" hidden="1" spans="1:5">
       <c r="A226" s="1" t="s">
-        <v>966</v>
+        <v>995</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>950</v>
+        <v>979</v>
       </c>
       <c r="E226" s="2">
         <v>2673000</v>
@@ -19141,7 +19536,7 @@
         <v>402</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>1032</v>
+        <v>1061</v>
       </c>
       <c r="E227" s="2">
         <v>1419990</v>
@@ -19149,7 +19544,7 @@
     </row>
     <row r="228" ht="27.15" hidden="1" spans="1:5">
       <c r="A228" s="1" t="s">
-        <v>959</v>
+        <v>988</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>265</v>
@@ -19158,7 +19553,7 @@
         <v>402</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>1033</v>
+        <v>1062</v>
       </c>
       <c r="E228" s="2">
         <v>1494000</v>
@@ -19175,7 +19570,7 @@
         <v>402</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E229" s="2">
         <v>2849990</v>
@@ -19189,10 +19584,10 @@
         <v>573</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>1034</v>
+        <v>1063</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>946</v>
+        <v>975</v>
       </c>
       <c r="E230" s="2">
         <v>3173000</v>
@@ -19203,13 +19598,13 @@
         <v>50</v>
       </c>
       <c r="B231" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C231" s="1" t="s">
         <v>1035</v>
       </c>
-      <c r="C231" s="1" t="s">
-        <v>1006</v>
-      </c>
       <c r="D231" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E231" s="2">
         <v>2380000</v>
@@ -19226,7 +19621,7 @@
         <v>402</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E232" s="2">
         <v>2599000</v>
@@ -19234,16 +19629,16 @@
     </row>
     <row r="233" ht="27.15" hidden="1" spans="1:5">
       <c r="A233" s="1" t="s">
-        <v>1014</v>
+        <v>1043</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>1036</v>
+        <v>1065</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E233" s="2">
         <v>2999000</v>
@@ -19254,13 +19649,13 @@
         <v>20</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>1037</v>
+        <v>1066</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>956</v>
+        <v>985</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E234" s="2">
         <v>3590000</v>
@@ -19268,16 +19663,16 @@
     </row>
     <row r="235" ht="40.35" hidden="1" spans="1:5">
       <c r="A235" s="1" t="s">
-        <v>960</v>
+        <v>989</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>1038</v>
+        <v>1067</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E235" s="2">
         <v>2569900</v>
@@ -19294,7 +19689,7 @@
         <v>402</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E236" s="2">
         <v>4750000</v>
@@ -19302,16 +19697,16 @@
     </row>
     <row r="237" ht="40.35" hidden="1" spans="1:5">
       <c r="A237" s="1" t="s">
-        <v>966</v>
+        <v>995</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>1039</v>
+        <v>1068</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E237" s="2">
         <v>2499990</v>
@@ -19319,7 +19714,7 @@
     </row>
     <row r="238" ht="27.15" hidden="1" spans="1:5">
       <c r="A238" s="1" t="s">
-        <v>966</v>
+        <v>995</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>770</v>
@@ -19328,7 +19723,7 @@
         <v>402</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E238" s="2">
         <v>2779990</v>
@@ -19342,10 +19737,10 @@
         <v>13</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>1006</v>
+        <v>1035</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E239" s="2">
         <v>2649000</v>
@@ -19359,10 +19754,10 @@
         <v>580</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>920</v>
+        <v>949</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>921</v>
+        <v>950</v>
       </c>
       <c r="E240" s="2">
         <v>1899000</v>
@@ -19379,7 +19774,7 @@
         <v>402</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E241" s="2">
         <v>2825990</v>
@@ -19387,7 +19782,7 @@
     </row>
     <row r="242" ht="27.15" hidden="1" spans="1:5">
       <c r="A242" s="1" t="s">
-        <v>937</v>
+        <v>966</v>
       </c>
       <c r="B242" s="2">
         <v>400</v>
@@ -19396,7 +19791,7 @@
         <v>402</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>932</v>
+        <v>961</v>
       </c>
       <c r="E242" s="2">
         <v>5799000</v>
@@ -19404,7 +19799,7 @@
     </row>
     <row r="243" ht="27.15" hidden="1" spans="1:5">
       <c r="A243" s="1" t="s">
-        <v>959</v>
+        <v>988</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>268</v>
@@ -19413,7 +19808,7 @@
         <v>402</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>1040</v>
+        <v>1069</v>
       </c>
       <c r="E243" s="2">
         <v>2899000</v>
@@ -19430,7 +19825,7 @@
         <v>402</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>921</v>
+        <v>950</v>
       </c>
       <c r="E244" s="2">
         <v>1887500</v>
@@ -19447,7 +19842,7 @@
         <v>402</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>921</v>
+        <v>950</v>
       </c>
       <c r="E245" s="2">
         <v>1805000</v>
@@ -19464,7 +19859,7 @@
         <v>402</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>927</v>
+        <v>956</v>
       </c>
       <c r="E246" s="2">
         <v>1684500</v>
@@ -19472,7 +19867,7 @@
     </row>
     <row r="247" ht="27.15" hidden="1" spans="1:5">
       <c r="A247" s="1" t="s">
-        <v>1041</v>
+        <v>1070</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>762</v>
@@ -19481,7 +19876,7 @@
         <v>402</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E247" s="2">
         <v>3899000</v>
@@ -19489,7 +19884,7 @@
     </row>
     <row r="248" ht="27.15" hidden="1" spans="1:5">
       <c r="A248" s="1" t="s">
-        <v>1041</v>
+        <v>1070</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>761</v>
@@ -19498,7 +19893,7 @@
         <v>402</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E248" s="2">
         <v>3099000</v>
@@ -19506,7 +19901,7 @@
     </row>
     <row r="249" ht="27.15" hidden="1" spans="1:5">
       <c r="A249" s="1" t="s">
-        <v>1042</v>
+        <v>1071</v>
       </c>
       <c r="B249" s="2">
         <v>1</v>
@@ -19515,7 +19910,7 @@
         <v>402</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>949</v>
+        <v>978</v>
       </c>
       <c r="E249" s="2">
         <v>4162990</v>

</xml_diff>

<commit_message>
Add rule to dmitrovka, moscow, add id > 169 to all regions
</commit_message>
<xml_diff>
--- a/id.xlsx
+++ b/id.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="8615"/>
+    <workbookView windowWidth="22188" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$E$879</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$E$907</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Лист2!$A$1:$E$249</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2815" uniqueCount="1072">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="1074">
   <si>
     <t>Aito</t>
   </si>
@@ -2852,6 +2852,12 @@
   </si>
   <si>
     <t>ET</t>
+  </si>
+  <si>
+    <t>H7</t>
+  </si>
+  <si>
+    <t>Empow</t>
   </si>
   <si>
     <t>Марка</t>
@@ -4238,10 +4244,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F907"/>
+  <dimension ref="A1:F909"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A890" workbookViewId="0">
-      <selection activeCell="E901" sqref="E901"/>
+    <sheetView tabSelected="1" topLeftCell="A892" workbookViewId="0">
+      <selection activeCell="G908" sqref="G908"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -15663,8 +15669,30 @@
         <v>939</v>
       </c>
     </row>
+    <row r="908" spans="1:3">
+      <c r="A908">
+        <v>1007</v>
+      </c>
+      <c r="B908" t="s">
+        <v>208</v>
+      </c>
+      <c r="C908" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="909" spans="1:3">
+      <c r="A909">
+        <v>1008</v>
+      </c>
+      <c r="B909" t="s">
+        <v>157</v>
+      </c>
+      <c r="C909" t="s">
+        <v>941</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:E879" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:E907" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15685,19 +15713,19 @@
   <sheetData>
     <row r="1" ht="27.15" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
     </row>
     <row r="2" ht="40.35" hidden="1" spans="1:5">
@@ -15705,13 +15733,13 @@
         <v>328</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E2" s="2">
         <v>1239900</v>
@@ -15725,10 +15753,10 @@
         <v>364</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E3" s="2">
         <v>1759000</v>
@@ -15742,10 +15770,10 @@
         <v>370</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E4" s="2">
         <v>1655000</v>
@@ -15759,10 +15787,10 @@
         <v>372</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E5" s="2">
         <v>1879000</v>
@@ -15773,13 +15801,13 @@
         <v>328</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E6" s="2">
         <v>1077000</v>
@@ -15793,10 +15821,10 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="E7" s="2">
         <v>1408000</v>
@@ -15807,13 +15835,13 @@
         <v>328</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E8" s="2">
         <v>749900</v>
@@ -15827,10 +15855,10 @@
         <v>330</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E9" s="2">
         <v>1175000</v>
@@ -15844,10 +15872,10 @@
         <v>242</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="E10" s="2">
         <v>2149000</v>
@@ -15861,10 +15889,10 @@
         <v>346</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E11" s="2">
         <v>1660000</v>
@@ -15878,10 +15906,10 @@
         <v>347</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E12" s="2">
         <v>2020000</v>
@@ -15895,10 +15923,10 @@
         <v>236</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="E13" s="2">
         <v>1859000</v>
@@ -15912,10 +15940,10 @@
         <v>300</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E14" s="2">
         <v>1334900</v>
@@ -15926,13 +15954,13 @@
         <v>169</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E15" s="2">
         <v>3512990</v>
@@ -15949,7 +15977,7 @@
         <v>402</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E16" s="2">
         <v>2836990</v>
@@ -15966,7 +15994,7 @@
         <v>402</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="E17" s="2">
         <v>1850000</v>
@@ -15980,10 +16008,10 @@
         <v>256</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="E18" s="2">
         <v>2749000</v>
@@ -15997,10 +16025,10 @@
         <v>180</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E19" s="2">
         <v>2179990</v>
@@ -16011,13 +16039,13 @@
         <v>169</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E20" s="2">
         <v>2794990</v>
@@ -16031,10 +16059,10 @@
         <v>190</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E21" s="2">
         <v>3959990</v>
@@ -16042,7 +16070,7 @@
     </row>
     <row r="22" ht="27.15" hidden="1" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="B22" s="2">
         <v>300</v>
@@ -16051,7 +16079,7 @@
         <v>402</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E22" s="2">
         <v>4499000</v>
@@ -16059,7 +16087,7 @@
     </row>
     <row r="23" ht="27.15" hidden="1" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="B23" s="2">
         <v>500</v>
@@ -16068,7 +16096,7 @@
         <v>402</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E23" s="2">
         <v>6799000</v>
@@ -16079,13 +16107,13 @@
         <v>328</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E24" s="2">
         <v>778500</v>
@@ -16096,13 +16124,13 @@
         <v>328</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E25" s="2">
         <v>719300</v>
@@ -16113,13 +16141,13 @@
         <v>328</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E26" s="2">
         <v>950900</v>
@@ -16133,10 +16161,10 @@
         <v>363</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E27" s="2">
         <v>1316900</v>
@@ -16147,13 +16175,13 @@
         <v>234</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="E28" s="2">
         <v>2769000</v>
@@ -16167,10 +16195,10 @@
         <v>290</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E29" s="2">
         <v>2244900</v>
@@ -16184,10 +16212,10 @@
         <v>305</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="E30" s="2">
         <v>1574900</v>
@@ -16201,10 +16229,10 @@
         <v>303</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="E31" s="2">
         <v>1434900</v>
@@ -16215,13 +16243,13 @@
         <v>328</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E32" s="2">
         <v>1059000</v>
@@ -16235,10 +16263,10 @@
         <v>249</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="E33" s="2">
         <v>3969000</v>
@@ -16255,7 +16283,7 @@
         <v>402</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E34" s="2">
         <v>1314000</v>
@@ -16266,13 +16294,13 @@
         <v>208</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E35" s="2">
         <v>2149000</v>
@@ -16286,10 +16314,10 @@
         <v>224</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="E36" s="2">
         <v>2599000</v>
@@ -16300,13 +16328,13 @@
         <v>208</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="E37" s="2">
         <v>2599000</v>
@@ -16323,7 +16351,7 @@
         <v>402</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="E38" s="2">
         <v>5269000</v>
@@ -16337,10 +16365,10 @@
         <v>292</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E39" s="2">
         <v>2314900</v>
@@ -16351,13 +16379,13 @@
         <v>328</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E40" s="2">
         <v>918900</v>
@@ -16371,10 +16399,10 @@
         <v>295</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E41" s="2">
         <v>2159900</v>
@@ -16391,7 +16419,7 @@
         <v>402</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E42" s="2">
         <v>1106900</v>
@@ -16408,7 +16436,7 @@
         <v>402</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E43" s="2">
         <v>1249900</v>
@@ -16425,7 +16453,7 @@
         <v>402</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E44" s="2">
         <v>2900000</v>
@@ -16436,13 +16464,13 @@
         <v>20</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E45" s="2">
         <v>2439900</v>
@@ -16456,10 +16484,10 @@
         <v>298</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E46" s="2">
         <v>2734900</v>
@@ -16473,10 +16501,10 @@
         <v>317</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E47" s="2">
         <v>1934900</v>
@@ -16493,7 +16521,7 @@
         <v>402</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E48" s="2">
         <v>2064900</v>
@@ -16507,10 +16535,10 @@
         <v>318</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E49" s="2">
         <v>2849900</v>
@@ -16518,7 +16546,7 @@
     </row>
     <row r="50" ht="27.15" hidden="1" spans="1:5">
       <c r="A50" s="1" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>267</v>
@@ -16527,7 +16555,7 @@
         <v>402</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E50" s="2">
         <v>1779000</v>
@@ -16535,7 +16563,7 @@
     </row>
     <row r="51" ht="27.15" hidden="1" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>261</v>
@@ -16544,7 +16572,7 @@
         <v>402</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E51" s="2">
         <v>2150000</v>
@@ -16552,7 +16580,7 @@
     </row>
     <row r="52" ht="27.15" hidden="1" spans="1:5">
       <c r="A52" s="1" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>266</v>
@@ -16561,7 +16589,7 @@
         <v>402</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E52" s="2">
         <v>2129900</v>
@@ -16569,7 +16597,7 @@
     </row>
     <row r="53" ht="27.15" hidden="1" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>456</v>
@@ -16578,7 +16606,7 @@
         <v>402</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E53" s="2">
         <v>2369900</v>
@@ -16595,7 +16623,7 @@
         <v>402</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E54" s="2">
         <v>1690000</v>
@@ -16612,7 +16640,7 @@
         <v>402</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E55" s="2">
         <v>2869900</v>
@@ -16623,13 +16651,13 @@
         <v>20</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E56" s="2">
         <v>2569900</v>
@@ -16640,13 +16668,13 @@
         <v>20</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E57" s="2">
         <v>2839900</v>
@@ -16660,10 +16688,10 @@
         <v>27</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E58" s="2">
         <v>3969900</v>
@@ -16677,10 +16705,10 @@
         <v>30</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E59" s="2">
         <v>3069900</v>
@@ -16694,10 +16722,10 @@
         <v>33</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E60" s="2">
         <v>3069900</v>
@@ -16708,13 +16736,13 @@
         <v>20</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E61" s="2">
         <v>2899900</v>
@@ -16722,16 +16750,16 @@
     </row>
     <row r="62" ht="40.35" hidden="1" spans="1:5">
       <c r="A62" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>128</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E62" s="2">
         <v>2374000</v>
@@ -16739,16 +16767,16 @@
     </row>
     <row r="63" ht="40.35" hidden="1" spans="1:5">
       <c r="A63" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>129</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E63" s="2">
         <v>2411000</v>
@@ -16756,16 +16784,16 @@
     </row>
     <row r="64" ht="40.35" hidden="1" spans="1:5">
       <c r="A64" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E64" s="2">
         <v>2024000</v>
@@ -16779,10 +16807,10 @@
         <v>494</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="E65" s="2">
         <v>1124000</v>
@@ -16796,10 +16824,10 @@
         <v>519</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E66" s="2">
         <v>1051000</v>
@@ -16813,10 +16841,10 @@
         <v>516</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E67" s="2">
         <v>1657000</v>
@@ -16830,10 +16858,10 @@
         <v>509</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E68" s="2">
         <v>1705000</v>
@@ -16847,10 +16875,10 @@
         <v>57</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E69" s="2">
         <v>1699900</v>
@@ -16864,10 +16892,10 @@
         <v>274</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E70" s="2">
         <v>2489900</v>
@@ -16875,16 +16903,16 @@
     </row>
     <row r="71" ht="40.35" hidden="1" spans="1:5">
       <c r="A71" s="1" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>261</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E71" s="2">
         <v>2959900</v>
@@ -16892,16 +16920,16 @@
     </row>
     <row r="72" ht="40.35" hidden="1" spans="1:5">
       <c r="A72" s="1" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="B72" s="2">
         <v>3</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E72" s="2">
         <v>1765000</v>
@@ -16915,10 +16943,10 @@
         <v>447</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="E73" s="2">
         <v>4409000</v>
@@ -16932,10 +16960,10 @@
         <v>452</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="E74" s="2">
         <v>1690000</v>
@@ -16949,10 +16977,10 @@
         <v>79</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E75" s="2">
         <v>950900</v>
@@ -16969,7 +16997,7 @@
         <v>402</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E76" s="2">
         <v>880900</v>
@@ -16983,10 +17011,10 @@
         <v>77</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E77" s="2">
         <v>953900</v>
@@ -17000,10 +17028,10 @@
         <v>227</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E78" s="2">
         <v>2179000</v>
@@ -17020,7 +17048,7 @@
         <v>402</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="E79" s="2">
         <v>1579000</v>
@@ -17034,10 +17062,10 @@
         <v>220</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E80" s="2">
         <v>4299000</v>
@@ -17054,7 +17082,7 @@
         <v>402</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E81" s="2">
         <v>2049000</v>
@@ -17071,7 +17099,7 @@
         <v>402</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E82" s="2">
         <v>3149000</v>
@@ -17085,10 +17113,10 @@
         <v>450</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="E83" s="2">
         <v>2337000</v>
@@ -17099,13 +17127,13 @@
         <v>441</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="E84" s="2">
         <v>2762000</v>
@@ -17119,10 +17147,10 @@
         <v>489</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E85" s="2">
         <v>1618000</v>
@@ -17136,10 +17164,10 @@
         <v>495</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="E86" s="2">
         <v>1301000</v>
@@ -17153,10 +17181,10 @@
         <v>501</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="E87" s="2">
         <v>1258000</v>
@@ -17170,10 +17198,10 @@
         <v>502</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="E88" s="2">
         <v>1373000</v>
@@ -17187,10 +17215,10 @@
         <v>492</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="E89" s="2">
         <v>1724000</v>
@@ -17207,7 +17235,7 @@
         <v>402</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E90" s="2">
         <v>1874000</v>
@@ -17221,10 +17249,10 @@
         <v>512</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E91" s="2">
         <v>2057000</v>
@@ -17238,10 +17266,10 @@
         <v>528</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E92" s="2">
         <v>2118900</v>
@@ -17255,10 +17283,10 @@
         <v>529</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E93" s="2">
         <v>3248000</v>
@@ -17272,10 +17300,10 @@
         <v>530</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E94" s="2">
         <v>5378000</v>
@@ -17289,10 +17317,10 @@
         <v>531</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E95" s="2">
         <v>5806000</v>
@@ -17306,10 +17334,10 @@
         <v>523</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E96" s="2">
         <v>2388000</v>
@@ -17323,10 +17351,10 @@
         <v>524</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E97" s="2">
         <v>2681000</v>
@@ -17340,10 +17368,10 @@
         <v>595</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="E98" s="2">
         <v>1385900</v>
@@ -17357,10 +17385,10 @@
         <v>279</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="E99" s="2">
         <v>1518000</v>
@@ -17374,10 +17402,10 @@
         <v>600</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E100" s="2">
         <v>3375900</v>
@@ -17394,7 +17422,7 @@
         <v>402</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E101" s="2">
         <v>2828900</v>
@@ -17408,10 +17436,10 @@
         <v>32</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E102" s="2">
         <v>4449900</v>
@@ -17428,7 +17456,7 @@
         <v>402</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="E103" s="2">
         <v>1229000</v>
@@ -17442,10 +17470,10 @@
         <v>580</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E104" s="2">
         <v>2499000</v>
@@ -17453,16 +17481,16 @@
     </row>
     <row r="105" ht="40.35" hidden="1" spans="1:5">
       <c r="A105" s="1" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>577</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="E105" s="2">
         <v>1680000</v>
@@ -17470,16 +17498,16 @@
     </row>
     <row r="106" ht="40.35" hidden="1" spans="1:5">
       <c r="A106" s="1" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B106" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>1014</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>1012</v>
-      </c>
       <c r="D106" s="1" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="E106" s="2">
         <v>1705000</v>
@@ -17487,7 +17515,7 @@
     </row>
     <row r="107" ht="27.15" hidden="1" spans="1:5">
       <c r="A107" s="1" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>36</v>
@@ -17496,7 +17524,7 @@
         <v>402</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="E107" s="2">
         <v>1510000</v>
@@ -17513,7 +17541,7 @@
         <v>402</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E108" s="2">
         <v>2570000</v>
@@ -17530,7 +17558,7 @@
         <v>402</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E109" s="2">
         <v>3430000</v>
@@ -17541,13 +17569,13 @@
         <v>50</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E110" s="2">
         <v>2770000</v>
@@ -17561,10 +17589,10 @@
         <v>906</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E111" s="2">
         <v>1970000</v>
@@ -17575,13 +17603,13 @@
         <v>50</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E112" s="2">
         <v>3250000</v>
@@ -17592,13 +17620,13 @@
         <v>50</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E113" s="2">
         <v>3370000</v>
@@ -17615,7 +17643,7 @@
         <v>402</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E114" s="2">
         <v>3759900</v>
@@ -17629,10 +17657,10 @@
         <v>117</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E115" s="2">
         <v>3380000</v>
@@ -17646,10 +17674,10 @@
         <v>115</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E116" s="2">
         <v>3810000</v>
@@ -17666,7 +17694,7 @@
         <v>402</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E117" s="2">
         <v>4910000</v>
@@ -17683,7 +17711,7 @@
         <v>402</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E118" s="2">
         <v>4550000</v>
@@ -17700,7 +17728,7 @@
         <v>402</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E119" s="2">
         <v>2080000</v>
@@ -17717,7 +17745,7 @@
         <v>402</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E120" s="2">
         <v>2225000</v>
@@ -17734,7 +17762,7 @@
         <v>402</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E121" s="2">
         <v>2970000</v>
@@ -17748,10 +17776,10 @@
         <v>4</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E122" s="2">
         <v>4350000</v>
@@ -17765,10 +17793,10 @@
         <v>277</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E123" s="2">
         <v>2999900</v>
@@ -17785,7 +17813,7 @@
         <v>402</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E124" s="2">
         <v>3479900</v>
@@ -17799,10 +17827,10 @@
         <v>281</v>
       </c>
       <c r="C125" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="D125" s="1" t="s">
         <v>949</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>947</v>
       </c>
       <c r="E125" s="2">
         <v>1990000</v>
@@ -17816,10 +17844,10 @@
         <v>282</v>
       </c>
       <c r="C126" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="D126" s="1" t="s">
         <v>949</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>947</v>
       </c>
       <c r="E126" s="2">
         <v>2149000</v>
@@ -17836,7 +17864,7 @@
         <v>402</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E127" s="2">
         <v>2115000</v>
@@ -17853,7 +17881,7 @@
         <v>402</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E128" s="2">
         <v>2238000</v>
@@ -17870,7 +17898,7 @@
         <v>402</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E129" s="2">
         <v>2514900</v>
@@ -17887,7 +17915,7 @@
         <v>402</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E130" s="2">
         <v>2997900</v>
@@ -17895,16 +17923,16 @@
     </row>
     <row r="131" ht="27.15" hidden="1" spans="1:5">
       <c r="A131" s="1" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E131" s="2">
         <v>2549900</v>
@@ -17912,16 +17940,16 @@
     </row>
     <row r="132" ht="27.15" hidden="1" spans="1:5">
       <c r="A132" s="1" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E132" s="2">
         <v>2629900</v>
@@ -17929,16 +17957,16 @@
     </row>
     <row r="133" ht="27.15" hidden="1" spans="1:5">
       <c r="A133" s="1" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E133" s="2">
         <v>4100000</v>
@@ -17955,7 +17983,7 @@
         <v>402</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="E134" s="2">
         <v>2219900</v>
@@ -17966,13 +17994,13 @@
         <v>20</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E135" s="2">
         <v>2499900</v>
@@ -17980,7 +18008,7 @@
     </row>
     <row r="136" ht="27.15" hidden="1" spans="1:5">
       <c r="A136" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>138</v>
@@ -17989,7 +18017,7 @@
         <v>402</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="E136" s="2">
         <v>1602000</v>
@@ -17997,16 +18025,16 @@
     </row>
     <row r="137" ht="40.35" hidden="1" spans="1:5">
       <c r="A137" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="E137" s="2">
         <v>1508000</v>
@@ -18023,7 +18051,7 @@
         <v>402</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E138" s="2">
         <v>4549990</v>
@@ -18040,7 +18068,7 @@
         <v>402</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E139" s="2">
         <v>2479990</v>
@@ -18057,7 +18085,7 @@
         <v>402</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="E140" s="2">
         <v>2075990</v>
@@ -18074,7 +18102,7 @@
         <v>402</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E141" s="2">
         <v>2080990</v>
@@ -18088,10 +18116,10 @@
         <v>369</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E142" s="2">
         <v>2273000</v>
@@ -18105,10 +18133,10 @@
         <v>651</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E143" s="2">
         <v>2443000</v>
@@ -18122,10 +18150,10 @@
         <v>670</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E144" s="2">
         <v>1341000</v>
@@ -18136,13 +18164,13 @@
         <v>328</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E145" s="2">
         <v>1381000</v>
@@ -18153,13 +18181,13 @@
         <v>328</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E146" s="2">
         <v>1493000</v>
@@ -18170,13 +18198,13 @@
         <v>328</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E147" s="2">
         <v>1533000</v>
@@ -18190,10 +18218,10 @@
         <v>348</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E148" s="2">
         <v>1670000</v>
@@ -18210,7 +18238,7 @@
         <v>402</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E149" s="2">
         <v>1487000</v>
@@ -18221,13 +18249,13 @@
         <v>50</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E150" s="2">
         <v>4850000</v>
@@ -18238,13 +18266,13 @@
         <v>50</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>1030</v>
+        <v>1032</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E151" s="2">
         <v>4000000</v>
@@ -18255,13 +18283,13 @@
         <v>50</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E152" s="2">
         <v>4930000</v>
@@ -18275,10 +18303,10 @@
         <v>187</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E153" s="2">
         <v>3692990</v>
@@ -18292,10 +18320,10 @@
         <v>734</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="E154" s="2">
         <v>3979000</v>
@@ -18312,7 +18340,7 @@
         <v>402</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E155" s="2">
         <v>4099000</v>
@@ -18329,7 +18357,7 @@
         <v>402</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E156" s="2">
         <v>3449000</v>
@@ -18346,7 +18374,7 @@
         <v>402</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E157" s="2">
         <v>2799000</v>
@@ -18357,13 +18385,13 @@
         <v>193</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E158" s="2">
         <v>3549000</v>
@@ -18374,13 +18402,13 @@
         <v>193</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E159" s="2">
         <v>3299000</v>
@@ -18394,10 +18422,10 @@
         <v>315</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E160" s="2">
         <v>7374900</v>
@@ -18411,10 +18439,10 @@
         <v>324</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E161" s="2">
         <v>3789900</v>
@@ -18428,10 +18456,10 @@
         <v>326</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E162" s="2">
         <v>5829900</v>
@@ -18445,10 +18473,10 @@
         <v>289</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E163" s="2">
         <v>4144900</v>
@@ -18456,16 +18484,16 @@
     </row>
     <row r="164" ht="27.15" hidden="1" spans="1:5">
       <c r="A164" s="1" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E164" s="2">
         <v>1672000</v>
@@ -18482,7 +18510,7 @@
         <v>402</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E165" s="2">
         <v>2040546</v>
@@ -18499,7 +18527,7 @@
         <v>402</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E166" s="2">
         <v>3100000</v>
@@ -18516,7 +18544,7 @@
         <v>402</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E167" s="2">
         <v>2990000</v>
@@ -18530,10 +18558,10 @@
         <v>602</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E168" s="2">
         <v>8669500</v>
@@ -18547,10 +18575,10 @@
         <v>654</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>1037</v>
+        <v>1039</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E169" s="2">
         <v>4291000</v>
@@ -18564,10 +18592,10 @@
         <v>598</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E170" s="2">
         <v>6146500</v>
@@ -18575,7 +18603,7 @@
     </row>
     <row r="171" ht="27.15" hidden="1" spans="1:5">
       <c r="A171" s="1" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>262</v>
@@ -18584,7 +18612,7 @@
         <v>402</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E171" s="2">
         <v>1889000</v>
@@ -18592,7 +18620,7 @@
     </row>
     <row r="172" ht="27.15" hidden="1" spans="1:5">
       <c r="A172" s="1" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>264</v>
@@ -18601,7 +18629,7 @@
         <v>402</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E172" s="2">
         <v>2399000</v>
@@ -18609,7 +18637,7 @@
     </row>
     <row r="173" ht="27.15" hidden="1" spans="1:5">
       <c r="A173" s="1" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>631</v>
@@ -18618,7 +18646,7 @@
         <v>402</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E173" s="2">
         <v>3059000</v>
@@ -18626,16 +18654,16 @@
     </row>
     <row r="174" ht="27.15" hidden="1" spans="1:5">
       <c r="A174" s="1" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E174" s="2">
         <v>3279000</v>
@@ -18643,7 +18671,7 @@
     </row>
     <row r="175" ht="27.15" hidden="1" spans="1:5">
       <c r="A175" s="1" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>632</v>
@@ -18652,7 +18680,7 @@
         <v>402</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E175" s="2">
         <v>3599000</v>
@@ -18660,7 +18688,7 @@
     </row>
     <row r="176" ht="27.15" hidden="1" spans="1:5">
       <c r="A176" s="1" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>168</v>
@@ -18669,7 +18697,7 @@
         <v>402</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E176" s="2">
         <v>5499999</v>
@@ -18677,16 +18705,16 @@
     </row>
     <row r="177" ht="27.15" hidden="1" spans="1:5">
       <c r="A177" s="1" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>165</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E177" s="2">
         <v>4099000</v>
@@ -18694,7 +18722,7 @@
     </row>
     <row r="178" ht="27.15" hidden="1" spans="1:5">
       <c r="A178" s="1" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>162</v>
@@ -18703,7 +18731,7 @@
         <v>402</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E178" s="2">
         <v>2449000</v>
@@ -18714,13 +18742,13 @@
         <v>20</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E179" s="2">
         <v>4529900</v>
@@ -18737,7 +18765,7 @@
         <v>402</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E180" s="2">
         <v>3739900</v>
@@ -18748,13 +18776,13 @@
         <v>20</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E181" s="2">
         <v>5219900</v>
@@ -18765,13 +18793,13 @@
         <v>50</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E182" s="2">
         <v>2780000</v>
@@ -18788,7 +18816,7 @@
         <v>402</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E183" s="2">
         <v>2020000</v>
@@ -18805,7 +18833,7 @@
         <v>402</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E184" s="2">
         <v>2650000</v>
@@ -18822,7 +18850,7 @@
         <v>402</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E185" s="2">
         <v>2080000</v>
@@ -18839,7 +18867,7 @@
         <v>402</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E186" s="2">
         <v>2181000</v>
@@ -18853,10 +18881,10 @@
         <v>5</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E187" s="2">
         <v>2279000</v>
@@ -18870,10 +18898,10 @@
         <v>6</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E188" s="2">
         <v>2899000</v>
@@ -18887,10 +18915,10 @@
         <v>424</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E189" s="2">
         <v>2379000</v>
@@ -18898,16 +18926,16 @@
     </row>
     <row r="190" ht="27.15" hidden="1" spans="1:5">
       <c r="A190" s="1" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>1044</v>
+        <v>1046</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E190" s="2">
         <v>2499000</v>
@@ -18915,7 +18943,7 @@
     </row>
     <row r="191" ht="27.15" hidden="1" spans="1:5">
       <c r="A191" s="1" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>457</v>
@@ -18924,7 +18952,7 @@
         <v>402</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E191" s="2">
         <v>2479900</v>
@@ -18941,7 +18969,7 @@
         <v>402</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E192" s="2">
         <v>3959000</v>
@@ -18952,13 +18980,13 @@
         <v>114</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E193" s="2">
         <v>2890000</v>
@@ -18969,13 +18997,13 @@
         <v>114</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E194" s="2">
         <v>4080000</v>
@@ -18986,13 +19014,13 @@
         <v>114</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E195" s="2">
         <v>6290000</v>
@@ -19000,7 +19028,7 @@
     </row>
     <row r="196" ht="27.15" hidden="1" spans="1:5">
       <c r="A196" s="1" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="B196" s="2">
         <v>6</v>
@@ -19009,7 +19037,7 @@
         <v>402</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E196" s="2">
         <v>2200000</v>
@@ -19017,7 +19045,7 @@
     </row>
     <row r="197" ht="27.15" hidden="1" spans="1:5">
       <c r="A197" s="1" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>272</v>
@@ -19026,7 +19054,7 @@
         <v>402</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E197" s="2">
         <v>4599000</v>
@@ -19043,7 +19071,7 @@
         <v>402</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E198" s="2">
         <v>2199000</v>
@@ -19054,13 +19082,13 @@
         <v>208</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E199" s="2">
         <v>4599000</v>
@@ -19071,13 +19099,13 @@
         <v>98</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>1049</v>
+        <v>1051</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E200" s="2">
         <v>1990000</v>
@@ -19088,13 +19116,13 @@
         <v>98</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E201" s="2">
         <v>3590000</v>
@@ -19111,7 +19139,7 @@
         <v>402</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E202" s="2">
         <v>2650000</v>
@@ -19122,13 +19150,13 @@
         <v>208</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>1051</v>
+        <v>1053</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E203" s="2">
         <v>2849000</v>
@@ -19136,7 +19164,7 @@
     </row>
     <row r="204" ht="27.15" hidden="1" spans="1:5">
       <c r="A204" s="1" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>164</v>
@@ -19145,7 +19173,7 @@
         <v>402</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E204" s="2">
         <v>2099000</v>
@@ -19162,7 +19190,7 @@
         <v>402</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="E205" s="2">
         <v>1263000</v>
@@ -19179,7 +19207,7 @@
         <v>402</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E206" s="2">
         <v>1546500</v>
@@ -19196,7 +19224,7 @@
         <v>402</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="E207" s="2">
         <v>883000</v>
@@ -19213,7 +19241,7 @@
         <v>402</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="E208" s="2">
         <v>825000</v>
@@ -19230,7 +19258,7 @@
         <v>402</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="E209" s="2">
         <v>851000</v>
@@ -19241,13 +19269,13 @@
         <v>169</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E210" s="2">
         <v>3357990</v>
@@ -19258,13 +19286,13 @@
         <v>208</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E211" s="2">
         <v>3899000</v>
@@ -19281,7 +19309,7 @@
         <v>402</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E212" s="2">
         <v>1990000</v>
@@ -19298,7 +19326,7 @@
         <v>402</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E213" s="2">
         <v>2199000</v>
@@ -19315,7 +19343,7 @@
         <v>402</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="E214" s="2">
         <v>789900</v>
@@ -19329,10 +19357,10 @@
         <v>388</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="E215" s="2">
         <v>869900</v>
@@ -19349,7 +19377,7 @@
         <v>402</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="E216" s="2">
         <v>1089000</v>
@@ -19366,7 +19394,7 @@
         <v>402</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="E217" s="2">
         <v>999900</v>
@@ -19383,7 +19411,7 @@
         <v>402</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="E218" s="2">
         <v>1455000</v>
@@ -19397,10 +19425,10 @@
         <v>386</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="E219" s="2">
         <v>809900</v>
@@ -19417,7 +19445,7 @@
         <v>402</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="E220" s="2">
         <v>2000000</v>
@@ -19434,7 +19462,7 @@
         <v>402</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="E221" s="2">
         <v>1229900</v>
@@ -19451,7 +19479,7 @@
         <v>402</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="E222" s="2">
         <v>2656800</v>
@@ -19462,13 +19490,13 @@
         <v>328</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>1059</v>
+        <v>1061</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="E223" s="2">
         <v>824000</v>
@@ -19479,13 +19507,13 @@
         <v>288</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="E224" s="2">
         <v>1204900</v>
@@ -19502,7 +19530,7 @@
         <v>402</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="E225" s="2">
         <v>2234900</v>
@@ -19510,16 +19538,16 @@
     </row>
     <row r="226" ht="40.35" hidden="1" spans="1:5">
       <c r="A226" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="E226" s="2">
         <v>2673000</v>
@@ -19536,7 +19564,7 @@
         <v>402</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>1061</v>
+        <v>1063</v>
       </c>
       <c r="E227" s="2">
         <v>1419990</v>
@@ -19544,7 +19572,7 @@
     </row>
     <row r="228" ht="27.15" hidden="1" spans="1:5">
       <c r="A228" s="1" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>265</v>
@@ -19553,7 +19581,7 @@
         <v>402</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
       <c r="E228" s="2">
         <v>1494000</v>
@@ -19570,7 +19598,7 @@
         <v>402</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E229" s="2">
         <v>2849990</v>
@@ -19584,10 +19612,10 @@
         <v>573</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E230" s="2">
         <v>3173000</v>
@@ -19598,13 +19626,13 @@
         <v>50</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E231" s="2">
         <v>2380000</v>
@@ -19621,7 +19649,7 @@
         <v>402</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E232" s="2">
         <v>2599000</v>
@@ -19629,16 +19657,16 @@
     </row>
     <row r="233" ht="27.15" hidden="1" spans="1:5">
       <c r="A233" s="1" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E233" s="2">
         <v>2999000</v>
@@ -19649,13 +19677,13 @@
         <v>20</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>1066</v>
+        <v>1068</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E234" s="2">
         <v>3590000</v>
@@ -19663,16 +19691,16 @@
     </row>
     <row r="235" ht="40.35" hidden="1" spans="1:5">
       <c r="A235" s="1" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E235" s="2">
         <v>2569900</v>
@@ -19689,7 +19717,7 @@
         <v>402</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E236" s="2">
         <v>4750000</v>
@@ -19697,16 +19725,16 @@
     </row>
     <row r="237" ht="40.35" hidden="1" spans="1:5">
       <c r="A237" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E237" s="2">
         <v>2499990</v>
@@ -19714,7 +19742,7 @@
     </row>
     <row r="238" ht="27.15" hidden="1" spans="1:5">
       <c r="A238" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>770</v>
@@ -19723,7 +19751,7 @@
         <v>402</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E238" s="2">
         <v>2779990</v>
@@ -19737,10 +19765,10 @@
         <v>13</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E239" s="2">
         <v>2649000</v>
@@ -19754,10 +19782,10 @@
         <v>580</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E240" s="2">
         <v>1899000</v>
@@ -19774,7 +19802,7 @@
         <v>402</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E241" s="2">
         <v>2825990</v>
@@ -19782,7 +19810,7 @@
     </row>
     <row r="242" ht="27.15" hidden="1" spans="1:5">
       <c r="A242" s="1" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="B242" s="2">
         <v>400</v>
@@ -19791,7 +19819,7 @@
         <v>402</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E242" s="2">
         <v>5799000</v>
@@ -19799,7 +19827,7 @@
     </row>
     <row r="243" ht="27.15" hidden="1" spans="1:5">
       <c r="A243" s="1" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>268</v>
@@ -19808,7 +19836,7 @@
         <v>402</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="E243" s="2">
         <v>2899000</v>
@@ -19825,7 +19853,7 @@
         <v>402</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E244" s="2">
         <v>1887500</v>
@@ -19842,7 +19870,7 @@
         <v>402</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E245" s="2">
         <v>1805000</v>
@@ -19859,7 +19887,7 @@
         <v>402</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E246" s="2">
         <v>1684500</v>
@@ -19867,7 +19895,7 @@
     </row>
     <row r="247" ht="27.15" hidden="1" spans="1:5">
       <c r="A247" s="1" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>762</v>
@@ -19876,7 +19904,7 @@
         <v>402</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E247" s="2">
         <v>3899000</v>
@@ -19884,7 +19912,7 @@
     </row>
     <row r="248" ht="27.15" hidden="1" spans="1:5">
       <c r="A248" s="1" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>761</v>
@@ -19893,7 +19921,7 @@
         <v>402</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E248" s="2">
         <v>3099000</v>
@@ -19901,7 +19929,7 @@
     </row>
     <row r="249" ht="27.15" hidden="1" spans="1:5">
       <c r="A249" s="1" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="B249" s="2">
         <v>1</v>
@@ -19910,7 +19938,7 @@
         <v>402</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E249" s="2">
         <v>4162990</v>

</xml_diff>

<commit_message>
Add rule to kemerovo
</commit_message>
<xml_diff>
--- a/id.xlsx
+++ b/id.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$G$911</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$G$912</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Лист2!$A$1:$E$249</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3051" uniqueCount="1079">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3055" uniqueCount="1081">
   <si>
     <t>Aito</t>
   </si>
@@ -2936,6 +2936,12 @@
   </si>
   <si>
     <t>Avante</t>
+  </si>
+  <si>
+    <t>GS8 Traveller</t>
+  </si>
+  <si>
+    <t>X70 New</t>
   </si>
   <si>
     <t>Марка</t>
@@ -4259,10 +4265,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G912"/>
+  <dimension ref="A1:G914"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A893" workbookViewId="0">
-      <selection activeCell="E909" sqref="E909"/>
+      <selection activeCell="G910" sqref="G910"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -16418,8 +16424,30 @@
         <v>967</v>
       </c>
     </row>
+    <row r="913" spans="1:3">
+      <c r="A913">
+        <v>1012</v>
+      </c>
+      <c r="B913" t="s">
+        <v>164</v>
+      </c>
+      <c r="C913" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="914" spans="1:3">
+      <c r="A914">
+        <v>1013</v>
+      </c>
+      <c r="B914" t="s">
+        <v>285</v>
+      </c>
+      <c r="C914" t="s">
+        <v>969</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G911" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G912" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -16440,19 +16468,19 @@
   <sheetData>
     <row r="1" ht="27.15" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
     </row>
     <row r="2" ht="40.35" hidden="1" customHeight="1" spans="1:5">
@@ -16460,13 +16488,13 @@
         <v>344</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>380</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E2" s="2">
         <v>1239900</v>
@@ -16483,7 +16511,7 @@
         <v>380</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E3" s="2">
         <v>1759000</v>
@@ -16500,7 +16528,7 @@
         <v>380</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E4" s="2">
         <v>1655000</v>
@@ -16517,7 +16545,7 @@
         <v>380</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E5" s="2">
         <v>1879000</v>
@@ -16528,13 +16556,13 @@
         <v>344</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E6" s="2">
         <v>1077000</v>
@@ -16551,7 +16579,7 @@
         <v>82</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="E7" s="2">
         <v>1408000</v>
@@ -16562,13 +16590,13 @@
         <v>344</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E8" s="2">
         <v>749900</v>
@@ -16585,7 +16613,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E9" s="2">
         <v>1175000</v>
@@ -16602,7 +16630,7 @@
         <v>252</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="E10" s="2">
         <v>2149000</v>
@@ -16619,7 +16647,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E11" s="2">
         <v>1660000</v>
@@ -16636,7 +16664,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E12" s="2">
         <v>2020000</v>
@@ -16653,7 +16681,7 @@
         <v>103</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="E13" s="2">
         <v>1859000</v>
@@ -16670,7 +16698,7 @@
         <v>303</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E14" s="2">
         <v>1334900</v>
@@ -16681,13 +16709,13 @@
         <v>176</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E15" s="2">
         <v>3512990</v>
@@ -16704,7 +16732,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E16" s="2">
         <v>2836990</v>
@@ -16721,7 +16749,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E17" s="2">
         <v>1850000</v>
@@ -16738,7 +16766,7 @@
         <v>270</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="E18" s="2">
         <v>2749000</v>
@@ -16755,7 +16783,7 @@
         <v>103</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E19" s="2">
         <v>2179990</v>
@@ -16766,13 +16794,13 @@
         <v>176</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E20" s="2">
         <v>2794990</v>
@@ -16789,7 +16817,7 @@
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E21" s="2">
         <v>3959990</v>
@@ -16797,7 +16825,7 @@
     </row>
     <row r="22" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="B22" s="2">
         <v>300</v>
@@ -16806,7 +16834,7 @@
         <v>8</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E22" s="2">
         <v>4499000</v>
@@ -16814,7 +16842,7 @@
     </row>
     <row r="23" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="B23" s="2">
         <v>500</v>
@@ -16823,7 +16851,7 @@
         <v>8</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E23" s="2">
         <v>6799000</v>
@@ -16834,13 +16862,13 @@
         <v>344</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E24" s="2">
         <v>778500</v>
@@ -16851,13 +16879,13 @@
         <v>344</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E25" s="2">
         <v>719300</v>
@@ -16868,13 +16896,13 @@
         <v>344</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E26" s="2">
         <v>950900</v>
@@ -16891,7 +16919,7 @@
         <v>380</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E27" s="2">
         <v>1316900</v>
@@ -16902,13 +16930,13 @@
         <v>242</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>264</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="E28" s="2">
         <v>2769000</v>
@@ -16925,7 +16953,7 @@
         <v>303</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E29" s="2">
         <v>2244900</v>
@@ -16942,7 +16970,7 @@
         <v>259</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="E30" s="2">
         <v>1574900</v>
@@ -16959,7 +16987,7 @@
         <v>259</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="E31" s="2">
         <v>1434900</v>
@@ -16970,13 +16998,13 @@
         <v>344</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E32" s="2">
         <v>1059000</v>
@@ -16993,7 +17021,7 @@
         <v>259</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="E33" s="2">
         <v>3969000</v>
@@ -17010,7 +17038,7 @@
         <v>8</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="E34" s="2">
         <v>1314000</v>
@@ -17021,13 +17049,13 @@
         <v>215</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E35" s="2">
         <v>2149000</v>
@@ -17044,7 +17072,7 @@
         <v>5</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="E36" s="2">
         <v>2599000</v>
@@ -17055,13 +17083,13 @@
         <v>215</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="E37" s="2">
         <v>2599000</v>
@@ -17078,7 +17106,7 @@
         <v>8</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="E38" s="2">
         <v>5269000</v>
@@ -17095,7 +17123,7 @@
         <v>303</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E39" s="2">
         <v>2314900</v>
@@ -17106,13 +17134,13 @@
         <v>344</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E40" s="2">
         <v>918900</v>
@@ -17129,7 +17157,7 @@
         <v>259</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E41" s="2">
         <v>2159900</v>
@@ -17146,7 +17174,7 @@
         <v>8</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="E42" s="2">
         <v>1106900</v>
@@ -17163,7 +17191,7 @@
         <v>8</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="E43" s="2">
         <v>1249900</v>
@@ -17180,7 +17208,7 @@
         <v>8</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E44" s="2">
         <v>2900000</v>
@@ -17191,13 +17219,13 @@
         <v>22</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E45" s="2">
         <v>2439900</v>
@@ -17214,7 +17242,7 @@
         <v>312</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E46" s="2">
         <v>2734900</v>
@@ -17231,7 +17259,7 @@
         <v>312</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E47" s="2">
         <v>1934900</v>
@@ -17248,7 +17276,7 @@
         <v>8</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E48" s="2">
         <v>2064900</v>
@@ -17265,7 +17293,7 @@
         <v>334</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E49" s="2">
         <v>2849900</v>
@@ -17273,7 +17301,7 @@
     </row>
     <row r="50" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A50" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>279</v>
@@ -17282,7 +17310,7 @@
         <v>8</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E50" s="2">
         <v>1779000</v>
@@ -17290,7 +17318,7 @@
     </row>
     <row r="51" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>273</v>
@@ -17299,7 +17327,7 @@
         <v>8</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E51" s="2">
         <v>2150000</v>
@@ -17307,7 +17335,7 @@
     </row>
     <row r="52" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A52" s="1" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>278</v>
@@ -17316,7 +17344,7 @@
         <v>8</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E52" s="2">
         <v>2129900</v>
@@ -17324,7 +17352,7 @@
     </row>
     <row r="53" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>472</v>
@@ -17333,7 +17361,7 @@
         <v>8</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E53" s="2">
         <v>2369900</v>
@@ -17350,7 +17378,7 @@
         <v>8</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E54" s="2">
         <v>1690000</v>
@@ -17367,7 +17395,7 @@
         <v>8</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E55" s="2">
         <v>2869900</v>
@@ -17378,13 +17406,13 @@
         <v>22</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E56" s="2">
         <v>2569900</v>
@@ -17395,13 +17423,13 @@
         <v>22</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E57" s="2">
         <v>2839900</v>
@@ -17418,7 +17446,7 @@
         <v>26</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E58" s="2">
         <v>3969900</v>
@@ -17435,7 +17463,7 @@
         <v>26</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E59" s="2">
         <v>3069900</v>
@@ -17452,7 +17480,7 @@
         <v>26</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E60" s="2">
         <v>3069900</v>
@@ -17463,13 +17491,13 @@
         <v>22</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="E61" s="2">
         <v>2899900</v>
@@ -17477,7 +17505,7 @@
     </row>
     <row r="62" ht="40.35" customHeight="1" spans="1:5">
       <c r="A62" s="1" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>135</v>
@@ -17486,7 +17514,7 @@
         <v>26</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E62" s="2">
         <v>2374000</v>
@@ -17494,7 +17522,7 @@
     </row>
     <row r="63" ht="40.35" customHeight="1" spans="1:5">
       <c r="A63" s="1" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>136</v>
@@ -17503,7 +17531,7 @@
         <v>26</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E63" s="2">
         <v>2411000</v>
@@ -17511,7 +17539,7 @@
     </row>
     <row r="64" ht="40.35" customHeight="1" spans="1:5">
       <c r="A64" s="1" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>137</v>
@@ -17520,7 +17548,7 @@
         <v>26</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E64" s="2">
         <v>2024000</v>
@@ -17537,7 +17565,7 @@
         <v>82</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="E65" s="2">
         <v>1124000</v>
@@ -17554,7 +17582,7 @@
         <v>103</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E66" s="2">
         <v>1051000</v>
@@ -17571,7 +17599,7 @@
         <v>534</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E67" s="2">
         <v>1657000</v>
@@ -17588,7 +17616,7 @@
         <v>5</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E68" s="2">
         <v>1705000</v>
@@ -17605,7 +17633,7 @@
         <v>5</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="E69" s="2">
         <v>1699900</v>
@@ -17622,7 +17650,7 @@
         <v>26</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E70" s="2">
         <v>2489900</v>
@@ -17630,7 +17658,7 @@
     </row>
     <row r="71" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A71" s="1" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>273</v>
@@ -17639,7 +17667,7 @@
         <v>26</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E71" s="2">
         <v>2959900</v>
@@ -17647,7 +17675,7 @@
     </row>
     <row r="72" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A72" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="B72" s="2">
         <v>3</v>
@@ -17656,7 +17684,7 @@
         <v>26</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E72" s="2">
         <v>1765000</v>
@@ -17673,7 +17701,7 @@
         <v>226</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="E73" s="2">
         <v>4409000</v>
@@ -17690,7 +17718,7 @@
         <v>226</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="E74" s="2">
         <v>1690000</v>
@@ -17707,7 +17735,7 @@
         <v>85</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E75" s="2">
         <v>950900</v>
@@ -17724,7 +17752,7 @@
         <v>8</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="E76" s="2">
         <v>880900</v>
@@ -17741,7 +17769,7 @@
         <v>82</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E77" s="2">
         <v>953900</v>
@@ -17758,7 +17786,7 @@
         <v>103</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E78" s="2">
         <v>2179000</v>
@@ -17775,7 +17803,7 @@
         <v>8</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="E79" s="2">
         <v>1579000</v>
@@ -17792,7 +17820,7 @@
         <v>5</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="E80" s="2">
         <v>4299000</v>
@@ -17809,7 +17837,7 @@
         <v>8</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="E81" s="2">
         <v>2049000</v>
@@ -17826,7 +17854,7 @@
         <v>8</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E82" s="2">
         <v>3149000</v>
@@ -17843,7 +17871,7 @@
         <v>82</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="E83" s="2">
         <v>2337000</v>
@@ -17854,13 +17882,13 @@
         <v>457</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>303</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="E84" s="2">
         <v>2762000</v>
@@ -17877,7 +17905,7 @@
         <v>103</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E85" s="2">
         <v>1618000</v>
@@ -17894,7 +17922,7 @@
         <v>82</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="E86" s="2">
         <v>1301000</v>
@@ -17911,7 +17939,7 @@
         <v>82</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="E87" s="2">
         <v>1258000</v>
@@ -17928,7 +17956,7 @@
         <v>82</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="E88" s="2">
         <v>1373000</v>
@@ -17945,7 +17973,7 @@
         <v>5</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="E89" s="2">
         <v>1724000</v>
@@ -17962,7 +17990,7 @@
         <v>8</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E90" s="2">
         <v>1874000</v>
@@ -17979,7 +18007,7 @@
         <v>5</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E91" s="2">
         <v>2057000</v>
@@ -17996,7 +18024,7 @@
         <v>5</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E92" s="2">
         <v>2118900</v>
@@ -18013,7 +18041,7 @@
         <v>5</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E93" s="2">
         <v>3248000</v>
@@ -18030,7 +18058,7 @@
         <v>5</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E94" s="2">
         <v>5378000</v>
@@ -18047,7 +18075,7 @@
         <v>5</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E95" s="2">
         <v>5806000</v>
@@ -18064,7 +18092,7 @@
         <v>303</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E96" s="2">
         <v>2388000</v>
@@ -18081,7 +18109,7 @@
         <v>303</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E97" s="2">
         <v>2681000</v>
@@ -18098,7 +18126,7 @@
         <v>617</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="E98" s="2">
         <v>1385900</v>
@@ -18115,7 +18143,7 @@
         <v>608</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="E99" s="2">
         <v>1518000</v>
@@ -18132,7 +18160,7 @@
         <v>82</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E100" s="2">
         <v>3375900</v>
@@ -18149,7 +18177,7 @@
         <v>8</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E101" s="2">
         <v>2828900</v>
@@ -18166,7 +18194,7 @@
         <v>5</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E102" s="2">
         <v>4449900</v>
@@ -18183,7 +18211,7 @@
         <v>8</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="E103" s="2">
         <v>1229000</v>
@@ -18200,7 +18228,7 @@
         <v>103</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E104" s="2">
         <v>2499000</v>
@@ -18208,7 +18236,7 @@
     </row>
     <row r="105" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A105" s="1" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>595</v>
@@ -18217,7 +18245,7 @@
         <v>596</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="E105" s="2">
         <v>1680000</v>
@@ -18225,16 +18253,16 @@
     </row>
     <row r="106" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A106" s="1" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>596</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="E106" s="2">
         <v>1705000</v>
@@ -18242,7 +18270,7 @@
     </row>
     <row r="107" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A107" s="1" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>39</v>
@@ -18251,7 +18279,7 @@
         <v>8</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="E107" s="2">
         <v>1510000</v>
@@ -18268,7 +18296,7 @@
         <v>8</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E108" s="2">
         <v>2570000</v>
@@ -18285,7 +18313,7 @@
         <v>8</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E109" s="2">
         <v>3430000</v>
@@ -18296,13 +18324,13 @@
         <v>54</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E110" s="2">
         <v>2770000</v>
@@ -18319,7 +18347,7 @@
         <v>5</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E111" s="2">
         <v>1970000</v>
@@ -18330,13 +18358,13 @@
         <v>54</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E112" s="2">
         <v>3250000</v>
@@ -18347,13 +18375,13 @@
         <v>54</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E113" s="2">
         <v>3370000</v>
@@ -18370,7 +18398,7 @@
         <v>8</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E114" s="2">
         <v>3759900</v>
@@ -18387,7 +18415,7 @@
         <v>5</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E115" s="2">
         <v>3380000</v>
@@ -18404,7 +18432,7 @@
         <v>5</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E116" s="2">
         <v>3810000</v>
@@ -18421,7 +18449,7 @@
         <v>8</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E117" s="2">
         <v>4910000</v>
@@ -18438,7 +18466,7 @@
         <v>8</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E118" s="2">
         <v>4550000</v>
@@ -18455,7 +18483,7 @@
         <v>8</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E119" s="2">
         <v>2080000</v>
@@ -18472,7 +18500,7 @@
         <v>8</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E120" s="2">
         <v>2225000</v>
@@ -18489,7 +18517,7 @@
         <v>8</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E121" s="2">
         <v>2970000</v>
@@ -18506,7 +18534,7 @@
         <v>5</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E122" s="2">
         <v>4350000</v>
@@ -18523,7 +18551,7 @@
         <v>5</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E123" s="2">
         <v>2999900</v>
@@ -18540,7 +18568,7 @@
         <v>8</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E124" s="2">
         <v>3479900</v>
@@ -18557,7 +18585,7 @@
         <v>5</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E125" s="2">
         <v>1990000</v>
@@ -18574,7 +18602,7 @@
         <v>5</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E126" s="2">
         <v>2149000</v>
@@ -18591,7 +18619,7 @@
         <v>8</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E127" s="2">
         <v>2115000</v>
@@ -18608,7 +18636,7 @@
         <v>8</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E128" s="2">
         <v>2238000</v>
@@ -18625,7 +18653,7 @@
         <v>8</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E129" s="2">
         <v>2514900</v>
@@ -18642,7 +18670,7 @@
         <v>8</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E130" s="2">
         <v>2997900</v>
@@ -18650,16 +18678,16 @@
     </row>
     <row r="131" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A131" s="1" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>1030</v>
+        <v>1032</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E131" s="2">
         <v>2549900</v>
@@ -18667,16 +18695,16 @@
     </row>
     <row r="132" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A132" s="1" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E132" s="2">
         <v>2629900</v>
@@ -18684,16 +18712,16 @@
     </row>
     <row r="133" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A133" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E133" s="2">
         <v>4100000</v>
@@ -18710,7 +18738,7 @@
         <v>8</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="E134" s="2">
         <v>2219900</v>
@@ -18721,13 +18749,13 @@
         <v>22</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E135" s="2">
         <v>2499900</v>
@@ -18735,7 +18763,7 @@
     </row>
     <row r="136" ht="27.15" customHeight="1" spans="1:5">
       <c r="A136" s="1" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>145</v>
@@ -18744,7 +18772,7 @@
         <v>8</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="E136" s="2">
         <v>1602000</v>
@@ -18752,7 +18780,7 @@
     </row>
     <row r="137" ht="40.35" customHeight="1" spans="1:5">
       <c r="A137" s="1" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>146</v>
@@ -18761,7 +18789,7 @@
         <v>5</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="E137" s="2">
         <v>1508000</v>
@@ -18778,7 +18806,7 @@
         <v>8</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E138" s="2">
         <v>4549990</v>
@@ -18795,7 +18823,7 @@
         <v>8</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E139" s="2">
         <v>2479990</v>
@@ -18812,7 +18840,7 @@
         <v>8</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="E140" s="2">
         <v>2075990</v>
@@ -18829,7 +18857,7 @@
         <v>8</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E141" s="2">
         <v>2080990</v>
@@ -18846,7 +18874,7 @@
         <v>380</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E142" s="2">
         <v>2273000</v>
@@ -18863,7 +18891,7 @@
         <v>380</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E143" s="2">
         <v>2443000</v>
@@ -18880,7 +18908,7 @@
         <v>5</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E144" s="2">
         <v>1341000</v>
@@ -18891,13 +18919,13 @@
         <v>344</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E145" s="2">
         <v>1381000</v>
@@ -18908,13 +18936,13 @@
         <v>344</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>1037</v>
+        <v>1039</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E146" s="2">
         <v>1493000</v>
@@ -18925,13 +18953,13 @@
         <v>344</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E147" s="2">
         <v>1533000</v>
@@ -18948,7 +18976,7 @@
         <v>5</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E148" s="2">
         <v>1670000</v>
@@ -18965,7 +18993,7 @@
         <v>8</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E149" s="2">
         <v>1487000</v>
@@ -18976,13 +19004,13 @@
         <v>54</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E150" s="2">
         <v>4850000</v>
@@ -18993,13 +19021,13 @@
         <v>54</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E151" s="2">
         <v>4000000</v>
@@ -19010,13 +19038,13 @@
         <v>54</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E152" s="2">
         <v>4930000</v>
@@ -19033,7 +19061,7 @@
         <v>5</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E153" s="2">
         <v>3692990</v>
@@ -19050,7 +19078,7 @@
         <v>270</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="E154" s="2">
         <v>3979000</v>
@@ -19067,7 +19095,7 @@
         <v>8</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E155" s="2">
         <v>4099000</v>
@@ -19084,7 +19112,7 @@
         <v>8</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E156" s="2">
         <v>3449000</v>
@@ -19101,7 +19129,7 @@
         <v>8</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E157" s="2">
         <v>2799000</v>
@@ -19112,13 +19140,13 @@
         <v>200</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E158" s="2">
         <v>3549000</v>
@@ -19129,13 +19157,13 @@
         <v>200</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E159" s="2">
         <v>3299000</v>
@@ -19152,7 +19180,7 @@
         <v>330</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E160" s="2">
         <v>7374900</v>
@@ -19169,7 +19197,7 @@
         <v>270</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E161" s="2">
         <v>3789900</v>
@@ -19186,7 +19214,7 @@
         <v>51</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E162" s="2">
         <v>5829900</v>
@@ -19203,7 +19231,7 @@
         <v>270</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E163" s="2">
         <v>4144900</v>
@@ -19211,16 +19239,16 @@
     </row>
     <row r="164" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A164" s="1" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>1044</v>
+        <v>1046</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E164" s="2">
         <v>1672000</v>
@@ -19237,7 +19265,7 @@
         <v>8</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E165" s="2">
         <v>2040546</v>
@@ -19254,7 +19282,7 @@
         <v>8</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E166" s="2">
         <v>3100000</v>
@@ -19271,7 +19299,7 @@
         <v>8</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E167" s="2">
         <v>2990000</v>
@@ -19288,7 +19316,7 @@
         <v>312</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="E168" s="2">
         <v>8669500</v>
@@ -19305,7 +19333,7 @@
         <v>677</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E169" s="2">
         <v>4291000</v>
@@ -19322,7 +19350,7 @@
         <v>5</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E170" s="2">
         <v>6146500</v>
@@ -19330,7 +19358,7 @@
     </row>
     <row r="171" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A171" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>274</v>
@@ -19339,7 +19367,7 @@
         <v>8</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E171" s="2">
         <v>1889000</v>
@@ -19347,7 +19375,7 @@
     </row>
     <row r="172" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A172" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>276</v>
@@ -19356,7 +19384,7 @@
         <v>8</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E172" s="2">
         <v>2399000</v>
@@ -19364,7 +19392,7 @@
     </row>
     <row r="173" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A173" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>653</v>
@@ -19373,7 +19401,7 @@
         <v>8</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E173" s="2">
         <v>3059000</v>
@@ -19381,16 +19409,16 @@
     </row>
     <row r="174" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A174" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E174" s="2">
         <v>3279000</v>
@@ -19398,7 +19426,7 @@
     </row>
     <row r="175" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A175" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>654</v>
@@ -19407,7 +19435,7 @@
         <v>8</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E175" s="2">
         <v>3599000</v>
@@ -19415,7 +19443,7 @@
     </row>
     <row r="176" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A176" s="1" t="s">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>175</v>
@@ -19424,7 +19452,7 @@
         <v>8</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E176" s="2">
         <v>5499999</v>
@@ -19432,7 +19460,7 @@
     </row>
     <row r="177" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A177" s="1" t="s">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>172</v>
@@ -19441,7 +19469,7 @@
         <v>103</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E177" s="2">
         <v>4099000</v>
@@ -19449,7 +19477,7 @@
     </row>
     <row r="178" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A178" s="1" t="s">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>169</v>
@@ -19458,7 +19486,7 @@
         <v>8</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E178" s="2">
         <v>2449000</v>
@@ -19469,13 +19497,13 @@
         <v>22</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E179" s="2">
         <v>4529900</v>
@@ -19492,7 +19520,7 @@
         <v>8</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E180" s="2">
         <v>3739900</v>
@@ -19503,13 +19531,13 @@
         <v>22</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E181" s="2">
         <v>5219900</v>
@@ -19520,13 +19548,13 @@
         <v>54</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>1049</v>
+        <v>1051</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E182" s="2">
         <v>2780000</v>
@@ -19543,7 +19571,7 @@
         <v>8</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E183" s="2">
         <v>2020000</v>
@@ -19560,7 +19588,7 @@
         <v>8</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E184" s="2">
         <v>2650000</v>
@@ -19577,7 +19605,7 @@
         <v>8</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E185" s="2">
         <v>2080000</v>
@@ -19594,7 +19622,7 @@
         <v>8</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E186" s="2">
         <v>2181000</v>
@@ -19611,7 +19639,7 @@
         <v>5</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="E187" s="2">
         <v>2279000</v>
@@ -19628,7 +19656,7 @@
         <v>103</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="E188" s="2">
         <v>2899000</v>
@@ -19645,7 +19673,7 @@
         <v>82</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E189" s="2">
         <v>2379000</v>
@@ -19653,16 +19681,16 @@
     </row>
     <row r="190" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A190" s="1" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>1051</v>
+        <v>1053</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E190" s="2">
         <v>2499000</v>
@@ -19670,7 +19698,7 @@
     </row>
     <row r="191" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A191" s="1" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>473</v>
@@ -19679,7 +19707,7 @@
         <v>8</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E191" s="2">
         <v>2479900</v>
@@ -19696,7 +19724,7 @@
         <v>8</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E192" s="2">
         <v>3959000</v>
@@ -19707,13 +19735,13 @@
         <v>121</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E193" s="2">
         <v>2890000</v>
@@ -19724,13 +19752,13 @@
         <v>121</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E194" s="2">
         <v>4080000</v>
@@ -19741,13 +19769,13 @@
         <v>121</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E195" s="2">
         <v>6290000</v>
@@ -19755,7 +19783,7 @@
     </row>
     <row r="196" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A196" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="B196" s="2">
         <v>6</v>
@@ -19764,7 +19792,7 @@
         <v>8</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E196" s="2">
         <v>2200000</v>
@@ -19772,7 +19800,7 @@
     </row>
     <row r="197" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A197" s="1" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>284</v>
@@ -19781,7 +19809,7 @@
         <v>8</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E197" s="2">
         <v>4599000</v>
@@ -19798,7 +19826,7 @@
         <v>8</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E198" s="2">
         <v>2199000</v>
@@ -19809,13 +19837,13 @@
         <v>215</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E199" s="2">
         <v>4599000</v>
@@ -19826,13 +19854,13 @@
         <v>105</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E200" s="2">
         <v>1990000</v>
@@ -19843,13 +19871,13 @@
         <v>105</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E201" s="2">
         <v>3590000</v>
@@ -19866,7 +19894,7 @@
         <v>8</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E202" s="2">
         <v>2650000</v>
@@ -19877,13 +19905,13 @@
         <v>215</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E203" s="2">
         <v>2849000</v>
@@ -19891,7 +19919,7 @@
     </row>
     <row r="204" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A204" s="1" t="s">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>171</v>
@@ -19900,7 +19928,7 @@
         <v>8</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E204" s="2">
         <v>2099000</v>
@@ -19917,7 +19945,7 @@
         <v>8</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>1059</v>
+        <v>1061</v>
       </c>
       <c r="E205" s="2">
         <v>1263000</v>
@@ -19934,7 +19962,7 @@
         <v>8</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E206" s="2">
         <v>1546500</v>
@@ -19951,7 +19979,7 @@
         <v>8</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="E207" s="2">
         <v>883000</v>
@@ -19968,7 +19996,7 @@
         <v>8</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>1061</v>
+        <v>1063</v>
       </c>
       <c r="E208" s="2">
         <v>825000</v>
@@ -19985,7 +20013,7 @@
         <v>8</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="E209" s="2">
         <v>851000</v>
@@ -19996,13 +20024,13 @@
         <v>176</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E210" s="2">
         <v>3357990</v>
@@ -20013,13 +20041,13 @@
         <v>215</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E211" s="2">
         <v>3899000</v>
@@ -20036,7 +20064,7 @@
         <v>8</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E212" s="2">
         <v>1990000</v>
@@ -20053,7 +20081,7 @@
         <v>8</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E213" s="2">
         <v>2199000</v>
@@ -20070,7 +20098,7 @@
         <v>8</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="E214" s="2">
         <v>789900</v>
@@ -20087,7 +20115,7 @@
         <v>51</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="E215" s="2">
         <v>869900</v>
@@ -20104,7 +20132,7 @@
         <v>8</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="E216" s="2">
         <v>1089000</v>
@@ -20121,7 +20149,7 @@
         <v>8</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="E217" s="2">
         <v>999900</v>
@@ -20138,7 +20166,7 @@
         <v>8</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>1061</v>
+        <v>1063</v>
       </c>
       <c r="E218" s="2">
         <v>1455000</v>
@@ -20155,7 +20183,7 @@
         <v>103</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="E219" s="2">
         <v>809900</v>
@@ -20172,7 +20200,7 @@
         <v>8</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="E220" s="2">
         <v>2000000</v>
@@ -20189,7 +20217,7 @@
         <v>8</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="E221" s="2">
         <v>1229900</v>
@@ -20206,7 +20234,7 @@
         <v>8</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="E222" s="2">
         <v>2656800</v>
@@ -20217,13 +20245,13 @@
         <v>344</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>1066</v>
+        <v>1068</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="E223" s="2">
         <v>824000</v>
@@ -20234,13 +20262,13 @@
         <v>300</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="E224" s="2">
         <v>1204900</v>
@@ -20257,7 +20285,7 @@
         <v>8</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="E225" s="2">
         <v>2234900</v>
@@ -20265,7 +20293,7 @@
     </row>
     <row r="226" ht="40.35" customHeight="1" spans="1:5">
       <c r="A226" s="1" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>138</v>
@@ -20274,7 +20302,7 @@
         <v>5</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="E226" s="2">
         <v>2673000</v>
@@ -20291,7 +20319,7 @@
         <v>8</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="E227" s="2">
         <v>1419990</v>
@@ -20299,7 +20327,7 @@
     </row>
     <row r="228" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A228" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>277</v>
@@ -20308,7 +20336,7 @@
         <v>8</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="E228" s="2">
         <v>1494000</v>
@@ -20325,7 +20353,7 @@
         <v>8</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E229" s="2">
         <v>2849990</v>
@@ -20339,10 +20367,10 @@
         <v>591</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E230" s="2">
         <v>3173000</v>
@@ -20353,13 +20381,13 @@
         <v>54</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E231" s="2">
         <v>2380000</v>
@@ -20376,7 +20404,7 @@
         <v>8</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E232" s="2">
         <v>2599000</v>
@@ -20384,16 +20412,16 @@
     </row>
     <row r="233" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A233" s="1" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E233" s="2">
         <v>2999000</v>
@@ -20404,13 +20432,13 @@
         <v>22</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>1073</v>
+        <v>1075</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>312</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E234" s="2">
         <v>3590000</v>
@@ -20418,16 +20446,16 @@
     </row>
     <row r="235" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A235" s="1" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>1074</v>
+        <v>1076</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E235" s="2">
         <v>2569900</v>
@@ -20444,7 +20472,7 @@
         <v>8</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E236" s="2">
         <v>4750000</v>
@@ -20452,16 +20480,16 @@
     </row>
     <row r="237" ht="40.35" customHeight="1" spans="1:5">
       <c r="A237" s="1" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>1075</v>
+        <v>1077</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E237" s="2">
         <v>2499990</v>
@@ -20469,7 +20497,7 @@
     </row>
     <row r="238" ht="27.15" customHeight="1" spans="1:5">
       <c r="A238" s="1" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>793</v>
@@ -20478,7 +20506,7 @@
         <v>8</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E238" s="2">
         <v>2779990</v>
@@ -20495,7 +20523,7 @@
         <v>51</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E239" s="2">
         <v>2649000</v>
@@ -20512,7 +20540,7 @@
         <v>5</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E240" s="2">
         <v>1899000</v>
@@ -20529,7 +20557,7 @@
         <v>8</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E241" s="2">
         <v>2825990</v>
@@ -20537,7 +20565,7 @@
     </row>
     <row r="242" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A242" s="1" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="B242" s="2">
         <v>400</v>
@@ -20546,7 +20574,7 @@
         <v>8</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E242" s="2">
         <v>5799000</v>
@@ -20554,7 +20582,7 @@
     </row>
     <row r="243" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A243" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>280</v>
@@ -20563,7 +20591,7 @@
         <v>8</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="E243" s="2">
         <v>2899000</v>
@@ -20580,7 +20608,7 @@
         <v>8</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E244" s="2">
         <v>1887500</v>
@@ -20597,7 +20625,7 @@
         <v>8</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E245" s="2">
         <v>1805000</v>
@@ -20614,7 +20642,7 @@
         <v>8</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E246" s="2">
         <v>1684500</v>
@@ -20622,7 +20650,7 @@
     </row>
     <row r="247" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A247" s="1" t="s">
-        <v>1077</v>
+        <v>1079</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>785</v>
@@ -20631,7 +20659,7 @@
         <v>8</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E247" s="2">
         <v>3899000</v>
@@ -20639,7 +20667,7 @@
     </row>
     <row r="248" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A248" s="1" t="s">
-        <v>1077</v>
+        <v>1079</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>784</v>
@@ -20648,7 +20676,7 @@
         <v>8</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E248" s="2">
         <v>3099000</v>
@@ -20656,7 +20684,7 @@
     </row>
     <row r="249" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A249" s="1" t="s">
-        <v>1078</v>
+        <v>1080</v>
       </c>
       <c r="B249" s="2">
         <v>1</v>
@@ -20665,7 +20693,7 @@
         <v>8</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E249" s="2">
         <v>4162990</v>

</xml_diff>

<commit_message>
Add spb2, del astella from spb
</commit_message>
<xml_diff>
--- a/id.xlsx
+++ b/id.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$G$916</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$G$917</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Лист2!$A$1:$E$249</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3061" uniqueCount="1083">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3073" uniqueCount="1089">
   <si>
     <t>Aito</t>
   </si>
@@ -2948,6 +2948,24 @@
   </si>
   <si>
     <t>Tiggo 7L</t>
+  </si>
+  <si>
+    <t>Palasso</t>
+  </si>
+  <si>
+    <t>POER New</t>
+  </si>
+  <si>
+    <t>C5 4WD</t>
+  </si>
+  <si>
+    <t>Tiggo 7L 4WD</t>
+  </si>
+  <si>
+    <t>SF1</t>
+  </si>
+  <si>
+    <t>Monza</t>
   </si>
   <si>
     <t>Марка</t>
@@ -4271,10 +4289,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G917"/>
+  <dimension ref="A1:G923"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A898" workbookViewId="0">
-      <selection activeCell="C917" sqref="C917"/>
+      <selection activeCell="G919" sqref="G919"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -16485,8 +16503,74 @@
         <v>971</v>
       </c>
     </row>
+    <row r="918" spans="1:3">
+      <c r="A918">
+        <v>1017</v>
+      </c>
+      <c r="B918" t="s">
+        <v>484</v>
+      </c>
+      <c r="C918" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="919" spans="1:3">
+      <c r="A919">
+        <v>1018</v>
+      </c>
+      <c r="B919" t="s">
+        <v>200</v>
+      </c>
+      <c r="C919" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="920" spans="1:3">
+      <c r="A920">
+        <v>1019</v>
+      </c>
+      <c r="B920" t="s">
+        <v>471</v>
+      </c>
+      <c r="C920" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="921" spans="1:3">
+      <c r="A921">
+        <v>1020</v>
+      </c>
+      <c r="B921" t="s">
+        <v>54</v>
+      </c>
+      <c r="C921" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="922" spans="1:3">
+      <c r="A922">
+        <v>1021</v>
+      </c>
+      <c r="B922" t="s">
+        <v>697</v>
+      </c>
+      <c r="C922" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="923" spans="1:3">
+      <c r="A923">
+        <v>1022</v>
+      </c>
+      <c r="B923" t="s">
+        <v>78</v>
+      </c>
+      <c r="C923" t="s">
+        <v>977</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G916" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G917" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -16507,19 +16591,19 @@
   <sheetData>
     <row r="1" ht="27.15" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>972</v>
+        <v>978</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>973</v>
+        <v>979</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>974</v>
+        <v>980</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>975</v>
+        <v>981</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>976</v>
+        <v>982</v>
       </c>
     </row>
     <row r="2" ht="40.35" hidden="1" customHeight="1" spans="1:5">
@@ -16527,13 +16611,13 @@
         <v>344</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>977</v>
+        <v>983</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>380</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E2" s="2">
         <v>1239900</v>
@@ -16550,7 +16634,7 @@
         <v>380</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E3" s="2">
         <v>1759000</v>
@@ -16567,7 +16651,7 @@
         <v>380</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E4" s="2">
         <v>1655000</v>
@@ -16584,7 +16668,7 @@
         <v>380</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E5" s="2">
         <v>1879000</v>
@@ -16595,13 +16679,13 @@
         <v>344</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>979</v>
+        <v>985</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>980</v>
+        <v>986</v>
       </c>
       <c r="E6" s="2">
         <v>1077000</v>
@@ -16618,7 +16702,7 @@
         <v>82</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>981</v>
+        <v>987</v>
       </c>
       <c r="E7" s="2">
         <v>1408000</v>
@@ -16629,13 +16713,13 @@
         <v>344</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>982</v>
+        <v>988</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>980</v>
+        <v>986</v>
       </c>
       <c r="E8" s="2">
         <v>749900</v>
@@ -16652,7 +16736,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>980</v>
+        <v>986</v>
       </c>
       <c r="E9" s="2">
         <v>1175000</v>
@@ -16669,7 +16753,7 @@
         <v>252</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="E10" s="2">
         <v>2149000</v>
@@ -16686,7 +16770,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E11" s="2">
         <v>1660000</v>
@@ -16703,7 +16787,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E12" s="2">
         <v>2020000</v>
@@ -16720,7 +16804,7 @@
         <v>103</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>985</v>
+        <v>991</v>
       </c>
       <c r="E13" s="2">
         <v>1859000</v>
@@ -16737,7 +16821,7 @@
         <v>303</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E14" s="2">
         <v>1334900</v>
@@ -16748,13 +16832,13 @@
         <v>176</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>986</v>
+        <v>992</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E15" s="2">
         <v>3512990</v>
@@ -16771,7 +16855,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E16" s="2">
         <v>2836990</v>
@@ -16788,7 +16872,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>988</v>
+        <v>994</v>
       </c>
       <c r="E17" s="2">
         <v>1850000</v>
@@ -16805,7 +16889,7 @@
         <v>270</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="E18" s="2">
         <v>2749000</v>
@@ -16822,7 +16906,7 @@
         <v>103</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E19" s="2">
         <v>2179990</v>
@@ -16833,13 +16917,13 @@
         <v>176</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>990</v>
+        <v>996</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E20" s="2">
         <v>2794990</v>
@@ -16856,7 +16940,7 @@
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E21" s="2">
         <v>3959990</v>
@@ -16864,7 +16948,7 @@
     </row>
     <row r="22" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>991</v>
+        <v>997</v>
       </c>
       <c r="B22" s="2">
         <v>300</v>
@@ -16873,7 +16957,7 @@
         <v>8</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E22" s="2">
         <v>4499000</v>
@@ -16881,7 +16965,7 @@
     </row>
     <row r="23" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>991</v>
+        <v>997</v>
       </c>
       <c r="B23" s="2">
         <v>500</v>
@@ -16890,7 +16974,7 @@
         <v>8</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E23" s="2">
         <v>6799000</v>
@@ -16901,13 +16985,13 @@
         <v>344</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>992</v>
+        <v>998</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>980</v>
+        <v>986</v>
       </c>
       <c r="E24" s="2">
         <v>778500</v>
@@ -16918,13 +17002,13 @@
         <v>344</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>980</v>
+        <v>986</v>
       </c>
       <c r="E25" s="2">
         <v>719300</v>
@@ -16935,13 +17019,13 @@
         <v>344</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>994</v>
+        <v>1000</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>980</v>
+        <v>986</v>
       </c>
       <c r="E26" s="2">
         <v>950900</v>
@@ -16958,7 +17042,7 @@
         <v>380</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E27" s="2">
         <v>1316900</v>
@@ -16969,13 +17053,13 @@
         <v>242</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>995</v>
+        <v>1001</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>264</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E28" s="2">
         <v>2769000</v>
@@ -16992,7 +17076,7 @@
         <v>303</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E29" s="2">
         <v>2244900</v>
@@ -17009,7 +17093,7 @@
         <v>259</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>981</v>
+        <v>987</v>
       </c>
       <c r="E30" s="2">
         <v>1574900</v>
@@ -17026,7 +17110,7 @@
         <v>259</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>981</v>
+        <v>987</v>
       </c>
       <c r="E31" s="2">
         <v>1434900</v>
@@ -17037,13 +17121,13 @@
         <v>344</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>997</v>
+        <v>1003</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E32" s="2">
         <v>1059000</v>
@@ -17060,7 +17144,7 @@
         <v>259</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="E33" s="2">
         <v>3969000</v>
@@ -17077,7 +17161,7 @@
         <v>8</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>999</v>
+        <v>1005</v>
       </c>
       <c r="E34" s="2">
         <v>1314000</v>
@@ -17088,13 +17172,13 @@
         <v>215</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1000</v>
+        <v>1006</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E35" s="2">
         <v>2149000</v>
@@ -17111,7 +17195,7 @@
         <v>5</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>1002</v>
+        <v>1008</v>
       </c>
       <c r="E36" s="2">
         <v>2599000</v>
@@ -17122,13 +17206,13 @@
         <v>215</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1003</v>
+        <v>1009</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>1002</v>
+        <v>1008</v>
       </c>
       <c r="E37" s="2">
         <v>2599000</v>
@@ -17145,7 +17229,7 @@
         <v>8</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>1004</v>
+        <v>1010</v>
       </c>
       <c r="E38" s="2">
         <v>5269000</v>
@@ -17162,7 +17246,7 @@
         <v>303</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E39" s="2">
         <v>2314900</v>
@@ -17173,13 +17257,13 @@
         <v>344</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>1005</v>
+        <v>1011</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E40" s="2">
         <v>918900</v>
@@ -17196,7 +17280,7 @@
         <v>259</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E41" s="2">
         <v>2159900</v>
@@ -17213,7 +17297,7 @@
         <v>8</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>1006</v>
+        <v>1012</v>
       </c>
       <c r="E42" s="2">
         <v>1106900</v>
@@ -17230,7 +17314,7 @@
         <v>8</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>1006</v>
+        <v>1012</v>
       </c>
       <c r="E43" s="2">
         <v>1249900</v>
@@ -17247,7 +17331,7 @@
         <v>8</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E44" s="2">
         <v>2900000</v>
@@ -17258,13 +17342,13 @@
         <v>22</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E45" s="2">
         <v>2439900</v>
@@ -17281,7 +17365,7 @@
         <v>312</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E46" s="2">
         <v>2734900</v>
@@ -17298,7 +17382,7 @@
         <v>312</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E47" s="2">
         <v>1934900</v>
@@ -17315,7 +17399,7 @@
         <v>8</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E48" s="2">
         <v>2064900</v>
@@ -17332,7 +17416,7 @@
         <v>334</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E49" s="2">
         <v>2849900</v>
@@ -17340,7 +17424,7 @@
     </row>
     <row r="50" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A50" s="1" t="s">
-        <v>1009</v>
+        <v>1015</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>279</v>
@@ -17349,7 +17433,7 @@
         <v>8</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E50" s="2">
         <v>1779000</v>
@@ -17357,7 +17441,7 @@
     </row>
     <row r="51" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>1009</v>
+        <v>1015</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>273</v>
@@ -17366,7 +17450,7 @@
         <v>8</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E51" s="2">
         <v>2150000</v>
@@ -17374,7 +17458,7 @@
     </row>
     <row r="52" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A52" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>278</v>
@@ -17383,7 +17467,7 @@
         <v>8</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E52" s="2">
         <v>2129900</v>
@@ -17391,7 +17475,7 @@
     </row>
     <row r="53" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>472</v>
@@ -17400,7 +17484,7 @@
         <v>8</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E53" s="2">
         <v>2369900</v>
@@ -17417,7 +17501,7 @@
         <v>8</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E54" s="2">
         <v>1690000</v>
@@ -17434,7 +17518,7 @@
         <v>8</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E55" s="2">
         <v>2869900</v>
@@ -17445,13 +17529,13 @@
         <v>22</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1011</v>
+        <v>1017</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E56" s="2">
         <v>2569900</v>
@@ -17462,13 +17546,13 @@
         <v>22</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1012</v>
+        <v>1018</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E57" s="2">
         <v>2839900</v>
@@ -17485,7 +17569,7 @@
         <v>26</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E58" s="2">
         <v>3969900</v>
@@ -17502,7 +17586,7 @@
         <v>26</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E59" s="2">
         <v>3069900</v>
@@ -17519,7 +17603,7 @@
         <v>26</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E60" s="2">
         <v>3069900</v>
@@ -17530,13 +17614,13 @@
         <v>22</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>1013</v>
+        <v>1019</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>1014</v>
+        <v>1020</v>
       </c>
       <c r="E61" s="2">
         <v>2899900</v>
@@ -17544,7 +17628,7 @@
     </row>
     <row r="62" ht="40.35" customHeight="1" spans="1:5">
       <c r="A62" s="1" t="s">
-        <v>1015</v>
+        <v>1021</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>135</v>
@@ -17553,7 +17637,7 @@
         <v>26</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E62" s="2">
         <v>2374000</v>
@@ -17561,7 +17645,7 @@
     </row>
     <row r="63" ht="40.35" customHeight="1" spans="1:5">
       <c r="A63" s="1" t="s">
-        <v>1015</v>
+        <v>1021</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>136</v>
@@ -17570,7 +17654,7 @@
         <v>26</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E63" s="2">
         <v>2411000</v>
@@ -17578,7 +17662,7 @@
     </row>
     <row r="64" ht="40.35" customHeight="1" spans="1:5">
       <c r="A64" s="1" t="s">
-        <v>1015</v>
+        <v>1021</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>137</v>
@@ -17587,7 +17671,7 @@
         <v>26</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>980</v>
+        <v>986</v>
       </c>
       <c r="E64" s="2">
         <v>2024000</v>
@@ -17604,7 +17688,7 @@
         <v>82</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>1004</v>
+        <v>1010</v>
       </c>
       <c r="E65" s="2">
         <v>1124000</v>
@@ -17621,7 +17705,7 @@
         <v>103</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E66" s="2">
         <v>1051000</v>
@@ -17638,7 +17722,7 @@
         <v>534</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E67" s="2">
         <v>1657000</v>
@@ -17655,7 +17739,7 @@
         <v>5</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E68" s="2">
         <v>1705000</v>
@@ -17672,7 +17756,7 @@
         <v>5</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1016</v>
+        <v>1022</v>
       </c>
       <c r="E69" s="2">
         <v>1699900</v>
@@ -17689,7 +17773,7 @@
         <v>26</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E70" s="2">
         <v>2489900</v>
@@ -17697,7 +17781,7 @@
     </row>
     <row r="71" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A71" s="1" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>273</v>
@@ -17706,7 +17790,7 @@
         <v>26</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E71" s="2">
         <v>2959900</v>
@@ -17714,7 +17798,7 @@
     </row>
     <row r="72" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A72" s="1" t="s">
-        <v>1018</v>
+        <v>1024</v>
       </c>
       <c r="B72" s="2">
         <v>3</v>
@@ -17723,7 +17807,7 @@
         <v>26</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E72" s="2">
         <v>1765000</v>
@@ -17740,7 +17824,7 @@
         <v>226</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1019</v>
+        <v>1025</v>
       </c>
       <c r="E73" s="2">
         <v>4409000</v>
@@ -17757,7 +17841,7 @@
         <v>226</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>1019</v>
+        <v>1025</v>
       </c>
       <c r="E74" s="2">
         <v>1690000</v>
@@ -17774,7 +17858,7 @@
         <v>85</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E75" s="2">
         <v>950900</v>
@@ -17791,7 +17875,7 @@
         <v>8</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>999</v>
+        <v>1005</v>
       </c>
       <c r="E76" s="2">
         <v>880900</v>
@@ -17808,7 +17892,7 @@
         <v>82</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E77" s="2">
         <v>953900</v>
@@ -17825,7 +17909,7 @@
         <v>103</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E78" s="2">
         <v>2179000</v>
@@ -17842,7 +17926,7 @@
         <v>8</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>1020</v>
+        <v>1026</v>
       </c>
       <c r="E79" s="2">
         <v>1579000</v>
@@ -17859,7 +17943,7 @@
         <v>5</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>999</v>
+        <v>1005</v>
       </c>
       <c r="E80" s="2">
         <v>4299000</v>
@@ -17876,7 +17960,7 @@
         <v>8</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>1021</v>
+        <v>1027</v>
       </c>
       <c r="E81" s="2">
         <v>2049000</v>
@@ -17893,7 +17977,7 @@
         <v>8</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E82" s="2">
         <v>3149000</v>
@@ -17910,7 +17994,7 @@
         <v>82</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>1022</v>
+        <v>1028</v>
       </c>
       <c r="E83" s="2">
         <v>2337000</v>
@@ -17921,13 +18005,13 @@
         <v>457</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>1023</v>
+        <v>1029</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>303</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>1022</v>
+        <v>1028</v>
       </c>
       <c r="E84" s="2">
         <v>2762000</v>
@@ -17944,7 +18028,7 @@
         <v>103</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E85" s="2">
         <v>1618000</v>
@@ -17961,7 +18045,7 @@
         <v>82</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>1004</v>
+        <v>1010</v>
       </c>
       <c r="E86" s="2">
         <v>1301000</v>
@@ -17978,7 +18062,7 @@
         <v>82</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>1004</v>
+        <v>1010</v>
       </c>
       <c r="E87" s="2">
         <v>1258000</v>
@@ -17995,7 +18079,7 @@
         <v>82</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>1004</v>
+        <v>1010</v>
       </c>
       <c r="E88" s="2">
         <v>1373000</v>
@@ -18012,7 +18096,7 @@
         <v>5</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>981</v>
+        <v>987</v>
       </c>
       <c r="E89" s="2">
         <v>1724000</v>
@@ -18029,7 +18113,7 @@
         <v>8</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E90" s="2">
         <v>1874000</v>
@@ -18046,7 +18130,7 @@
         <v>5</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E91" s="2">
         <v>2057000</v>
@@ -18063,7 +18147,7 @@
         <v>5</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E92" s="2">
         <v>2118900</v>
@@ -18080,7 +18164,7 @@
         <v>5</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E93" s="2">
         <v>3248000</v>
@@ -18097,7 +18181,7 @@
         <v>5</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E94" s="2">
         <v>5378000</v>
@@ -18114,7 +18198,7 @@
         <v>5</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E95" s="2">
         <v>5806000</v>
@@ -18131,7 +18215,7 @@
         <v>303</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E96" s="2">
         <v>2388000</v>
@@ -18148,7 +18232,7 @@
         <v>303</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E97" s="2">
         <v>2681000</v>
@@ -18165,7 +18249,7 @@
         <v>617</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>981</v>
+        <v>987</v>
       </c>
       <c r="E98" s="2">
         <v>1385900</v>
@@ -18182,7 +18266,7 @@
         <v>608</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>1024</v>
+        <v>1030</v>
       </c>
       <c r="E99" s="2">
         <v>1518000</v>
@@ -18199,7 +18283,7 @@
         <v>82</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E100" s="2">
         <v>3375900</v>
@@ -18216,7 +18300,7 @@
         <v>8</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E101" s="2">
         <v>2828900</v>
@@ -18233,7 +18317,7 @@
         <v>5</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E102" s="2">
         <v>4449900</v>
@@ -18250,7 +18334,7 @@
         <v>8</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>1025</v>
+        <v>1031</v>
       </c>
       <c r="E103" s="2">
         <v>1229000</v>
@@ -18267,7 +18351,7 @@
         <v>103</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E104" s="2">
         <v>2499000</v>
@@ -18275,7 +18359,7 @@
     </row>
     <row r="105" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A105" s="1" t="s">
-        <v>1026</v>
+        <v>1032</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>595</v>
@@ -18284,7 +18368,7 @@
         <v>596</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>1027</v>
+        <v>1033</v>
       </c>
       <c r="E105" s="2">
         <v>1680000</v>
@@ -18292,16 +18376,16 @@
     </row>
     <row r="106" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A106" s="1" t="s">
-        <v>1026</v>
+        <v>1032</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>1028</v>
+        <v>1034</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>596</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>1027</v>
+        <v>1033</v>
       </c>
       <c r="E106" s="2">
         <v>1705000</v>
@@ -18309,7 +18393,7 @@
     </row>
     <row r="107" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A107" s="1" t="s">
-        <v>1026</v>
+        <v>1032</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>39</v>
@@ -18318,7 +18402,7 @@
         <v>8</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>1029</v>
+        <v>1035</v>
       </c>
       <c r="E107" s="2">
         <v>1510000</v>
@@ -18335,7 +18419,7 @@
         <v>8</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E108" s="2">
         <v>2570000</v>
@@ -18352,7 +18436,7 @@
         <v>8</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E109" s="2">
         <v>3430000</v>
@@ -18363,13 +18447,13 @@
         <v>54</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>1030</v>
+        <v>1036</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E110" s="2">
         <v>2770000</v>
@@ -18386,7 +18470,7 @@
         <v>5</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E111" s="2">
         <v>1970000</v>
@@ -18397,13 +18481,13 @@
         <v>54</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>1031</v>
+        <v>1037</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E112" s="2">
         <v>3250000</v>
@@ -18414,13 +18498,13 @@
         <v>54</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>1032</v>
+        <v>1038</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E113" s="2">
         <v>3370000</v>
@@ -18437,7 +18521,7 @@
         <v>8</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E114" s="2">
         <v>3759900</v>
@@ -18454,7 +18538,7 @@
         <v>5</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E115" s="2">
         <v>3380000</v>
@@ -18471,7 +18555,7 @@
         <v>5</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E116" s="2">
         <v>3810000</v>
@@ -18488,7 +18572,7 @@
         <v>8</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E117" s="2">
         <v>4910000</v>
@@ -18505,7 +18589,7 @@
         <v>8</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E118" s="2">
         <v>4550000</v>
@@ -18522,7 +18606,7 @@
         <v>8</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E119" s="2">
         <v>2080000</v>
@@ -18539,7 +18623,7 @@
         <v>8</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E120" s="2">
         <v>2225000</v>
@@ -18556,7 +18640,7 @@
         <v>8</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E121" s="2">
         <v>2970000</v>
@@ -18573,7 +18657,7 @@
         <v>5</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E122" s="2">
         <v>4350000</v>
@@ -18590,7 +18674,7 @@
         <v>5</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E123" s="2">
         <v>2999900</v>
@@ -18607,7 +18691,7 @@
         <v>8</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E124" s="2">
         <v>3479900</v>
@@ -18624,7 +18708,7 @@
         <v>5</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E125" s="2">
         <v>1990000</v>
@@ -18641,7 +18725,7 @@
         <v>5</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E126" s="2">
         <v>2149000</v>
@@ -18658,7 +18742,7 @@
         <v>8</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E127" s="2">
         <v>2115000</v>
@@ -18675,7 +18759,7 @@
         <v>8</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E128" s="2">
         <v>2238000</v>
@@ -18692,7 +18776,7 @@
         <v>8</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E129" s="2">
         <v>2514900</v>
@@ -18709,7 +18793,7 @@
         <v>8</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E130" s="2">
         <v>2997900</v>
@@ -18717,16 +18801,16 @@
     </row>
     <row r="131" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A131" s="1" t="s">
-        <v>1033</v>
+        <v>1039</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>1034</v>
+        <v>1040</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E131" s="2">
         <v>2549900</v>
@@ -18734,16 +18818,16 @@
     </row>
     <row r="132" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A132" s="1" t="s">
-        <v>1033</v>
+        <v>1039</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>1035</v>
+        <v>1041</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E132" s="2">
         <v>2629900</v>
@@ -18751,16 +18835,16 @@
     </row>
     <row r="133" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A133" s="1" t="s">
-        <v>1018</v>
+        <v>1024</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>1036</v>
+        <v>1042</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E133" s="2">
         <v>4100000</v>
@@ -18777,7 +18861,7 @@
         <v>8</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>1022</v>
+        <v>1028</v>
       </c>
       <c r="E134" s="2">
         <v>2219900</v>
@@ -18788,13 +18872,13 @@
         <v>22</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>1037</v>
+        <v>1043</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>980</v>
+        <v>986</v>
       </c>
       <c r="E135" s="2">
         <v>2499900</v>
@@ -18802,7 +18886,7 @@
     </row>
     <row r="136" ht="27.15" customHeight="1" spans="1:5">
       <c r="A136" s="1" t="s">
-        <v>1015</v>
+        <v>1021</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>145</v>
@@ -18811,7 +18895,7 @@
         <v>8</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>1038</v>
+        <v>1044</v>
       </c>
       <c r="E136" s="2">
         <v>1602000</v>
@@ -18819,7 +18903,7 @@
     </row>
     <row r="137" ht="40.35" customHeight="1" spans="1:5">
       <c r="A137" s="1" t="s">
-        <v>1015</v>
+        <v>1021</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>146</v>
@@ -18828,7 +18912,7 @@
         <v>5</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>1004</v>
+        <v>1010</v>
       </c>
       <c r="E137" s="2">
         <v>1508000</v>
@@ -18845,7 +18929,7 @@
         <v>8</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E138" s="2">
         <v>4549990</v>
@@ -18862,7 +18946,7 @@
         <v>8</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E139" s="2">
         <v>2479990</v>
@@ -18879,7 +18963,7 @@
         <v>8</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>1039</v>
+        <v>1045</v>
       </c>
       <c r="E140" s="2">
         <v>2075990</v>
@@ -18896,7 +18980,7 @@
         <v>8</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E141" s="2">
         <v>2080990</v>
@@ -18913,7 +18997,7 @@
         <v>380</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E142" s="2">
         <v>2273000</v>
@@ -18930,7 +19014,7 @@
         <v>380</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E143" s="2">
         <v>2443000</v>
@@ -18947,7 +19031,7 @@
         <v>5</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>980</v>
+        <v>986</v>
       </c>
       <c r="E144" s="2">
         <v>1341000</v>
@@ -18958,13 +19042,13 @@
         <v>344</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>980</v>
+        <v>986</v>
       </c>
       <c r="E145" s="2">
         <v>1381000</v>
@@ -18975,13 +19059,13 @@
         <v>344</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>1041</v>
+        <v>1047</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>980</v>
+        <v>986</v>
       </c>
       <c r="E146" s="2">
         <v>1493000</v>
@@ -18992,13 +19076,13 @@
         <v>344</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>1042</v>
+        <v>1048</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>980</v>
+        <v>986</v>
       </c>
       <c r="E147" s="2">
         <v>1533000</v>
@@ -19015,7 +19099,7 @@
         <v>5</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E148" s="2">
         <v>1670000</v>
@@ -19032,7 +19116,7 @@
         <v>8</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E149" s="2">
         <v>1487000</v>
@@ -19043,13 +19127,13 @@
         <v>54</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>1043</v>
+        <v>1049</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E150" s="2">
         <v>4850000</v>
@@ -19060,13 +19144,13 @@
         <v>54</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>1044</v>
+        <v>1050</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E151" s="2">
         <v>4000000</v>
@@ -19077,13 +19161,13 @@
         <v>54</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>1045</v>
+        <v>1051</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E152" s="2">
         <v>4930000</v>
@@ -19100,7 +19184,7 @@
         <v>5</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E153" s="2">
         <v>3692990</v>
@@ -19117,7 +19201,7 @@
         <v>270</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="E154" s="2">
         <v>3979000</v>
@@ -19134,7 +19218,7 @@
         <v>8</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E155" s="2">
         <v>4099000</v>
@@ -19151,7 +19235,7 @@
         <v>8</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E156" s="2">
         <v>3449000</v>
@@ -19168,7 +19252,7 @@
         <v>8</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E157" s="2">
         <v>2799000</v>
@@ -19179,13 +19263,13 @@
         <v>200</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>1046</v>
+        <v>1052</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E158" s="2">
         <v>3549000</v>
@@ -19196,13 +19280,13 @@
         <v>200</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>1047</v>
+        <v>1053</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E159" s="2">
         <v>3299000</v>
@@ -19219,7 +19303,7 @@
         <v>330</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E160" s="2">
         <v>7374900</v>
@@ -19236,7 +19320,7 @@
         <v>270</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E161" s="2">
         <v>3789900</v>
@@ -19253,7 +19337,7 @@
         <v>51</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E162" s="2">
         <v>5829900</v>
@@ -19270,7 +19354,7 @@
         <v>270</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E163" s="2">
         <v>4144900</v>
@@ -19278,16 +19362,16 @@
     </row>
     <row r="164" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A164" s="1" t="s">
-        <v>1033</v>
+        <v>1039</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>1048</v>
+        <v>1054</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E164" s="2">
         <v>1672000</v>
@@ -19304,7 +19388,7 @@
         <v>8</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E165" s="2">
         <v>2040546</v>
@@ -19321,7 +19405,7 @@
         <v>8</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E166" s="2">
         <v>3100000</v>
@@ -19338,7 +19422,7 @@
         <v>8</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E167" s="2">
         <v>2990000</v>
@@ -19355,7 +19439,7 @@
         <v>312</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>1016</v>
+        <v>1022</v>
       </c>
       <c r="E168" s="2">
         <v>8669500</v>
@@ -19372,7 +19456,7 @@
         <v>677</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E169" s="2">
         <v>4291000</v>
@@ -19389,7 +19473,7 @@
         <v>5</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E170" s="2">
         <v>6146500</v>
@@ -19397,7 +19481,7 @@
     </row>
     <row r="171" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A171" s="1" t="s">
-        <v>1009</v>
+        <v>1015</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>274</v>
@@ -19406,7 +19490,7 @@
         <v>8</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E171" s="2">
         <v>1889000</v>
@@ -19414,7 +19498,7 @@
     </row>
     <row r="172" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A172" s="1" t="s">
-        <v>1009</v>
+        <v>1015</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>276</v>
@@ -19423,7 +19507,7 @@
         <v>8</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E172" s="2">
         <v>2399000</v>
@@ -19431,7 +19515,7 @@
     </row>
     <row r="173" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A173" s="1" t="s">
-        <v>1009</v>
+        <v>1015</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>653</v>
@@ -19440,7 +19524,7 @@
         <v>8</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E173" s="2">
         <v>3059000</v>
@@ -19448,16 +19532,16 @@
     </row>
     <row r="174" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A174" s="1" t="s">
-        <v>1009</v>
+        <v>1015</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>1049</v>
+        <v>1055</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E174" s="2">
         <v>3279000</v>
@@ -19465,7 +19549,7 @@
     </row>
     <row r="175" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A175" s="1" t="s">
-        <v>1009</v>
+        <v>1015</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>654</v>
@@ -19474,7 +19558,7 @@
         <v>8</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E175" s="2">
         <v>3599000</v>
@@ -19482,7 +19566,7 @@
     </row>
     <row r="176" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A176" s="1" t="s">
-        <v>1050</v>
+        <v>1056</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>175</v>
@@ -19491,7 +19575,7 @@
         <v>8</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E176" s="2">
         <v>5499999</v>
@@ -19499,7 +19583,7 @@
     </row>
     <row r="177" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A177" s="1" t="s">
-        <v>1050</v>
+        <v>1056</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>172</v>
@@ -19508,7 +19592,7 @@
         <v>103</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E177" s="2">
         <v>4099000</v>
@@ -19516,7 +19600,7 @@
     </row>
     <row r="178" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A178" s="1" t="s">
-        <v>1050</v>
+        <v>1056</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>169</v>
@@ -19525,7 +19609,7 @@
         <v>8</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E178" s="2">
         <v>2449000</v>
@@ -19536,13 +19620,13 @@
         <v>22</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>1051</v>
+        <v>1057</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E179" s="2">
         <v>4529900</v>
@@ -19559,7 +19643,7 @@
         <v>8</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E180" s="2">
         <v>3739900</v>
@@ -19570,13 +19654,13 @@
         <v>22</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>1052</v>
+        <v>1058</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E181" s="2">
         <v>5219900</v>
@@ -19587,13 +19671,13 @@
         <v>54</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>1053</v>
+        <v>1059</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E182" s="2">
         <v>2780000</v>
@@ -19610,7 +19694,7 @@
         <v>8</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E183" s="2">
         <v>2020000</v>
@@ -19627,7 +19711,7 @@
         <v>8</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E184" s="2">
         <v>2650000</v>
@@ -19644,7 +19728,7 @@
         <v>8</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E185" s="2">
         <v>2080000</v>
@@ -19661,7 +19745,7 @@
         <v>8</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E186" s="2">
         <v>2181000</v>
@@ -19678,7 +19762,7 @@
         <v>5</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>999</v>
+        <v>1005</v>
       </c>
       <c r="E187" s="2">
         <v>2279000</v>
@@ -19695,7 +19779,7 @@
         <v>103</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>999</v>
+        <v>1005</v>
       </c>
       <c r="E188" s="2">
         <v>2899000</v>
@@ -19712,7 +19796,7 @@
         <v>82</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E189" s="2">
         <v>2379000</v>
@@ -19720,16 +19804,16 @@
     </row>
     <row r="190" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A190" s="1" t="s">
-        <v>1054</v>
+        <v>1060</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>1055</v>
+        <v>1061</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E190" s="2">
         <v>2499000</v>
@@ -19737,7 +19821,7 @@
     </row>
     <row r="191" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A191" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>473</v>
@@ -19746,7 +19830,7 @@
         <v>8</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E191" s="2">
         <v>2479900</v>
@@ -19763,7 +19847,7 @@
         <v>8</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E192" s="2">
         <v>3959000</v>
@@ -19774,13 +19858,13 @@
         <v>121</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>1056</v>
+        <v>1062</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E193" s="2">
         <v>2890000</v>
@@ -19791,13 +19875,13 @@
         <v>121</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>1057</v>
+        <v>1063</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E194" s="2">
         <v>4080000</v>
@@ -19808,13 +19892,13 @@
         <v>121</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>1058</v>
+        <v>1064</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E195" s="2">
         <v>6290000</v>
@@ -19822,7 +19906,7 @@
     </row>
     <row r="196" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A196" s="1" t="s">
-        <v>1018</v>
+        <v>1024</v>
       </c>
       <c r="B196" s="2">
         <v>6</v>
@@ -19831,7 +19915,7 @@
         <v>8</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E196" s="2">
         <v>2200000</v>
@@ -19839,7 +19923,7 @@
     </row>
     <row r="197" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A197" s="1" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>284</v>
@@ -19848,7 +19932,7 @@
         <v>8</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E197" s="2">
         <v>4599000</v>
@@ -19865,7 +19949,7 @@
         <v>8</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E198" s="2">
         <v>2199000</v>
@@ -19876,13 +19960,13 @@
         <v>215</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>1059</v>
+        <v>1065</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E199" s="2">
         <v>4599000</v>
@@ -19893,13 +19977,13 @@
         <v>105</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>1060</v>
+        <v>1066</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E200" s="2">
         <v>1990000</v>
@@ -19910,13 +19994,13 @@
         <v>105</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>1061</v>
+        <v>1067</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E201" s="2">
         <v>3590000</v>
@@ -19933,7 +20017,7 @@
         <v>8</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E202" s="2">
         <v>2650000</v>
@@ -19944,13 +20028,13 @@
         <v>215</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>1062</v>
+        <v>1068</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E203" s="2">
         <v>2849000</v>
@@ -19958,7 +20042,7 @@
     </row>
     <row r="204" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A204" s="1" t="s">
-        <v>1050</v>
+        <v>1056</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>171</v>
@@ -19967,7 +20051,7 @@
         <v>8</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E204" s="2">
         <v>2099000</v>
@@ -19984,7 +20068,7 @@
         <v>8</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>1063</v>
+        <v>1069</v>
       </c>
       <c r="E205" s="2">
         <v>1263000</v>
@@ -20001,7 +20085,7 @@
         <v>8</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>980</v>
+        <v>986</v>
       </c>
       <c r="E206" s="2">
         <v>1546500</v>
@@ -20018,7 +20102,7 @@
         <v>8</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>1064</v>
+        <v>1070</v>
       </c>
       <c r="E207" s="2">
         <v>883000</v>
@@ -20035,7 +20119,7 @@
         <v>8</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>1065</v>
+        <v>1071</v>
       </c>
       <c r="E208" s="2">
         <v>825000</v>
@@ -20052,7 +20136,7 @@
         <v>8</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>1064</v>
+        <v>1070</v>
       </c>
       <c r="E209" s="2">
         <v>851000</v>
@@ -20063,13 +20147,13 @@
         <v>176</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>1066</v>
+        <v>1072</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E210" s="2">
         <v>3357990</v>
@@ -20080,13 +20164,13 @@
         <v>215</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>1067</v>
+        <v>1073</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E211" s="2">
         <v>3899000</v>
@@ -20103,7 +20187,7 @@
         <v>8</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E212" s="2">
         <v>1990000</v>
@@ -20120,7 +20204,7 @@
         <v>8</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E213" s="2">
         <v>2199000</v>
@@ -20137,7 +20221,7 @@
         <v>8</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>1025</v>
+        <v>1031</v>
       </c>
       <c r="E214" s="2">
         <v>789900</v>
@@ -20154,7 +20238,7 @@
         <v>51</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>1068</v>
+        <v>1074</v>
       </c>
       <c r="E215" s="2">
         <v>869900</v>
@@ -20171,7 +20255,7 @@
         <v>8</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>1069</v>
+        <v>1075</v>
       </c>
       <c r="E216" s="2">
         <v>1089000</v>
@@ -20188,7 +20272,7 @@
         <v>8</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>1064</v>
+        <v>1070</v>
       </c>
       <c r="E217" s="2">
         <v>999900</v>
@@ -20205,7 +20289,7 @@
         <v>8</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>1065</v>
+        <v>1071</v>
       </c>
       <c r="E218" s="2">
         <v>1455000</v>
@@ -20222,7 +20306,7 @@
         <v>103</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>1068</v>
+        <v>1074</v>
       </c>
       <c r="E219" s="2">
         <v>809900</v>
@@ -20239,7 +20323,7 @@
         <v>8</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="E220" s="2">
         <v>2000000</v>
@@ -20256,7 +20340,7 @@
         <v>8</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>1064</v>
+        <v>1070</v>
       </c>
       <c r="E221" s="2">
         <v>1229900</v>
@@ -20273,7 +20357,7 @@
         <v>8</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>1004</v>
+        <v>1010</v>
       </c>
       <c r="E222" s="2">
         <v>2656800</v>
@@ -20284,13 +20368,13 @@
         <v>344</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>1070</v>
+        <v>1076</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>1020</v>
+        <v>1026</v>
       </c>
       <c r="E223" s="2">
         <v>824000</v>
@@ -20301,13 +20385,13 @@
         <v>300</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>1071</v>
+        <v>1077</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>1024</v>
+        <v>1030</v>
       </c>
       <c r="E224" s="2">
         <v>1204900</v>
@@ -20324,7 +20408,7 @@
         <v>8</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E225" s="2">
         <v>2234900</v>
@@ -20332,7 +20416,7 @@
     </row>
     <row r="226" ht="40.35" customHeight="1" spans="1:5">
       <c r="A226" s="1" t="s">
-        <v>1015</v>
+        <v>1021</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>138</v>
@@ -20341,7 +20425,7 @@
         <v>5</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>1002</v>
+        <v>1008</v>
       </c>
       <c r="E226" s="2">
         <v>2673000</v>
@@ -20358,7 +20442,7 @@
         <v>8</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>1072</v>
+        <v>1078</v>
       </c>
       <c r="E227" s="2">
         <v>1419990</v>
@@ -20366,7 +20450,7 @@
     </row>
     <row r="228" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A228" s="1" t="s">
-        <v>1009</v>
+        <v>1015</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>277</v>
@@ -20375,7 +20459,7 @@
         <v>8</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>1073</v>
+        <v>1079</v>
       </c>
       <c r="E228" s="2">
         <v>1494000</v>
@@ -20392,7 +20476,7 @@
         <v>8</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E229" s="2">
         <v>2849990</v>
@@ -20406,10 +20490,10 @@
         <v>591</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>1074</v>
+        <v>1080</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E230" s="2">
         <v>3173000</v>
@@ -20420,13 +20504,13 @@
         <v>54</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>1075</v>
+        <v>1081</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E231" s="2">
         <v>2380000</v>
@@ -20443,7 +20527,7 @@
         <v>8</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E232" s="2">
         <v>2599000</v>
@@ -20451,16 +20535,16 @@
     </row>
     <row r="233" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A233" s="1" t="s">
-        <v>1054</v>
+        <v>1060</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>1076</v>
+        <v>1082</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E233" s="2">
         <v>2999000</v>
@@ -20471,13 +20555,13 @@
         <v>22</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>1077</v>
+        <v>1083</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>312</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E234" s="2">
         <v>3590000</v>
@@ -20485,16 +20569,16 @@
     </row>
     <row r="235" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A235" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>1078</v>
+        <v>1084</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E235" s="2">
         <v>2569900</v>
@@ -20511,7 +20595,7 @@
         <v>8</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E236" s="2">
         <v>4750000</v>
@@ -20519,16 +20603,16 @@
     </row>
     <row r="237" ht="40.35" customHeight="1" spans="1:5">
       <c r="A237" s="1" t="s">
-        <v>1015</v>
+        <v>1021</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>1079</v>
+        <v>1085</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E237" s="2">
         <v>2499990</v>
@@ -20536,7 +20620,7 @@
     </row>
     <row r="238" ht="27.15" customHeight="1" spans="1:5">
       <c r="A238" s="1" t="s">
-        <v>1015</v>
+        <v>1021</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>793</v>
@@ -20545,7 +20629,7 @@
         <v>8</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E238" s="2">
         <v>2779990</v>
@@ -20562,7 +20646,7 @@
         <v>51</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E239" s="2">
         <v>2649000</v>
@@ -20579,7 +20663,7 @@
         <v>5</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>980</v>
+        <v>986</v>
       </c>
       <c r="E240" s="2">
         <v>1899000</v>
@@ -20596,7 +20680,7 @@
         <v>8</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E241" s="2">
         <v>2825990</v>
@@ -20604,7 +20688,7 @@
     </row>
     <row r="242" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A242" s="1" t="s">
-        <v>991</v>
+        <v>997</v>
       </c>
       <c r="B242" s="2">
         <v>400</v>
@@ -20613,7 +20697,7 @@
         <v>8</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E242" s="2">
         <v>5799000</v>
@@ -20621,7 +20705,7 @@
     </row>
     <row r="243" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A243" s="1" t="s">
-        <v>1009</v>
+        <v>1015</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>280</v>
@@ -20630,7 +20714,7 @@
         <v>8</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>1080</v>
+        <v>1086</v>
       </c>
       <c r="E243" s="2">
         <v>2899000</v>
@@ -20647,7 +20731,7 @@
         <v>8</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>980</v>
+        <v>986</v>
       </c>
       <c r="E244" s="2">
         <v>1887500</v>
@@ -20664,7 +20748,7 @@
         <v>8</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>980</v>
+        <v>986</v>
       </c>
       <c r="E245" s="2">
         <v>1805000</v>
@@ -20681,7 +20765,7 @@
         <v>8</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E246" s="2">
         <v>1684500</v>
@@ -20689,7 +20773,7 @@
     </row>
     <row r="247" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A247" s="1" t="s">
-        <v>1081</v>
+        <v>1087</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>785</v>
@@ -20698,7 +20782,7 @@
         <v>8</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E247" s="2">
         <v>3899000</v>
@@ -20706,7 +20790,7 @@
     </row>
     <row r="248" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A248" s="1" t="s">
-        <v>1081</v>
+        <v>1087</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>784</v>
@@ -20715,7 +20799,7 @@
         <v>8</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E248" s="2">
         <v>3099000</v>
@@ -20723,7 +20807,7 @@
     </row>
     <row r="249" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A249" s="1" t="s">
-        <v>1082</v>
+        <v>1088</v>
       </c>
       <c r="B249" s="2">
         <v>1</v>
@@ -20732,7 +20816,7 @@
         <v>8</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="E249" s="2">
         <v>4162990</v>

</xml_diff>

<commit_message>
Del 6 sites samara msk, surgut
</commit_message>
<xml_diff>
--- a/id.xlsx
+++ b/id.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$G$917</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$G$923</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Лист2!$A$1:$E$249</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3073" uniqueCount="1089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3077" uniqueCount="1091">
   <si>
     <t>Aito</t>
   </si>
@@ -2966,6 +2966,12 @@
   </si>
   <si>
     <t>Monza</t>
+  </si>
+  <si>
+    <t>C7 4WD</t>
+  </si>
+  <si>
+    <t>C7</t>
   </si>
   <si>
     <t>Марка</t>
@@ -4289,10 +4295,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G923"/>
+  <dimension ref="A1:G925"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A898" workbookViewId="0">
-      <selection activeCell="G919" sqref="G919"/>
+    <sheetView tabSelected="1" topLeftCell="A905" workbookViewId="0">
+      <selection activeCell="F920" sqref="F920"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -16569,8 +16575,30 @@
         <v>977</v>
       </c>
     </row>
+    <row r="924" spans="1:3">
+      <c r="A924">
+        <v>1023</v>
+      </c>
+      <c r="B924" t="s">
+        <v>471</v>
+      </c>
+      <c r="C924" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="925" spans="1:3">
+      <c r="A925">
+        <v>1024</v>
+      </c>
+      <c r="B925" t="s">
+        <v>471</v>
+      </c>
+      <c r="C925" t="s">
+        <v>979</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G917" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G923" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -16591,19 +16619,19 @@
   <sheetData>
     <row r="1" ht="27.15" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="2" ht="40.35" hidden="1" customHeight="1" spans="1:5">
@@ -16611,13 +16639,13 @@
         <v>344</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>380</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E2" s="2">
         <v>1239900</v>
@@ -16634,7 +16662,7 @@
         <v>380</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E3" s="2">
         <v>1759000</v>
@@ -16651,7 +16679,7 @@
         <v>380</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E4" s="2">
         <v>1655000</v>
@@ -16668,7 +16696,7 @@
         <v>380</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E5" s="2">
         <v>1879000</v>
@@ -16679,13 +16707,13 @@
         <v>344</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E6" s="2">
         <v>1077000</v>
@@ -16702,7 +16730,7 @@
         <v>82</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="E7" s="2">
         <v>1408000</v>
@@ -16713,13 +16741,13 @@
         <v>344</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E8" s="2">
         <v>749900</v>
@@ -16736,7 +16764,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E9" s="2">
         <v>1175000</v>
@@ -16753,7 +16781,7 @@
         <v>252</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="E10" s="2">
         <v>2149000</v>
@@ -16770,7 +16798,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E11" s="2">
         <v>1660000</v>
@@ -16787,7 +16815,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E12" s="2">
         <v>2020000</v>
@@ -16804,7 +16832,7 @@
         <v>103</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="E13" s="2">
         <v>1859000</v>
@@ -16821,7 +16849,7 @@
         <v>303</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E14" s="2">
         <v>1334900</v>
@@ -16832,13 +16860,13 @@
         <v>176</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E15" s="2">
         <v>3512990</v>
@@ -16855,7 +16883,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E16" s="2">
         <v>2836990</v>
@@ -16872,7 +16900,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E17" s="2">
         <v>1850000</v>
@@ -16889,7 +16917,7 @@
         <v>270</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="E18" s="2">
         <v>2749000</v>
@@ -16906,7 +16934,7 @@
         <v>103</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E19" s="2">
         <v>2179990</v>
@@ -16917,13 +16945,13 @@
         <v>176</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E20" s="2">
         <v>2794990</v>
@@ -16940,7 +16968,7 @@
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E21" s="2">
         <v>3959990</v>
@@ -16948,7 +16976,7 @@
     </row>
     <row r="22" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="B22" s="2">
         <v>300</v>
@@ -16957,7 +16985,7 @@
         <v>8</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E22" s="2">
         <v>4499000</v>
@@ -16965,7 +16993,7 @@
     </row>
     <row r="23" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="B23" s="2">
         <v>500</v>
@@ -16974,7 +17002,7 @@
         <v>8</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E23" s="2">
         <v>6799000</v>
@@ -16985,13 +17013,13 @@
         <v>344</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E24" s="2">
         <v>778500</v>
@@ -17002,13 +17030,13 @@
         <v>344</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E25" s="2">
         <v>719300</v>
@@ -17019,13 +17047,13 @@
         <v>344</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E26" s="2">
         <v>950900</v>
@@ -17042,7 +17070,7 @@
         <v>380</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E27" s="2">
         <v>1316900</v>
@@ -17053,13 +17081,13 @@
         <v>242</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>264</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="E28" s="2">
         <v>2769000</v>
@@ -17076,7 +17104,7 @@
         <v>303</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E29" s="2">
         <v>2244900</v>
@@ -17093,7 +17121,7 @@
         <v>259</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="E30" s="2">
         <v>1574900</v>
@@ -17110,7 +17138,7 @@
         <v>259</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="E31" s="2">
         <v>1434900</v>
@@ -17121,13 +17149,13 @@
         <v>344</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E32" s="2">
         <v>1059000</v>
@@ -17144,7 +17172,7 @@
         <v>259</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="E33" s="2">
         <v>3969000</v>
@@ -17161,7 +17189,7 @@
         <v>8</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="E34" s="2">
         <v>1314000</v>
@@ -17172,13 +17200,13 @@
         <v>215</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E35" s="2">
         <v>2149000</v>
@@ -17195,7 +17223,7 @@
         <v>5</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="E36" s="2">
         <v>2599000</v>
@@ -17206,13 +17234,13 @@
         <v>215</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="E37" s="2">
         <v>2599000</v>
@@ -17229,7 +17257,7 @@
         <v>8</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="E38" s="2">
         <v>5269000</v>
@@ -17246,7 +17274,7 @@
         <v>303</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E39" s="2">
         <v>2314900</v>
@@ -17257,13 +17285,13 @@
         <v>344</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E40" s="2">
         <v>918900</v>
@@ -17280,7 +17308,7 @@
         <v>259</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E41" s="2">
         <v>2159900</v>
@@ -17297,7 +17325,7 @@
         <v>8</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="E42" s="2">
         <v>1106900</v>
@@ -17314,7 +17342,7 @@
         <v>8</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="E43" s="2">
         <v>1249900</v>
@@ -17331,7 +17359,7 @@
         <v>8</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E44" s="2">
         <v>2900000</v>
@@ -17342,13 +17370,13 @@
         <v>22</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E45" s="2">
         <v>2439900</v>
@@ -17365,7 +17393,7 @@
         <v>312</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E46" s="2">
         <v>2734900</v>
@@ -17382,7 +17410,7 @@
         <v>312</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E47" s="2">
         <v>1934900</v>
@@ -17399,7 +17427,7 @@
         <v>8</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E48" s="2">
         <v>2064900</v>
@@ -17416,7 +17444,7 @@
         <v>334</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E49" s="2">
         <v>2849900</v>
@@ -17424,7 +17452,7 @@
     </row>
     <row r="50" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A50" s="1" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>279</v>
@@ -17433,7 +17461,7 @@
         <v>8</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E50" s="2">
         <v>1779000</v>
@@ -17441,7 +17469,7 @@
     </row>
     <row r="51" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>273</v>
@@ -17450,7 +17478,7 @@
         <v>8</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E51" s="2">
         <v>2150000</v>
@@ -17458,7 +17486,7 @@
     </row>
     <row r="52" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A52" s="1" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>278</v>
@@ -17467,7 +17495,7 @@
         <v>8</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E52" s="2">
         <v>2129900</v>
@@ -17475,7 +17503,7 @@
     </row>
     <row r="53" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>472</v>
@@ -17484,7 +17512,7 @@
         <v>8</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E53" s="2">
         <v>2369900</v>
@@ -17501,7 +17529,7 @@
         <v>8</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E54" s="2">
         <v>1690000</v>
@@ -17518,7 +17546,7 @@
         <v>8</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E55" s="2">
         <v>2869900</v>
@@ -17529,13 +17557,13 @@
         <v>22</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E56" s="2">
         <v>2569900</v>
@@ -17546,13 +17574,13 @@
         <v>22</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E57" s="2">
         <v>2839900</v>
@@ -17569,7 +17597,7 @@
         <v>26</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E58" s="2">
         <v>3969900</v>
@@ -17586,7 +17614,7 @@
         <v>26</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E59" s="2">
         <v>3069900</v>
@@ -17603,7 +17631,7 @@
         <v>26</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E60" s="2">
         <v>3069900</v>
@@ -17614,13 +17642,13 @@
         <v>22</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="E61" s="2">
         <v>2899900</v>
@@ -17628,7 +17656,7 @@
     </row>
     <row r="62" ht="40.35" customHeight="1" spans="1:5">
       <c r="A62" s="1" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>135</v>
@@ -17637,7 +17665,7 @@
         <v>26</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E62" s="2">
         <v>2374000</v>
@@ -17645,7 +17673,7 @@
     </row>
     <row r="63" ht="40.35" customHeight="1" spans="1:5">
       <c r="A63" s="1" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>136</v>
@@ -17654,7 +17682,7 @@
         <v>26</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E63" s="2">
         <v>2411000</v>
@@ -17662,7 +17690,7 @@
     </row>
     <row r="64" ht="40.35" customHeight="1" spans="1:5">
       <c r="A64" s="1" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>137</v>
@@ -17671,7 +17699,7 @@
         <v>26</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E64" s="2">
         <v>2024000</v>
@@ -17688,7 +17716,7 @@
         <v>82</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="E65" s="2">
         <v>1124000</v>
@@ -17705,7 +17733,7 @@
         <v>103</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E66" s="2">
         <v>1051000</v>
@@ -17722,7 +17750,7 @@
         <v>534</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E67" s="2">
         <v>1657000</v>
@@ -17739,7 +17767,7 @@
         <v>5</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E68" s="2">
         <v>1705000</v>
@@ -17756,7 +17784,7 @@
         <v>5</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="E69" s="2">
         <v>1699900</v>
@@ -17773,7 +17801,7 @@
         <v>26</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E70" s="2">
         <v>2489900</v>
@@ -17781,7 +17809,7 @@
     </row>
     <row r="71" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A71" s="1" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>273</v>
@@ -17790,7 +17818,7 @@
         <v>26</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E71" s="2">
         <v>2959900</v>
@@ -17798,7 +17826,7 @@
     </row>
     <row r="72" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A72" s="1" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="B72" s="2">
         <v>3</v>
@@ -17807,7 +17835,7 @@
         <v>26</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E72" s="2">
         <v>1765000</v>
@@ -17824,7 +17852,7 @@
         <v>226</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="E73" s="2">
         <v>4409000</v>
@@ -17841,7 +17869,7 @@
         <v>226</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="E74" s="2">
         <v>1690000</v>
@@ -17858,7 +17886,7 @@
         <v>85</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E75" s="2">
         <v>950900</v>
@@ -17875,7 +17903,7 @@
         <v>8</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="E76" s="2">
         <v>880900</v>
@@ -17892,7 +17920,7 @@
         <v>82</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E77" s="2">
         <v>953900</v>
@@ -17909,7 +17937,7 @@
         <v>103</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E78" s="2">
         <v>2179000</v>
@@ -17926,7 +17954,7 @@
         <v>8</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="E79" s="2">
         <v>1579000</v>
@@ -17943,7 +17971,7 @@
         <v>5</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="E80" s="2">
         <v>4299000</v>
@@ -17960,7 +17988,7 @@
         <v>8</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="E81" s="2">
         <v>2049000</v>
@@ -17977,7 +18005,7 @@
         <v>8</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E82" s="2">
         <v>3149000</v>
@@ -17994,7 +18022,7 @@
         <v>82</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
       <c r="E83" s="2">
         <v>2337000</v>
@@ -18005,13 +18033,13 @@
         <v>457</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>303</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
       <c r="E84" s="2">
         <v>2762000</v>
@@ -18028,7 +18056,7 @@
         <v>103</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E85" s="2">
         <v>1618000</v>
@@ -18045,7 +18073,7 @@
         <v>82</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="E86" s="2">
         <v>1301000</v>
@@ -18062,7 +18090,7 @@
         <v>82</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="E87" s="2">
         <v>1258000</v>
@@ -18079,7 +18107,7 @@
         <v>82</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="E88" s="2">
         <v>1373000</v>
@@ -18096,7 +18124,7 @@
         <v>5</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="E89" s="2">
         <v>1724000</v>
@@ -18113,7 +18141,7 @@
         <v>8</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E90" s="2">
         <v>1874000</v>
@@ -18130,7 +18158,7 @@
         <v>5</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E91" s="2">
         <v>2057000</v>
@@ -18147,7 +18175,7 @@
         <v>5</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E92" s="2">
         <v>2118900</v>
@@ -18164,7 +18192,7 @@
         <v>5</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E93" s="2">
         <v>3248000</v>
@@ -18181,7 +18209,7 @@
         <v>5</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E94" s="2">
         <v>5378000</v>
@@ -18198,7 +18226,7 @@
         <v>5</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E95" s="2">
         <v>5806000</v>
@@ -18215,7 +18243,7 @@
         <v>303</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E96" s="2">
         <v>2388000</v>
@@ -18232,7 +18260,7 @@
         <v>303</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E97" s="2">
         <v>2681000</v>
@@ -18249,7 +18277,7 @@
         <v>617</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="E98" s="2">
         <v>1385900</v>
@@ -18266,7 +18294,7 @@
         <v>608</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>1030</v>
+        <v>1032</v>
       </c>
       <c r="E99" s="2">
         <v>1518000</v>
@@ -18283,7 +18311,7 @@
         <v>82</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E100" s="2">
         <v>3375900</v>
@@ -18300,7 +18328,7 @@
         <v>8</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E101" s="2">
         <v>2828900</v>
@@ -18317,7 +18345,7 @@
         <v>5</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E102" s="2">
         <v>4449900</v>
@@ -18334,7 +18362,7 @@
         <v>8</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="E103" s="2">
         <v>1229000</v>
@@ -18351,7 +18379,7 @@
         <v>103</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E104" s="2">
         <v>2499000</v>
@@ -18359,7 +18387,7 @@
     </row>
     <row r="105" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A105" s="1" t="s">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>595</v>
@@ -18368,7 +18396,7 @@
         <v>596</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="E105" s="2">
         <v>1680000</v>
@@ -18376,16 +18404,16 @@
     </row>
     <row r="106" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A106" s="1" t="s">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>596</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="E106" s="2">
         <v>1705000</v>
@@ -18393,7 +18421,7 @@
     </row>
     <row r="107" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A107" s="1" t="s">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>39</v>
@@ -18402,7 +18430,7 @@
         <v>8</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="E107" s="2">
         <v>1510000</v>
@@ -18419,7 +18447,7 @@
         <v>8</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E108" s="2">
         <v>2570000</v>
@@ -18436,7 +18464,7 @@
         <v>8</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E109" s="2">
         <v>3430000</v>
@@ -18447,13 +18475,13 @@
         <v>54</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E110" s="2">
         <v>2770000</v>
@@ -18470,7 +18498,7 @@
         <v>5</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E111" s="2">
         <v>1970000</v>
@@ -18481,13 +18509,13 @@
         <v>54</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>1037</v>
+        <v>1039</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E112" s="2">
         <v>3250000</v>
@@ -18498,13 +18526,13 @@
         <v>54</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E113" s="2">
         <v>3370000</v>
@@ -18521,7 +18549,7 @@
         <v>8</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E114" s="2">
         <v>3759900</v>
@@ -18538,7 +18566,7 @@
         <v>5</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E115" s="2">
         <v>3380000</v>
@@ -18555,7 +18583,7 @@
         <v>5</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E116" s="2">
         <v>3810000</v>
@@ -18572,7 +18600,7 @@
         <v>8</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E117" s="2">
         <v>4910000</v>
@@ -18589,7 +18617,7 @@
         <v>8</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E118" s="2">
         <v>4550000</v>
@@ -18606,7 +18634,7 @@
         <v>8</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E119" s="2">
         <v>2080000</v>
@@ -18623,7 +18651,7 @@
         <v>8</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E120" s="2">
         <v>2225000</v>
@@ -18640,7 +18668,7 @@
         <v>8</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E121" s="2">
         <v>2970000</v>
@@ -18657,7 +18685,7 @@
         <v>5</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E122" s="2">
         <v>4350000</v>
@@ -18674,7 +18702,7 @@
         <v>5</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E123" s="2">
         <v>2999900</v>
@@ -18691,7 +18719,7 @@
         <v>8</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E124" s="2">
         <v>3479900</v>
@@ -18708,7 +18736,7 @@
         <v>5</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E125" s="2">
         <v>1990000</v>
@@ -18725,7 +18753,7 @@
         <v>5</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E126" s="2">
         <v>2149000</v>
@@ -18742,7 +18770,7 @@
         <v>8</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E127" s="2">
         <v>2115000</v>
@@ -18759,7 +18787,7 @@
         <v>8</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E128" s="2">
         <v>2238000</v>
@@ -18776,7 +18804,7 @@
         <v>8</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E129" s="2">
         <v>2514900</v>
@@ -18793,7 +18821,7 @@
         <v>8</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E130" s="2">
         <v>2997900</v>
@@ -18801,16 +18829,16 @@
     </row>
     <row r="131" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A131" s="1" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E131" s="2">
         <v>2549900</v>
@@ -18818,16 +18846,16 @@
     </row>
     <row r="132" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A132" s="1" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E132" s="2">
         <v>2629900</v>
@@ -18835,16 +18863,16 @@
     </row>
     <row r="133" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A133" s="1" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E133" s="2">
         <v>4100000</v>
@@ -18861,7 +18889,7 @@
         <v>8</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
       <c r="E134" s="2">
         <v>2219900</v>
@@ -18872,13 +18900,13 @@
         <v>22</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E135" s="2">
         <v>2499900</v>
@@ -18886,7 +18914,7 @@
     </row>
     <row r="136" ht="27.15" customHeight="1" spans="1:5">
       <c r="A136" s="1" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>145</v>
@@ -18895,7 +18923,7 @@
         <v>8</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>1044</v>
+        <v>1046</v>
       </c>
       <c r="E136" s="2">
         <v>1602000</v>
@@ -18903,7 +18931,7 @@
     </row>
     <row r="137" ht="40.35" customHeight="1" spans="1:5">
       <c r="A137" s="1" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>146</v>
@@ -18912,7 +18940,7 @@
         <v>5</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="E137" s="2">
         <v>1508000</v>
@@ -18929,7 +18957,7 @@
         <v>8</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E138" s="2">
         <v>4549990</v>
@@ -18946,7 +18974,7 @@
         <v>8</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E139" s="2">
         <v>2479990</v>
@@ -18963,7 +18991,7 @@
         <v>8</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="E140" s="2">
         <v>2075990</v>
@@ -18980,7 +19008,7 @@
         <v>8</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E141" s="2">
         <v>2080990</v>
@@ -18997,7 +19025,7 @@
         <v>380</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E142" s="2">
         <v>2273000</v>
@@ -19014,7 +19042,7 @@
         <v>380</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E143" s="2">
         <v>2443000</v>
@@ -19031,7 +19059,7 @@
         <v>5</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E144" s="2">
         <v>1341000</v>
@@ -19042,13 +19070,13 @@
         <v>344</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E145" s="2">
         <v>1381000</v>
@@ -19059,13 +19087,13 @@
         <v>344</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E146" s="2">
         <v>1493000</v>
@@ -19076,13 +19104,13 @@
         <v>344</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E147" s="2">
         <v>1533000</v>
@@ -19099,7 +19127,7 @@
         <v>5</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E148" s="2">
         <v>1670000</v>
@@ -19116,7 +19144,7 @@
         <v>8</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E149" s="2">
         <v>1487000</v>
@@ -19127,13 +19155,13 @@
         <v>54</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>1049</v>
+        <v>1051</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E150" s="2">
         <v>4850000</v>
@@ -19144,13 +19172,13 @@
         <v>54</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E151" s="2">
         <v>4000000</v>
@@ -19161,13 +19189,13 @@
         <v>54</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>1051</v>
+        <v>1053</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E152" s="2">
         <v>4930000</v>
@@ -19184,7 +19212,7 @@
         <v>5</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E153" s="2">
         <v>3692990</v>
@@ -19201,7 +19229,7 @@
         <v>270</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="E154" s="2">
         <v>3979000</v>
@@ -19218,7 +19246,7 @@
         <v>8</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E155" s="2">
         <v>4099000</v>
@@ -19235,7 +19263,7 @@
         <v>8</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E156" s="2">
         <v>3449000</v>
@@ -19252,7 +19280,7 @@
         <v>8</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E157" s="2">
         <v>2799000</v>
@@ -19263,13 +19291,13 @@
         <v>200</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E158" s="2">
         <v>3549000</v>
@@ -19280,13 +19308,13 @@
         <v>200</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E159" s="2">
         <v>3299000</v>
@@ -19303,7 +19331,7 @@
         <v>330</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E160" s="2">
         <v>7374900</v>
@@ -19320,7 +19348,7 @@
         <v>270</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E161" s="2">
         <v>3789900</v>
@@ -19337,7 +19365,7 @@
         <v>51</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E162" s="2">
         <v>5829900</v>
@@ -19354,7 +19382,7 @@
         <v>270</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E163" s="2">
         <v>4144900</v>
@@ -19362,16 +19390,16 @@
     </row>
     <row r="164" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A164" s="1" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E164" s="2">
         <v>1672000</v>
@@ -19388,7 +19416,7 @@
         <v>8</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E165" s="2">
         <v>2040546</v>
@@ -19405,7 +19433,7 @@
         <v>8</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E166" s="2">
         <v>3100000</v>
@@ -19422,7 +19450,7 @@
         <v>8</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E167" s="2">
         <v>2990000</v>
@@ -19439,7 +19467,7 @@
         <v>312</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="E168" s="2">
         <v>8669500</v>
@@ -19456,7 +19484,7 @@
         <v>677</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E169" s="2">
         <v>4291000</v>
@@ -19473,7 +19501,7 @@
         <v>5</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E170" s="2">
         <v>6146500</v>
@@ -19481,7 +19509,7 @@
     </row>
     <row r="171" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A171" s="1" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>274</v>
@@ -19490,7 +19518,7 @@
         <v>8</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E171" s="2">
         <v>1889000</v>
@@ -19498,7 +19526,7 @@
     </row>
     <row r="172" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A172" s="1" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>276</v>
@@ -19507,7 +19535,7 @@
         <v>8</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E172" s="2">
         <v>2399000</v>
@@ -19515,7 +19543,7 @@
     </row>
     <row r="173" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A173" s="1" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>653</v>
@@ -19524,7 +19552,7 @@
         <v>8</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E173" s="2">
         <v>3059000</v>
@@ -19532,16 +19560,16 @@
     </row>
     <row r="174" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A174" s="1" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E174" s="2">
         <v>3279000</v>
@@ -19549,7 +19577,7 @@
     </row>
     <row r="175" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A175" s="1" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>654</v>
@@ -19558,7 +19586,7 @@
         <v>8</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E175" s="2">
         <v>3599000</v>
@@ -19566,7 +19594,7 @@
     </row>
     <row r="176" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A176" s="1" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>175</v>
@@ -19575,7 +19603,7 @@
         <v>8</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E176" s="2">
         <v>5499999</v>
@@ -19583,7 +19611,7 @@
     </row>
     <row r="177" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A177" s="1" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>172</v>
@@ -19592,7 +19620,7 @@
         <v>103</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E177" s="2">
         <v>4099000</v>
@@ -19600,7 +19628,7 @@
     </row>
     <row r="178" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A178" s="1" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>169</v>
@@ -19609,7 +19637,7 @@
         <v>8</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E178" s="2">
         <v>2449000</v>
@@ -19620,13 +19648,13 @@
         <v>22</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E179" s="2">
         <v>4529900</v>
@@ -19643,7 +19671,7 @@
         <v>8</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E180" s="2">
         <v>3739900</v>
@@ -19654,13 +19682,13 @@
         <v>22</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E181" s="2">
         <v>5219900</v>
@@ -19671,13 +19699,13 @@
         <v>54</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>1059</v>
+        <v>1061</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E182" s="2">
         <v>2780000</v>
@@ -19694,7 +19722,7 @@
         <v>8</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E183" s="2">
         <v>2020000</v>
@@ -19711,7 +19739,7 @@
         <v>8</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E184" s="2">
         <v>2650000</v>
@@ -19728,7 +19756,7 @@
         <v>8</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E185" s="2">
         <v>2080000</v>
@@ -19745,7 +19773,7 @@
         <v>8</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E186" s="2">
         <v>2181000</v>
@@ -19762,7 +19790,7 @@
         <v>5</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="E187" s="2">
         <v>2279000</v>
@@ -19779,7 +19807,7 @@
         <v>103</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="E188" s="2">
         <v>2899000</v>
@@ -19796,7 +19824,7 @@
         <v>82</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E189" s="2">
         <v>2379000</v>
@@ -19804,16 +19832,16 @@
     </row>
     <row r="190" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A190" s="1" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>1061</v>
+        <v>1063</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E190" s="2">
         <v>2499000</v>
@@ -19821,7 +19849,7 @@
     </row>
     <row r="191" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A191" s="1" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>473</v>
@@ -19830,7 +19858,7 @@
         <v>8</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E191" s="2">
         <v>2479900</v>
@@ -19847,7 +19875,7 @@
         <v>8</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E192" s="2">
         <v>3959000</v>
@@ -19858,13 +19886,13 @@
         <v>121</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E193" s="2">
         <v>2890000</v>
@@ -19875,13 +19903,13 @@
         <v>121</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E194" s="2">
         <v>4080000</v>
@@ -19892,13 +19920,13 @@
         <v>121</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E195" s="2">
         <v>6290000</v>
@@ -19906,7 +19934,7 @@
     </row>
     <row r="196" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A196" s="1" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="B196" s="2">
         <v>6</v>
@@ -19915,7 +19943,7 @@
         <v>8</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E196" s="2">
         <v>2200000</v>
@@ -19923,7 +19951,7 @@
     </row>
     <row r="197" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A197" s="1" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>284</v>
@@ -19932,7 +19960,7 @@
         <v>8</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E197" s="2">
         <v>4599000</v>
@@ -19949,7 +19977,7 @@
         <v>8</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E198" s="2">
         <v>2199000</v>
@@ -19960,13 +19988,13 @@
         <v>215</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E199" s="2">
         <v>4599000</v>
@@ -19977,13 +20005,13 @@
         <v>105</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>1066</v>
+        <v>1068</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E200" s="2">
         <v>1990000</v>
@@ -19994,13 +20022,13 @@
         <v>105</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E201" s="2">
         <v>3590000</v>
@@ -20017,7 +20045,7 @@
         <v>8</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E202" s="2">
         <v>2650000</v>
@@ -20028,13 +20056,13 @@
         <v>215</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E203" s="2">
         <v>2849000</v>
@@ -20042,7 +20070,7 @@
     </row>
     <row r="204" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A204" s="1" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>171</v>
@@ -20051,7 +20079,7 @@
         <v>8</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E204" s="2">
         <v>2099000</v>
@@ -20068,7 +20096,7 @@
         <v>8</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="E205" s="2">
         <v>1263000</v>
@@ -20085,7 +20113,7 @@
         <v>8</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E206" s="2">
         <v>1546500</v>
@@ -20102,7 +20130,7 @@
         <v>8</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="E207" s="2">
         <v>883000</v>
@@ -20119,7 +20147,7 @@
         <v>8</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="E208" s="2">
         <v>825000</v>
@@ -20136,7 +20164,7 @@
         <v>8</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="E209" s="2">
         <v>851000</v>
@@ -20147,13 +20175,13 @@
         <v>176</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E210" s="2">
         <v>3357990</v>
@@ -20164,13 +20192,13 @@
         <v>215</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>1073</v>
+        <v>1075</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E211" s="2">
         <v>3899000</v>
@@ -20187,7 +20215,7 @@
         <v>8</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E212" s="2">
         <v>1990000</v>
@@ -20204,7 +20232,7 @@
         <v>8</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E213" s="2">
         <v>2199000</v>
@@ -20221,7 +20249,7 @@
         <v>8</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="E214" s="2">
         <v>789900</v>
@@ -20238,7 +20266,7 @@
         <v>51</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>1074</v>
+        <v>1076</v>
       </c>
       <c r="E215" s="2">
         <v>869900</v>
@@ -20255,7 +20283,7 @@
         <v>8</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>1075</v>
+        <v>1077</v>
       </c>
       <c r="E216" s="2">
         <v>1089000</v>
@@ -20272,7 +20300,7 @@
         <v>8</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="E217" s="2">
         <v>999900</v>
@@ -20289,7 +20317,7 @@
         <v>8</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="E218" s="2">
         <v>1455000</v>
@@ -20306,7 +20334,7 @@
         <v>103</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>1074</v>
+        <v>1076</v>
       </c>
       <c r="E219" s="2">
         <v>809900</v>
@@ -20323,7 +20351,7 @@
         <v>8</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="E220" s="2">
         <v>2000000</v>
@@ -20340,7 +20368,7 @@
         <v>8</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="E221" s="2">
         <v>1229900</v>
@@ -20357,7 +20385,7 @@
         <v>8</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="E222" s="2">
         <v>2656800</v>
@@ -20368,13 +20396,13 @@
         <v>344</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="E223" s="2">
         <v>824000</v>
@@ -20385,13 +20413,13 @@
         <v>300</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>1077</v>
+        <v>1079</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>1030</v>
+        <v>1032</v>
       </c>
       <c r="E224" s="2">
         <v>1204900</v>
@@ -20408,7 +20436,7 @@
         <v>8</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="E225" s="2">
         <v>2234900</v>
@@ -20416,7 +20444,7 @@
     </row>
     <row r="226" ht="40.35" customHeight="1" spans="1:5">
       <c r="A226" s="1" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>138</v>
@@ -20425,7 +20453,7 @@
         <v>5</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="E226" s="2">
         <v>2673000</v>
@@ -20442,7 +20470,7 @@
         <v>8</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>1078</v>
+        <v>1080</v>
       </c>
       <c r="E227" s="2">
         <v>1419990</v>
@@ -20450,7 +20478,7 @@
     </row>
     <row r="228" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A228" s="1" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>277</v>
@@ -20459,7 +20487,7 @@
         <v>8</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>1079</v>
+        <v>1081</v>
       </c>
       <c r="E228" s="2">
         <v>1494000</v>
@@ -20476,7 +20504,7 @@
         <v>8</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E229" s="2">
         <v>2849990</v>
@@ -20490,10 +20518,10 @@
         <v>591</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>1080</v>
+        <v>1082</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E230" s="2">
         <v>3173000</v>
@@ -20504,13 +20532,13 @@
         <v>54</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>1081</v>
+        <v>1083</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E231" s="2">
         <v>2380000</v>
@@ -20527,7 +20555,7 @@
         <v>8</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E232" s="2">
         <v>2599000</v>
@@ -20535,16 +20563,16 @@
     </row>
     <row r="233" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A233" s="1" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>1082</v>
+        <v>1084</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E233" s="2">
         <v>2999000</v>
@@ -20555,13 +20583,13 @@
         <v>22</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>1083</v>
+        <v>1085</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>312</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E234" s="2">
         <v>3590000</v>
@@ -20569,16 +20597,16 @@
     </row>
     <row r="235" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A235" s="1" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>1084</v>
+        <v>1086</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E235" s="2">
         <v>2569900</v>
@@ -20595,7 +20623,7 @@
         <v>8</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E236" s="2">
         <v>4750000</v>
@@ -20603,16 +20631,16 @@
     </row>
     <row r="237" ht="40.35" customHeight="1" spans="1:5">
       <c r="A237" s="1" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E237" s="2">
         <v>2499990</v>
@@ -20620,7 +20648,7 @@
     </row>
     <row r="238" ht="27.15" customHeight="1" spans="1:5">
       <c r="A238" s="1" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>793</v>
@@ -20629,7 +20657,7 @@
         <v>8</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E238" s="2">
         <v>2779990</v>
@@ -20646,7 +20674,7 @@
         <v>51</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E239" s="2">
         <v>2649000</v>
@@ -20663,7 +20691,7 @@
         <v>5</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E240" s="2">
         <v>1899000</v>
@@ -20680,7 +20708,7 @@
         <v>8</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E241" s="2">
         <v>2825990</v>
@@ -20688,7 +20716,7 @@
     </row>
     <row r="242" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A242" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="B242" s="2">
         <v>400</v>
@@ -20697,7 +20725,7 @@
         <v>8</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E242" s="2">
         <v>5799000</v>
@@ -20705,7 +20733,7 @@
     </row>
     <row r="243" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A243" s="1" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>280</v>
@@ -20714,7 +20742,7 @@
         <v>8</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>1086</v>
+        <v>1088</v>
       </c>
       <c r="E243" s="2">
         <v>2899000</v>
@@ -20731,7 +20759,7 @@
         <v>8</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E244" s="2">
         <v>1887500</v>
@@ -20748,7 +20776,7 @@
         <v>8</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E245" s="2">
         <v>1805000</v>
@@ -20765,7 +20793,7 @@
         <v>8</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E246" s="2">
         <v>1684500</v>
@@ -20773,7 +20801,7 @@
     </row>
     <row r="247" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A247" s="1" t="s">
-        <v>1087</v>
+        <v>1089</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>785</v>
@@ -20782,7 +20810,7 @@
         <v>8</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E247" s="2">
         <v>3899000</v>
@@ -20790,7 +20818,7 @@
     </row>
     <row r="248" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A248" s="1" t="s">
-        <v>1087</v>
+        <v>1089</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>784</v>
@@ -20799,7 +20827,7 @@
         <v>8</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E248" s="2">
         <v>3099000</v>
@@ -20807,7 +20835,7 @@
     </row>
     <row r="249" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A249" s="1" t="s">
-        <v>1088</v>
+        <v>1090</v>
       </c>
       <c r="B249" s="2">
         <v>1</v>
@@ -20816,7 +20844,7 @@
         <v>8</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="E249" s="2">
         <v>4162990</v>

</xml_diff>

<commit_message>
Fix avanta-avto-credit, add 3 cars
</commit_message>
<xml_diff>
--- a/id.xlsx
+++ b/id.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$G$923</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$G$925</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Лист2!$A$1:$E$249</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3077" uniqueCount="1091">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3079" uniqueCount="1092">
   <si>
     <t>Aito</t>
   </si>
@@ -2972,6 +2972,9 @@
   </si>
   <si>
     <t>C7</t>
+  </si>
+  <si>
+    <t>H7 New</t>
   </si>
   <si>
     <t>Марка</t>
@@ -4295,10 +4298,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G925"/>
+  <dimension ref="A1:G926"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A905" workbookViewId="0">
-      <selection activeCell="F920" sqref="F920"/>
+      <selection activeCell="D925" sqref="D925"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -16597,8 +16600,19 @@
         <v>979</v>
       </c>
     </row>
+    <row r="926" spans="1:3">
+      <c r="A926">
+        <v>1025</v>
+      </c>
+      <c r="B926" t="s">
+        <v>215</v>
+      </c>
+      <c r="C926" t="s">
+        <v>980</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G923" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G925" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -16619,19 +16633,19 @@
   <sheetData>
     <row r="1" ht="27.15" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
     </row>
     <row r="2" ht="40.35" hidden="1" customHeight="1" spans="1:5">
@@ -16639,13 +16653,13 @@
         <v>344</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>380</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E2" s="2">
         <v>1239900</v>
@@ -16662,7 +16676,7 @@
         <v>380</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E3" s="2">
         <v>1759000</v>
@@ -16679,7 +16693,7 @@
         <v>380</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E4" s="2">
         <v>1655000</v>
@@ -16696,7 +16710,7 @@
         <v>380</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E5" s="2">
         <v>1879000</v>
@@ -16707,13 +16721,13 @@
         <v>344</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E6" s="2">
         <v>1077000</v>
@@ -16730,7 +16744,7 @@
         <v>82</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="E7" s="2">
         <v>1408000</v>
@@ -16741,13 +16755,13 @@
         <v>344</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E8" s="2">
         <v>749900</v>
@@ -16764,7 +16778,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E9" s="2">
         <v>1175000</v>
@@ -16781,7 +16795,7 @@
         <v>252</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="E10" s="2">
         <v>2149000</v>
@@ -16798,7 +16812,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E11" s="2">
         <v>1660000</v>
@@ -16815,7 +16829,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E12" s="2">
         <v>2020000</v>
@@ -16832,7 +16846,7 @@
         <v>103</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="E13" s="2">
         <v>1859000</v>
@@ -16849,7 +16863,7 @@
         <v>303</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E14" s="2">
         <v>1334900</v>
@@ -16860,13 +16874,13 @@
         <v>176</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E15" s="2">
         <v>3512990</v>
@@ -16883,7 +16897,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E16" s="2">
         <v>2836990</v>
@@ -16900,7 +16914,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="E17" s="2">
         <v>1850000</v>
@@ -16917,7 +16931,7 @@
         <v>270</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="E18" s="2">
         <v>2749000</v>
@@ -16934,7 +16948,7 @@
         <v>103</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E19" s="2">
         <v>2179990</v>
@@ -16945,13 +16959,13 @@
         <v>176</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E20" s="2">
         <v>2794990</v>
@@ -16968,7 +16982,7 @@
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E21" s="2">
         <v>3959990</v>
@@ -16976,7 +16990,7 @@
     </row>
     <row r="22" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B22" s="2">
         <v>300</v>
@@ -16985,7 +16999,7 @@
         <v>8</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E22" s="2">
         <v>4499000</v>
@@ -16993,7 +17007,7 @@
     </row>
     <row r="23" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B23" s="2">
         <v>500</v>
@@ -17002,7 +17016,7 @@
         <v>8</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E23" s="2">
         <v>6799000</v>
@@ -17013,13 +17027,13 @@
         <v>344</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E24" s="2">
         <v>778500</v>
@@ -17030,13 +17044,13 @@
         <v>344</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E25" s="2">
         <v>719300</v>
@@ -17047,13 +17061,13 @@
         <v>344</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E26" s="2">
         <v>950900</v>
@@ -17070,7 +17084,7 @@
         <v>380</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E27" s="2">
         <v>1316900</v>
@@ -17081,13 +17095,13 @@
         <v>242</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>264</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="E28" s="2">
         <v>2769000</v>
@@ -17104,7 +17118,7 @@
         <v>303</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E29" s="2">
         <v>2244900</v>
@@ -17121,7 +17135,7 @@
         <v>259</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="E30" s="2">
         <v>1574900</v>
@@ -17138,7 +17152,7 @@
         <v>259</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="E31" s="2">
         <v>1434900</v>
@@ -17149,13 +17163,13 @@
         <v>344</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E32" s="2">
         <v>1059000</v>
@@ -17172,7 +17186,7 @@
         <v>259</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="E33" s="2">
         <v>3969000</v>
@@ -17189,7 +17203,7 @@
         <v>8</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="E34" s="2">
         <v>1314000</v>
@@ -17200,13 +17214,13 @@
         <v>215</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E35" s="2">
         <v>2149000</v>
@@ -17223,7 +17237,7 @@
         <v>5</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="E36" s="2">
         <v>2599000</v>
@@ -17234,13 +17248,13 @@
         <v>215</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="E37" s="2">
         <v>2599000</v>
@@ -17257,7 +17271,7 @@
         <v>8</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="E38" s="2">
         <v>5269000</v>
@@ -17274,7 +17288,7 @@
         <v>303</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E39" s="2">
         <v>2314900</v>
@@ -17285,13 +17299,13 @@
         <v>344</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E40" s="2">
         <v>918900</v>
@@ -17308,7 +17322,7 @@
         <v>259</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E41" s="2">
         <v>2159900</v>
@@ -17325,7 +17339,7 @@
         <v>8</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="E42" s="2">
         <v>1106900</v>
@@ -17342,7 +17356,7 @@
         <v>8</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="E43" s="2">
         <v>1249900</v>
@@ -17359,7 +17373,7 @@
         <v>8</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E44" s="2">
         <v>2900000</v>
@@ -17370,13 +17384,13 @@
         <v>22</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E45" s="2">
         <v>2439900</v>
@@ -17393,7 +17407,7 @@
         <v>312</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E46" s="2">
         <v>2734900</v>
@@ -17410,7 +17424,7 @@
         <v>312</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E47" s="2">
         <v>1934900</v>
@@ -17427,7 +17441,7 @@
         <v>8</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E48" s="2">
         <v>2064900</v>
@@ -17444,7 +17458,7 @@
         <v>334</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E49" s="2">
         <v>2849900</v>
@@ -17452,7 +17466,7 @@
     </row>
     <row r="50" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A50" s="1" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>279</v>
@@ -17461,7 +17475,7 @@
         <v>8</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E50" s="2">
         <v>1779000</v>
@@ -17469,7 +17483,7 @@
     </row>
     <row r="51" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>273</v>
@@ -17478,7 +17492,7 @@
         <v>8</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E51" s="2">
         <v>2150000</v>
@@ -17486,7 +17500,7 @@
     </row>
     <row r="52" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A52" s="1" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>278</v>
@@ -17495,7 +17509,7 @@
         <v>8</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E52" s="2">
         <v>2129900</v>
@@ -17503,7 +17517,7 @@
     </row>
     <row r="53" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>472</v>
@@ -17512,7 +17526,7 @@
         <v>8</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E53" s="2">
         <v>2369900</v>
@@ -17529,7 +17543,7 @@
         <v>8</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E54" s="2">
         <v>1690000</v>
@@ -17546,7 +17560,7 @@
         <v>8</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E55" s="2">
         <v>2869900</v>
@@ -17557,13 +17571,13 @@
         <v>22</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E56" s="2">
         <v>2569900</v>
@@ -17574,13 +17588,13 @@
         <v>22</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E57" s="2">
         <v>2839900</v>
@@ -17597,7 +17611,7 @@
         <v>26</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E58" s="2">
         <v>3969900</v>
@@ -17614,7 +17628,7 @@
         <v>26</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E59" s="2">
         <v>3069900</v>
@@ -17631,7 +17645,7 @@
         <v>26</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E60" s="2">
         <v>3069900</v>
@@ -17642,13 +17656,13 @@
         <v>22</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="E61" s="2">
         <v>2899900</v>
@@ -17656,7 +17670,7 @@
     </row>
     <row r="62" ht="40.35" customHeight="1" spans="1:5">
       <c r="A62" s="1" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>135</v>
@@ -17665,7 +17679,7 @@
         <v>26</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E62" s="2">
         <v>2374000</v>
@@ -17673,7 +17687,7 @@
     </row>
     <row r="63" ht="40.35" customHeight="1" spans="1:5">
       <c r="A63" s="1" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>136</v>
@@ -17682,7 +17696,7 @@
         <v>26</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E63" s="2">
         <v>2411000</v>
@@ -17690,7 +17704,7 @@
     </row>
     <row r="64" ht="40.35" customHeight="1" spans="1:5">
       <c r="A64" s="1" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>137</v>
@@ -17699,7 +17713,7 @@
         <v>26</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E64" s="2">
         <v>2024000</v>
@@ -17716,7 +17730,7 @@
         <v>82</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="E65" s="2">
         <v>1124000</v>
@@ -17733,7 +17747,7 @@
         <v>103</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E66" s="2">
         <v>1051000</v>
@@ -17750,7 +17764,7 @@
         <v>534</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E67" s="2">
         <v>1657000</v>
@@ -17767,7 +17781,7 @@
         <v>5</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E68" s="2">
         <v>1705000</v>
@@ -17784,7 +17798,7 @@
         <v>5</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="E69" s="2">
         <v>1699900</v>
@@ -17801,7 +17815,7 @@
         <v>26</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E70" s="2">
         <v>2489900</v>
@@ -17809,7 +17823,7 @@
     </row>
     <row r="71" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A71" s="1" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>273</v>
@@ -17818,7 +17832,7 @@
         <v>26</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E71" s="2">
         <v>2959900</v>
@@ -17826,7 +17840,7 @@
     </row>
     <row r="72" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A72" s="1" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="B72" s="2">
         <v>3</v>
@@ -17835,7 +17849,7 @@
         <v>26</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E72" s="2">
         <v>1765000</v>
@@ -17852,7 +17866,7 @@
         <v>226</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="E73" s="2">
         <v>4409000</v>
@@ -17869,7 +17883,7 @@
         <v>226</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="E74" s="2">
         <v>1690000</v>
@@ -17886,7 +17900,7 @@
         <v>85</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E75" s="2">
         <v>950900</v>
@@ -17903,7 +17917,7 @@
         <v>8</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="E76" s="2">
         <v>880900</v>
@@ -17920,7 +17934,7 @@
         <v>82</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E77" s="2">
         <v>953900</v>
@@ -17937,7 +17951,7 @@
         <v>103</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E78" s="2">
         <v>2179000</v>
@@ -17954,7 +17968,7 @@
         <v>8</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="E79" s="2">
         <v>1579000</v>
@@ -17971,7 +17985,7 @@
         <v>5</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="E80" s="2">
         <v>4299000</v>
@@ -17988,7 +18002,7 @@
         <v>8</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="E81" s="2">
         <v>2049000</v>
@@ -18005,7 +18019,7 @@
         <v>8</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E82" s="2">
         <v>3149000</v>
@@ -18022,7 +18036,7 @@
         <v>82</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="E83" s="2">
         <v>2337000</v>
@@ -18033,13 +18047,13 @@
         <v>457</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>303</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="E84" s="2">
         <v>2762000</v>
@@ -18056,7 +18070,7 @@
         <v>103</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E85" s="2">
         <v>1618000</v>
@@ -18073,7 +18087,7 @@
         <v>82</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="E86" s="2">
         <v>1301000</v>
@@ -18090,7 +18104,7 @@
         <v>82</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="E87" s="2">
         <v>1258000</v>
@@ -18107,7 +18121,7 @@
         <v>82</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="E88" s="2">
         <v>1373000</v>
@@ -18124,7 +18138,7 @@
         <v>5</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="E89" s="2">
         <v>1724000</v>
@@ -18141,7 +18155,7 @@
         <v>8</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E90" s="2">
         <v>1874000</v>
@@ -18158,7 +18172,7 @@
         <v>5</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E91" s="2">
         <v>2057000</v>
@@ -18175,7 +18189,7 @@
         <v>5</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E92" s="2">
         <v>2118900</v>
@@ -18192,7 +18206,7 @@
         <v>5</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E93" s="2">
         <v>3248000</v>
@@ -18209,7 +18223,7 @@
         <v>5</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E94" s="2">
         <v>5378000</v>
@@ -18226,7 +18240,7 @@
         <v>5</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E95" s="2">
         <v>5806000</v>
@@ -18243,7 +18257,7 @@
         <v>303</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E96" s="2">
         <v>2388000</v>
@@ -18260,7 +18274,7 @@
         <v>303</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E97" s="2">
         <v>2681000</v>
@@ -18277,7 +18291,7 @@
         <v>617</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="E98" s="2">
         <v>1385900</v>
@@ -18294,7 +18308,7 @@
         <v>608</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="E99" s="2">
         <v>1518000</v>
@@ -18311,7 +18325,7 @@
         <v>82</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E100" s="2">
         <v>3375900</v>
@@ -18328,7 +18342,7 @@
         <v>8</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E101" s="2">
         <v>2828900</v>
@@ -18345,7 +18359,7 @@
         <v>5</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E102" s="2">
         <v>4449900</v>
@@ -18362,7 +18376,7 @@
         <v>8</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="E103" s="2">
         <v>1229000</v>
@@ -18379,7 +18393,7 @@
         <v>103</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E104" s="2">
         <v>2499000</v>
@@ -18387,7 +18401,7 @@
     </row>
     <row r="105" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A105" s="1" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>595</v>
@@ -18396,7 +18410,7 @@
         <v>596</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="E105" s="2">
         <v>1680000</v>
@@ -18404,16 +18418,16 @@
     </row>
     <row r="106" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A106" s="1" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>596</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="E106" s="2">
         <v>1705000</v>
@@ -18421,7 +18435,7 @@
     </row>
     <row r="107" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A107" s="1" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>39</v>
@@ -18430,7 +18444,7 @@
         <v>8</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="E107" s="2">
         <v>1510000</v>
@@ -18447,7 +18461,7 @@
         <v>8</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E108" s="2">
         <v>2570000</v>
@@ -18464,7 +18478,7 @@
         <v>8</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E109" s="2">
         <v>3430000</v>
@@ -18475,13 +18489,13 @@
         <v>54</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E110" s="2">
         <v>2770000</v>
@@ -18498,7 +18512,7 @@
         <v>5</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E111" s="2">
         <v>1970000</v>
@@ -18509,13 +18523,13 @@
         <v>54</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E112" s="2">
         <v>3250000</v>
@@ -18526,13 +18540,13 @@
         <v>54</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E113" s="2">
         <v>3370000</v>
@@ -18549,7 +18563,7 @@
         <v>8</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E114" s="2">
         <v>3759900</v>
@@ -18566,7 +18580,7 @@
         <v>5</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E115" s="2">
         <v>3380000</v>
@@ -18583,7 +18597,7 @@
         <v>5</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E116" s="2">
         <v>3810000</v>
@@ -18600,7 +18614,7 @@
         <v>8</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E117" s="2">
         <v>4910000</v>
@@ -18617,7 +18631,7 @@
         <v>8</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E118" s="2">
         <v>4550000</v>
@@ -18634,7 +18648,7 @@
         <v>8</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E119" s="2">
         <v>2080000</v>
@@ -18651,7 +18665,7 @@
         <v>8</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E120" s="2">
         <v>2225000</v>
@@ -18668,7 +18682,7 @@
         <v>8</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E121" s="2">
         <v>2970000</v>
@@ -18685,7 +18699,7 @@
         <v>5</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E122" s="2">
         <v>4350000</v>
@@ -18702,7 +18716,7 @@
         <v>5</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E123" s="2">
         <v>2999900</v>
@@ -18719,7 +18733,7 @@
         <v>8</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E124" s="2">
         <v>3479900</v>
@@ -18736,7 +18750,7 @@
         <v>5</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E125" s="2">
         <v>1990000</v>
@@ -18753,7 +18767,7 @@
         <v>5</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E126" s="2">
         <v>2149000</v>
@@ -18770,7 +18784,7 @@
         <v>8</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E127" s="2">
         <v>2115000</v>
@@ -18787,7 +18801,7 @@
         <v>8</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E128" s="2">
         <v>2238000</v>
@@ -18804,7 +18818,7 @@
         <v>8</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E129" s="2">
         <v>2514900</v>
@@ -18821,7 +18835,7 @@
         <v>8</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E130" s="2">
         <v>2997900</v>
@@ -18829,16 +18843,16 @@
     </row>
     <row r="131" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A131" s="1" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E131" s="2">
         <v>2549900</v>
@@ -18846,16 +18860,16 @@
     </row>
     <row r="132" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A132" s="1" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E132" s="2">
         <v>2629900</v>
@@ -18863,16 +18877,16 @@
     </row>
     <row r="133" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A133" s="1" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E133" s="2">
         <v>4100000</v>
@@ -18889,7 +18903,7 @@
         <v>8</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="E134" s="2">
         <v>2219900</v>
@@ -18900,13 +18914,13 @@
         <v>22</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E135" s="2">
         <v>2499900</v>
@@ -18914,7 +18928,7 @@
     </row>
     <row r="136" ht="27.15" customHeight="1" spans="1:5">
       <c r="A136" s="1" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>145</v>
@@ -18923,7 +18937,7 @@
         <v>8</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="E136" s="2">
         <v>1602000</v>
@@ -18931,7 +18945,7 @@
     </row>
     <row r="137" ht="40.35" customHeight="1" spans="1:5">
       <c r="A137" s="1" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>146</v>
@@ -18940,7 +18954,7 @@
         <v>5</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="E137" s="2">
         <v>1508000</v>
@@ -18957,7 +18971,7 @@
         <v>8</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E138" s="2">
         <v>4549990</v>
@@ -18974,7 +18988,7 @@
         <v>8</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E139" s="2">
         <v>2479990</v>
@@ -18991,7 +19005,7 @@
         <v>8</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="E140" s="2">
         <v>2075990</v>
@@ -19008,7 +19022,7 @@
         <v>8</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E141" s="2">
         <v>2080990</v>
@@ -19025,7 +19039,7 @@
         <v>380</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E142" s="2">
         <v>2273000</v>
@@ -19042,7 +19056,7 @@
         <v>380</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E143" s="2">
         <v>2443000</v>
@@ -19059,7 +19073,7 @@
         <v>5</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E144" s="2">
         <v>1341000</v>
@@ -19070,13 +19084,13 @@
         <v>344</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E145" s="2">
         <v>1381000</v>
@@ -19087,13 +19101,13 @@
         <v>344</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E146" s="2">
         <v>1493000</v>
@@ -19104,13 +19118,13 @@
         <v>344</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E147" s="2">
         <v>1533000</v>
@@ -19127,7 +19141,7 @@
         <v>5</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E148" s="2">
         <v>1670000</v>
@@ -19144,7 +19158,7 @@
         <v>8</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E149" s="2">
         <v>1487000</v>
@@ -19155,13 +19169,13 @@
         <v>54</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E150" s="2">
         <v>4850000</v>
@@ -19172,13 +19186,13 @@
         <v>54</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E151" s="2">
         <v>4000000</v>
@@ -19189,13 +19203,13 @@
         <v>54</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E152" s="2">
         <v>4930000</v>
@@ -19212,7 +19226,7 @@
         <v>5</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E153" s="2">
         <v>3692990</v>
@@ -19229,7 +19243,7 @@
         <v>270</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="E154" s="2">
         <v>3979000</v>
@@ -19246,7 +19260,7 @@
         <v>8</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E155" s="2">
         <v>4099000</v>
@@ -19263,7 +19277,7 @@
         <v>8</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E156" s="2">
         <v>3449000</v>
@@ -19280,7 +19294,7 @@
         <v>8</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E157" s="2">
         <v>2799000</v>
@@ -19291,13 +19305,13 @@
         <v>200</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E158" s="2">
         <v>3549000</v>
@@ -19308,13 +19322,13 @@
         <v>200</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E159" s="2">
         <v>3299000</v>
@@ -19331,7 +19345,7 @@
         <v>330</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E160" s="2">
         <v>7374900</v>
@@ -19348,7 +19362,7 @@
         <v>270</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E161" s="2">
         <v>3789900</v>
@@ -19365,7 +19379,7 @@
         <v>51</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E162" s="2">
         <v>5829900</v>
@@ -19382,7 +19396,7 @@
         <v>270</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E163" s="2">
         <v>4144900</v>
@@ -19390,16 +19404,16 @@
     </row>
     <row r="164" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A164" s="1" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E164" s="2">
         <v>1672000</v>
@@ -19416,7 +19430,7 @@
         <v>8</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E165" s="2">
         <v>2040546</v>
@@ -19433,7 +19447,7 @@
         <v>8</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E166" s="2">
         <v>3100000</v>
@@ -19450,7 +19464,7 @@
         <v>8</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E167" s="2">
         <v>2990000</v>
@@ -19467,7 +19481,7 @@
         <v>312</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="E168" s="2">
         <v>8669500</v>
@@ -19484,7 +19498,7 @@
         <v>677</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E169" s="2">
         <v>4291000</v>
@@ -19501,7 +19515,7 @@
         <v>5</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E170" s="2">
         <v>6146500</v>
@@ -19509,7 +19523,7 @@
     </row>
     <row r="171" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A171" s="1" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>274</v>
@@ -19518,7 +19532,7 @@
         <v>8</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E171" s="2">
         <v>1889000</v>
@@ -19526,7 +19540,7 @@
     </row>
     <row r="172" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A172" s="1" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>276</v>
@@ -19535,7 +19549,7 @@
         <v>8</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E172" s="2">
         <v>2399000</v>
@@ -19543,7 +19557,7 @@
     </row>
     <row r="173" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A173" s="1" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>653</v>
@@ -19552,7 +19566,7 @@
         <v>8</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E173" s="2">
         <v>3059000</v>
@@ -19560,16 +19574,16 @@
     </row>
     <row r="174" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A174" s="1" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E174" s="2">
         <v>3279000</v>
@@ -19577,7 +19591,7 @@
     </row>
     <row r="175" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A175" s="1" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>654</v>
@@ -19586,7 +19600,7 @@
         <v>8</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E175" s="2">
         <v>3599000</v>
@@ -19594,7 +19608,7 @@
     </row>
     <row r="176" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A176" s="1" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>175</v>
@@ -19603,7 +19617,7 @@
         <v>8</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E176" s="2">
         <v>5499999</v>
@@ -19611,7 +19625,7 @@
     </row>
     <row r="177" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A177" s="1" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>172</v>
@@ -19620,7 +19634,7 @@
         <v>103</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E177" s="2">
         <v>4099000</v>
@@ -19628,7 +19642,7 @@
     </row>
     <row r="178" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A178" s="1" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>169</v>
@@ -19637,7 +19651,7 @@
         <v>8</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E178" s="2">
         <v>2449000</v>
@@ -19648,13 +19662,13 @@
         <v>22</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E179" s="2">
         <v>4529900</v>
@@ -19671,7 +19685,7 @@
         <v>8</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E180" s="2">
         <v>3739900</v>
@@ -19682,13 +19696,13 @@
         <v>22</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E181" s="2">
         <v>5219900</v>
@@ -19699,13 +19713,13 @@
         <v>54</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E182" s="2">
         <v>2780000</v>
@@ -19722,7 +19736,7 @@
         <v>8</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E183" s="2">
         <v>2020000</v>
@@ -19739,7 +19753,7 @@
         <v>8</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E184" s="2">
         <v>2650000</v>
@@ -19756,7 +19770,7 @@
         <v>8</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E185" s="2">
         <v>2080000</v>
@@ -19773,7 +19787,7 @@
         <v>8</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E186" s="2">
         <v>2181000</v>
@@ -19790,7 +19804,7 @@
         <v>5</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="E187" s="2">
         <v>2279000</v>
@@ -19807,7 +19821,7 @@
         <v>103</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="E188" s="2">
         <v>2899000</v>
@@ -19824,7 +19838,7 @@
         <v>82</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E189" s="2">
         <v>2379000</v>
@@ -19832,16 +19846,16 @@
     </row>
     <row r="190" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A190" s="1" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E190" s="2">
         <v>2499000</v>
@@ -19849,7 +19863,7 @@
     </row>
     <row r="191" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A191" s="1" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>473</v>
@@ -19858,7 +19872,7 @@
         <v>8</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E191" s="2">
         <v>2479900</v>
@@ -19875,7 +19889,7 @@
         <v>8</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E192" s="2">
         <v>3959000</v>
@@ -19886,13 +19900,13 @@
         <v>121</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E193" s="2">
         <v>2890000</v>
@@ -19903,13 +19917,13 @@
         <v>121</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E194" s="2">
         <v>4080000</v>
@@ -19920,13 +19934,13 @@
         <v>121</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E195" s="2">
         <v>6290000</v>
@@ -19934,7 +19948,7 @@
     </row>
     <row r="196" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A196" s="1" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="B196" s="2">
         <v>6</v>
@@ -19943,7 +19957,7 @@
         <v>8</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E196" s="2">
         <v>2200000</v>
@@ -19951,7 +19965,7 @@
     </row>
     <row r="197" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A197" s="1" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>284</v>
@@ -19960,7 +19974,7 @@
         <v>8</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E197" s="2">
         <v>4599000</v>
@@ -19977,7 +19991,7 @@
         <v>8</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E198" s="2">
         <v>2199000</v>
@@ -19988,13 +20002,13 @@
         <v>215</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E199" s="2">
         <v>4599000</v>
@@ -20005,13 +20019,13 @@
         <v>105</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E200" s="2">
         <v>1990000</v>
@@ -20022,13 +20036,13 @@
         <v>105</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E201" s="2">
         <v>3590000</v>
@@ -20045,7 +20059,7 @@
         <v>8</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E202" s="2">
         <v>2650000</v>
@@ -20056,13 +20070,13 @@
         <v>215</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E203" s="2">
         <v>2849000</v>
@@ -20070,7 +20084,7 @@
     </row>
     <row r="204" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A204" s="1" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>171</v>
@@ -20079,7 +20093,7 @@
         <v>8</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E204" s="2">
         <v>2099000</v>
@@ -20096,7 +20110,7 @@
         <v>8</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="E205" s="2">
         <v>1263000</v>
@@ -20113,7 +20127,7 @@
         <v>8</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E206" s="2">
         <v>1546500</v>
@@ -20130,7 +20144,7 @@
         <v>8</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="E207" s="2">
         <v>883000</v>
@@ -20147,7 +20161,7 @@
         <v>8</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="E208" s="2">
         <v>825000</v>
@@ -20164,7 +20178,7 @@
         <v>8</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="E209" s="2">
         <v>851000</v>
@@ -20175,13 +20189,13 @@
         <v>176</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E210" s="2">
         <v>3357990</v>
@@ -20192,13 +20206,13 @@
         <v>215</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E211" s="2">
         <v>3899000</v>
@@ -20215,7 +20229,7 @@
         <v>8</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E212" s="2">
         <v>1990000</v>
@@ -20232,7 +20246,7 @@
         <v>8</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E213" s="2">
         <v>2199000</v>
@@ -20249,7 +20263,7 @@
         <v>8</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="E214" s="2">
         <v>789900</v>
@@ -20266,7 +20280,7 @@
         <v>51</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="E215" s="2">
         <v>869900</v>
@@ -20283,7 +20297,7 @@
         <v>8</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="E216" s="2">
         <v>1089000</v>
@@ -20300,7 +20314,7 @@
         <v>8</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="E217" s="2">
         <v>999900</v>
@@ -20317,7 +20331,7 @@
         <v>8</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="E218" s="2">
         <v>1455000</v>
@@ -20334,7 +20348,7 @@
         <v>103</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="E219" s="2">
         <v>809900</v>
@@ -20351,7 +20365,7 @@
         <v>8</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="E220" s="2">
         <v>2000000</v>
@@ -20368,7 +20382,7 @@
         <v>8</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="E221" s="2">
         <v>1229900</v>
@@ -20385,7 +20399,7 @@
         <v>8</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="E222" s="2">
         <v>2656800</v>
@@ -20396,13 +20410,13 @@
         <v>344</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="E223" s="2">
         <v>824000</v>
@@ -20413,13 +20427,13 @@
         <v>300</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="E224" s="2">
         <v>1204900</v>
@@ -20436,7 +20450,7 @@
         <v>8</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="E225" s="2">
         <v>2234900</v>
@@ -20444,7 +20458,7 @@
     </row>
     <row r="226" ht="40.35" customHeight="1" spans="1:5">
       <c r="A226" s="1" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>138</v>
@@ -20453,7 +20467,7 @@
         <v>5</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="E226" s="2">
         <v>2673000</v>
@@ -20470,7 +20484,7 @@
         <v>8</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="E227" s="2">
         <v>1419990</v>
@@ -20478,7 +20492,7 @@
     </row>
     <row r="228" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A228" s="1" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>277</v>
@@ -20487,7 +20501,7 @@
         <v>8</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="E228" s="2">
         <v>1494000</v>
@@ -20504,7 +20518,7 @@
         <v>8</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E229" s="2">
         <v>2849990</v>
@@ -20518,10 +20532,10 @@
         <v>591</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E230" s="2">
         <v>3173000</v>
@@ -20532,13 +20546,13 @@
         <v>54</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E231" s="2">
         <v>2380000</v>
@@ -20555,7 +20569,7 @@
         <v>8</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E232" s="2">
         <v>2599000</v>
@@ -20563,16 +20577,16 @@
     </row>
     <row r="233" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A233" s="1" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E233" s="2">
         <v>2999000</v>
@@ -20583,13 +20597,13 @@
         <v>22</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>312</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E234" s="2">
         <v>3590000</v>
@@ -20597,16 +20611,16 @@
     </row>
     <row r="235" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A235" s="1" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E235" s="2">
         <v>2569900</v>
@@ -20623,7 +20637,7 @@
         <v>8</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E236" s="2">
         <v>4750000</v>
@@ -20631,16 +20645,16 @@
     </row>
     <row r="237" ht="40.35" customHeight="1" spans="1:5">
       <c r="A237" s="1" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E237" s="2">
         <v>2499990</v>
@@ -20648,7 +20662,7 @@
     </row>
     <row r="238" ht="27.15" customHeight="1" spans="1:5">
       <c r="A238" s="1" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>793</v>
@@ -20657,7 +20671,7 @@
         <v>8</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E238" s="2">
         <v>2779990</v>
@@ -20674,7 +20688,7 @@
         <v>51</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E239" s="2">
         <v>2649000</v>
@@ -20691,7 +20705,7 @@
         <v>5</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E240" s="2">
         <v>1899000</v>
@@ -20708,7 +20722,7 @@
         <v>8</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E241" s="2">
         <v>2825990</v>
@@ -20716,7 +20730,7 @@
     </row>
     <row r="242" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A242" s="1" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B242" s="2">
         <v>400</v>
@@ -20725,7 +20739,7 @@
         <v>8</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E242" s="2">
         <v>5799000</v>
@@ -20733,7 +20747,7 @@
     </row>
     <row r="243" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A243" s="1" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>280</v>
@@ -20742,7 +20756,7 @@
         <v>8</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="E243" s="2">
         <v>2899000</v>
@@ -20759,7 +20773,7 @@
         <v>8</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E244" s="2">
         <v>1887500</v>
@@ -20776,7 +20790,7 @@
         <v>8</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E245" s="2">
         <v>1805000</v>
@@ -20793,7 +20807,7 @@
         <v>8</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E246" s="2">
         <v>1684500</v>
@@ -20801,7 +20815,7 @@
     </row>
     <row r="247" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A247" s="1" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>785</v>
@@ -20810,7 +20824,7 @@
         <v>8</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E247" s="2">
         <v>3899000</v>
@@ -20818,7 +20832,7 @@
     </row>
     <row r="248" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A248" s="1" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>784</v>
@@ -20827,7 +20841,7 @@
         <v>8</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E248" s="2">
         <v>3099000</v>
@@ -20835,7 +20849,7 @@
     </row>
     <row r="249" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A249" s="1" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="B249" s="2">
         <v>1</v>
@@ -20844,7 +20858,7 @@
         <v>8</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E249" s="2">
         <v>4162990</v>

</xml_diff>

<commit_message>
del 25 sites, add cars
</commit_message>
<xml_diff>
--- a/id.xlsx
+++ b/id.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$G$925</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$G$933</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Лист2!$A$1:$E$249</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3079" uniqueCount="1092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3095" uniqueCount="1098">
   <si>
     <t>Aito</t>
   </si>
@@ -2975,6 +2975,24 @@
   </si>
   <si>
     <t>H7 New</t>
+  </si>
+  <si>
+    <t>GS4 Max</t>
+  </si>
+  <si>
+    <t>Huge</t>
+  </si>
+  <si>
+    <t>Mage</t>
+  </si>
+  <si>
+    <t>BJ90</t>
+  </si>
+  <si>
+    <t>GWM POER New</t>
+  </si>
+  <si>
+    <t>Granta Active Cross Liftback</t>
   </si>
   <si>
     <t>Марка</t>
@@ -4013,6 +4031,13 @@
 </styleSheet>
 </file>
 
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4298,10 +4323,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G926"/>
+  <dimension ref="A1:G934"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A905" workbookViewId="0">
-      <selection activeCell="D925" sqref="D925"/>
+    <sheetView tabSelected="1" topLeftCell="A914" workbookViewId="0">
+      <selection activeCell="C934" sqref="C934"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -16611,8 +16636,96 @@
         <v>980</v>
       </c>
     </row>
+    <row r="927" spans="1:3">
+      <c r="A927">
+        <v>1026</v>
+      </c>
+      <c r="B927" t="s">
+        <v>164</v>
+      </c>
+      <c r="C927" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="928" spans="1:3">
+      <c r="A928">
+        <v>1027</v>
+      </c>
+      <c r="B928" t="s">
+        <v>415</v>
+      </c>
+      <c r="C928" s="4" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="929" spans="1:3">
+      <c r="A929">
+        <v>1028</v>
+      </c>
+      <c r="B929" t="s">
+        <v>105</v>
+      </c>
+      <c r="C929" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="930" spans="1:3">
+      <c r="A930">
+        <v>1029</v>
+      </c>
+      <c r="B930" t="s">
+        <v>105</v>
+      </c>
+      <c r="C930" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="931" spans="1:3">
+      <c r="A931">
+        <v>1030</v>
+      </c>
+      <c r="B931" t="s">
+        <v>3</v>
+      </c>
+      <c r="C931" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="932" spans="1:3">
+      <c r="A932">
+        <v>1031</v>
+      </c>
+      <c r="B932" t="s">
+        <v>215</v>
+      </c>
+      <c r="C932" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="933" spans="1:3">
+      <c r="A933">
+        <v>1032</v>
+      </c>
+      <c r="B933" t="s">
+        <v>271</v>
+      </c>
+      <c r="C933" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="934" spans="1:3">
+      <c r="A934">
+        <v>1033</v>
+      </c>
+      <c r="B934" t="s">
+        <v>344</v>
+      </c>
+      <c r="C934" t="s">
+        <v>986</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G925" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G933" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -16633,19 +16746,19 @@
   <sheetData>
     <row r="1" ht="27.15" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>981</v>
+        <v>987</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>982</v>
+        <v>988</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>985</v>
+        <v>991</v>
       </c>
     </row>
     <row r="2" ht="40.35" hidden="1" customHeight="1" spans="1:5">
@@ -16653,13 +16766,13 @@
         <v>344</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>986</v>
+        <v>992</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>380</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E2" s="2">
         <v>1239900</v>
@@ -16676,7 +16789,7 @@
         <v>380</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E3" s="2">
         <v>1759000</v>
@@ -16693,7 +16806,7 @@
         <v>380</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E4" s="2">
         <v>1655000</v>
@@ -16710,7 +16823,7 @@
         <v>380</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E5" s="2">
         <v>1879000</v>
@@ -16721,13 +16834,13 @@
         <v>344</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>988</v>
+        <v>994</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="E6" s="2">
         <v>1077000</v>
@@ -16744,7 +16857,7 @@
         <v>82</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>990</v>
+        <v>996</v>
       </c>
       <c r="E7" s="2">
         <v>1408000</v>
@@ -16755,13 +16868,13 @@
         <v>344</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>991</v>
+        <v>997</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="E8" s="2">
         <v>749900</v>
@@ -16778,7 +16891,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="E9" s="2">
         <v>1175000</v>
@@ -16795,7 +16908,7 @@
         <v>252</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>992</v>
+        <v>998</v>
       </c>
       <c r="E10" s="2">
         <v>2149000</v>
@@ -16812,7 +16925,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E11" s="2">
         <v>1660000</v>
@@ -16829,7 +16942,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E12" s="2">
         <v>2020000</v>
@@ -16846,7 +16959,7 @@
         <v>103</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>994</v>
+        <v>1000</v>
       </c>
       <c r="E13" s="2">
         <v>1859000</v>
@@ -16863,7 +16976,7 @@
         <v>303</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E14" s="2">
         <v>1334900</v>
@@ -16874,13 +16987,13 @@
         <v>176</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>995</v>
+        <v>1001</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E15" s="2">
         <v>3512990</v>
@@ -16897,7 +17010,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E16" s="2">
         <v>2836990</v>
@@ -16914,7 +17027,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>997</v>
+        <v>1003</v>
       </c>
       <c r="E17" s="2">
         <v>1850000</v>
@@ -16931,7 +17044,7 @@
         <v>270</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E18" s="2">
         <v>2749000</v>
@@ -16948,7 +17061,7 @@
         <v>103</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E19" s="2">
         <v>2179990</v>
@@ -16959,13 +17072,13 @@
         <v>176</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>999</v>
+        <v>1005</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E20" s="2">
         <v>2794990</v>
@@ -16982,7 +17095,7 @@
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E21" s="2">
         <v>3959990</v>
@@ -16990,7 +17103,7 @@
     </row>
     <row r="22" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>1000</v>
+        <v>1006</v>
       </c>
       <c r="B22" s="2">
         <v>300</v>
@@ -16999,7 +17112,7 @@
         <v>8</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E22" s="2">
         <v>4499000</v>
@@ -17007,7 +17120,7 @@
     </row>
     <row r="23" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>1000</v>
+        <v>1006</v>
       </c>
       <c r="B23" s="2">
         <v>500</v>
@@ -17016,7 +17129,7 @@
         <v>8</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E23" s="2">
         <v>6799000</v>
@@ -17027,13 +17140,13 @@
         <v>344</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="E24" s="2">
         <v>778500</v>
@@ -17044,13 +17157,13 @@
         <v>344</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1002</v>
+        <v>1008</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="E25" s="2">
         <v>719300</v>
@@ -17061,13 +17174,13 @@
         <v>344</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1003</v>
+        <v>1009</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="E26" s="2">
         <v>950900</v>
@@ -17084,7 +17197,7 @@
         <v>380</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E27" s="2">
         <v>1316900</v>
@@ -17095,13 +17208,13 @@
         <v>242</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1004</v>
+        <v>1010</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>264</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1005</v>
+        <v>1011</v>
       </c>
       <c r="E28" s="2">
         <v>2769000</v>
@@ -17118,7 +17231,7 @@
         <v>303</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E29" s="2">
         <v>2244900</v>
@@ -17135,7 +17248,7 @@
         <v>259</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>990</v>
+        <v>996</v>
       </c>
       <c r="E30" s="2">
         <v>1574900</v>
@@ -17152,7 +17265,7 @@
         <v>259</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>990</v>
+        <v>996</v>
       </c>
       <c r="E31" s="2">
         <v>1434900</v>
@@ -17163,13 +17276,13 @@
         <v>344</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1006</v>
+        <v>1012</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E32" s="2">
         <v>1059000</v>
@@ -17186,7 +17299,7 @@
         <v>259</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>992</v>
+        <v>998</v>
       </c>
       <c r="E33" s="2">
         <v>3969000</v>
@@ -17203,7 +17316,7 @@
         <v>8</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E34" s="2">
         <v>1314000</v>
@@ -17214,13 +17327,13 @@
         <v>215</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1009</v>
+        <v>1015</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E35" s="2">
         <v>2149000</v>
@@ -17237,7 +17350,7 @@
         <v>5</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>1011</v>
+        <v>1017</v>
       </c>
       <c r="E36" s="2">
         <v>2599000</v>
@@ -17248,13 +17361,13 @@
         <v>215</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1012</v>
+        <v>1018</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>1011</v>
+        <v>1017</v>
       </c>
       <c r="E37" s="2">
         <v>2599000</v>
@@ -17271,7 +17384,7 @@
         <v>8</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>1013</v>
+        <v>1019</v>
       </c>
       <c r="E38" s="2">
         <v>5269000</v>
@@ -17288,7 +17401,7 @@
         <v>303</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E39" s="2">
         <v>2314900</v>
@@ -17299,13 +17412,13 @@
         <v>344</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>1014</v>
+        <v>1020</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E40" s="2">
         <v>918900</v>
@@ -17322,7 +17435,7 @@
         <v>259</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E41" s="2">
         <v>2159900</v>
@@ -17339,7 +17452,7 @@
         <v>8</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>1015</v>
+        <v>1021</v>
       </c>
       <c r="E42" s="2">
         <v>1106900</v>
@@ -17356,7 +17469,7 @@
         <v>8</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>1015</v>
+        <v>1021</v>
       </c>
       <c r="E43" s="2">
         <v>1249900</v>
@@ -17373,7 +17486,7 @@
         <v>8</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E44" s="2">
         <v>2900000</v>
@@ -17384,13 +17497,13 @@
         <v>22</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>1016</v>
+        <v>1022</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E45" s="2">
         <v>2439900</v>
@@ -17407,7 +17520,7 @@
         <v>312</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="E46" s="2">
         <v>2734900</v>
@@ -17424,7 +17537,7 @@
         <v>312</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="E47" s="2">
         <v>1934900</v>
@@ -17441,7 +17554,7 @@
         <v>8</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="E48" s="2">
         <v>2064900</v>
@@ -17458,7 +17571,7 @@
         <v>334</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E49" s="2">
         <v>2849900</v>
@@ -17466,7 +17579,7 @@
     </row>
     <row r="50" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A50" s="1" t="s">
-        <v>1018</v>
+        <v>1024</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>279</v>
@@ -17475,7 +17588,7 @@
         <v>8</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E50" s="2">
         <v>1779000</v>
@@ -17483,7 +17596,7 @@
     </row>
     <row r="51" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>1018</v>
+        <v>1024</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>273</v>
@@ -17492,7 +17605,7 @@
         <v>8</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E51" s="2">
         <v>2150000</v>
@@ -17500,7 +17613,7 @@
     </row>
     <row r="52" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A52" s="1" t="s">
-        <v>1019</v>
+        <v>1025</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>278</v>
@@ -17509,7 +17622,7 @@
         <v>8</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E52" s="2">
         <v>2129900</v>
@@ -17517,7 +17630,7 @@
     </row>
     <row r="53" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>1019</v>
+        <v>1025</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>472</v>
@@ -17526,7 +17639,7 @@
         <v>8</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E53" s="2">
         <v>2369900</v>
@@ -17543,7 +17656,7 @@
         <v>8</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="E54" s="2">
         <v>1690000</v>
@@ -17560,7 +17673,7 @@
         <v>8</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E55" s="2">
         <v>2869900</v>
@@ -17571,13 +17684,13 @@
         <v>22</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1020</v>
+        <v>1026</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E56" s="2">
         <v>2569900</v>
@@ -17588,13 +17701,13 @@
         <v>22</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1021</v>
+        <v>1027</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E57" s="2">
         <v>2839900</v>
@@ -17611,7 +17724,7 @@
         <v>26</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E58" s="2">
         <v>3969900</v>
@@ -17628,7 +17741,7 @@
         <v>26</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E59" s="2">
         <v>3069900</v>
@@ -17645,7 +17758,7 @@
         <v>26</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E60" s="2">
         <v>3069900</v>
@@ -17656,13 +17769,13 @@
         <v>22</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>1022</v>
+        <v>1028</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>1023</v>
+        <v>1029</v>
       </c>
       <c r="E61" s="2">
         <v>2899900</v>
@@ -17670,7 +17783,7 @@
     </row>
     <row r="62" ht="40.35" customHeight="1" spans="1:5">
       <c r="A62" s="1" t="s">
-        <v>1024</v>
+        <v>1030</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>135</v>
@@ -17679,7 +17792,7 @@
         <v>26</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E62" s="2">
         <v>2374000</v>
@@ -17687,7 +17800,7 @@
     </row>
     <row r="63" ht="40.35" customHeight="1" spans="1:5">
       <c r="A63" s="1" t="s">
-        <v>1024</v>
+        <v>1030</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>136</v>
@@ -17696,7 +17809,7 @@
         <v>26</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E63" s="2">
         <v>2411000</v>
@@ -17704,7 +17817,7 @@
     </row>
     <row r="64" ht="40.35" customHeight="1" spans="1:5">
       <c r="A64" s="1" t="s">
-        <v>1024</v>
+        <v>1030</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>137</v>
@@ -17713,7 +17826,7 @@
         <v>26</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="E64" s="2">
         <v>2024000</v>
@@ -17730,7 +17843,7 @@
         <v>82</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>1013</v>
+        <v>1019</v>
       </c>
       <c r="E65" s="2">
         <v>1124000</v>
@@ -17747,7 +17860,7 @@
         <v>103</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E66" s="2">
         <v>1051000</v>
@@ -17764,7 +17877,7 @@
         <v>534</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="E67" s="2">
         <v>1657000</v>
@@ -17781,7 +17894,7 @@
         <v>5</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E68" s="2">
         <v>1705000</v>
@@ -17798,7 +17911,7 @@
         <v>5</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1025</v>
+        <v>1031</v>
       </c>
       <c r="E69" s="2">
         <v>1699900</v>
@@ -17815,7 +17928,7 @@
         <v>26</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E70" s="2">
         <v>2489900</v>
@@ -17823,7 +17936,7 @@
     </row>
     <row r="71" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A71" s="1" t="s">
-        <v>1026</v>
+        <v>1032</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>273</v>
@@ -17832,7 +17945,7 @@
         <v>26</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E71" s="2">
         <v>2959900</v>
@@ -17840,7 +17953,7 @@
     </row>
     <row r="72" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A72" s="1" t="s">
-        <v>1027</v>
+        <v>1033</v>
       </c>
       <c r="B72" s="2">
         <v>3</v>
@@ -17849,7 +17962,7 @@
         <v>26</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E72" s="2">
         <v>1765000</v>
@@ -17866,7 +17979,7 @@
         <v>226</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1028</v>
+        <v>1034</v>
       </c>
       <c r="E73" s="2">
         <v>4409000</v>
@@ -17883,7 +17996,7 @@
         <v>226</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>1028</v>
+        <v>1034</v>
       </c>
       <c r="E74" s="2">
         <v>1690000</v>
@@ -17900,7 +18013,7 @@
         <v>85</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E75" s="2">
         <v>950900</v>
@@ -17917,7 +18030,7 @@
         <v>8</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E76" s="2">
         <v>880900</v>
@@ -17934,7 +18047,7 @@
         <v>82</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E77" s="2">
         <v>953900</v>
@@ -17951,7 +18064,7 @@
         <v>103</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E78" s="2">
         <v>2179000</v>
@@ -17968,7 +18081,7 @@
         <v>8</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>1029</v>
+        <v>1035</v>
       </c>
       <c r="E79" s="2">
         <v>1579000</v>
@@ -17985,7 +18098,7 @@
         <v>5</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E80" s="2">
         <v>4299000</v>
@@ -18002,7 +18115,7 @@
         <v>8</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>1030</v>
+        <v>1036</v>
       </c>
       <c r="E81" s="2">
         <v>2049000</v>
@@ -18019,7 +18132,7 @@
         <v>8</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E82" s="2">
         <v>3149000</v>
@@ -18036,7 +18149,7 @@
         <v>82</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>1031</v>
+        <v>1037</v>
       </c>
       <c r="E83" s="2">
         <v>2337000</v>
@@ -18047,13 +18160,13 @@
         <v>457</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>1032</v>
+        <v>1038</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>303</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>1031</v>
+        <v>1037</v>
       </c>
       <c r="E84" s="2">
         <v>2762000</v>
@@ -18070,7 +18183,7 @@
         <v>103</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E85" s="2">
         <v>1618000</v>
@@ -18087,7 +18200,7 @@
         <v>82</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>1013</v>
+        <v>1019</v>
       </c>
       <c r="E86" s="2">
         <v>1301000</v>
@@ -18104,7 +18217,7 @@
         <v>82</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>1013</v>
+        <v>1019</v>
       </c>
       <c r="E87" s="2">
         <v>1258000</v>
@@ -18121,7 +18234,7 @@
         <v>82</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>1013</v>
+        <v>1019</v>
       </c>
       <c r="E88" s="2">
         <v>1373000</v>
@@ -18138,7 +18251,7 @@
         <v>5</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>990</v>
+        <v>996</v>
       </c>
       <c r="E89" s="2">
         <v>1724000</v>
@@ -18155,7 +18268,7 @@
         <v>8</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="E90" s="2">
         <v>1874000</v>
@@ -18172,7 +18285,7 @@
         <v>5</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E91" s="2">
         <v>2057000</v>
@@ -18189,7 +18302,7 @@
         <v>5</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E92" s="2">
         <v>2118900</v>
@@ -18206,7 +18319,7 @@
         <v>5</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E93" s="2">
         <v>3248000</v>
@@ -18223,7 +18336,7 @@
         <v>5</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E94" s="2">
         <v>5378000</v>
@@ -18240,7 +18353,7 @@
         <v>5</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E95" s="2">
         <v>5806000</v>
@@ -18257,7 +18370,7 @@
         <v>303</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="E96" s="2">
         <v>2388000</v>
@@ -18274,7 +18387,7 @@
         <v>303</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="E97" s="2">
         <v>2681000</v>
@@ -18291,7 +18404,7 @@
         <v>617</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>990</v>
+        <v>996</v>
       </c>
       <c r="E98" s="2">
         <v>1385900</v>
@@ -18308,7 +18421,7 @@
         <v>608</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>1033</v>
+        <v>1039</v>
       </c>
       <c r="E99" s="2">
         <v>1518000</v>
@@ -18325,7 +18438,7 @@
         <v>82</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E100" s="2">
         <v>3375900</v>
@@ -18342,7 +18455,7 @@
         <v>8</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E101" s="2">
         <v>2828900</v>
@@ -18359,7 +18472,7 @@
         <v>5</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="E102" s="2">
         <v>4449900</v>
@@ -18376,7 +18489,7 @@
         <v>8</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>1034</v>
+        <v>1040</v>
       </c>
       <c r="E103" s="2">
         <v>1229000</v>
@@ -18393,7 +18506,7 @@
         <v>103</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E104" s="2">
         <v>2499000</v>
@@ -18401,7 +18514,7 @@
     </row>
     <row r="105" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A105" s="1" t="s">
-        <v>1035</v>
+        <v>1041</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>595</v>
@@ -18410,7 +18523,7 @@
         <v>596</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>1036</v>
+        <v>1042</v>
       </c>
       <c r="E105" s="2">
         <v>1680000</v>
@@ -18418,16 +18531,16 @@
     </row>
     <row r="106" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A106" s="1" t="s">
-        <v>1035</v>
+        <v>1041</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>1037</v>
+        <v>1043</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>596</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>1036</v>
+        <v>1042</v>
       </c>
       <c r="E106" s="2">
         <v>1705000</v>
@@ -18435,7 +18548,7 @@
     </row>
     <row r="107" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A107" s="1" t="s">
-        <v>1035</v>
+        <v>1041</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>39</v>
@@ -18444,7 +18557,7 @@
         <v>8</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>1038</v>
+        <v>1044</v>
       </c>
       <c r="E107" s="2">
         <v>1510000</v>
@@ -18461,7 +18574,7 @@
         <v>8</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E108" s="2">
         <v>2570000</v>
@@ -18478,7 +18591,7 @@
         <v>8</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E109" s="2">
         <v>3430000</v>
@@ -18489,13 +18602,13 @@
         <v>54</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>1039</v>
+        <v>1045</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E110" s="2">
         <v>2770000</v>
@@ -18512,7 +18625,7 @@
         <v>5</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E111" s="2">
         <v>1970000</v>
@@ -18523,13 +18636,13 @@
         <v>54</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E112" s="2">
         <v>3250000</v>
@@ -18540,13 +18653,13 @@
         <v>54</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>1041</v>
+        <v>1047</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E113" s="2">
         <v>3370000</v>
@@ -18563,7 +18676,7 @@
         <v>8</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="E114" s="2">
         <v>3759900</v>
@@ -18580,7 +18693,7 @@
         <v>5</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E115" s="2">
         <v>3380000</v>
@@ -18597,7 +18710,7 @@
         <v>5</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E116" s="2">
         <v>3810000</v>
@@ -18614,7 +18727,7 @@
         <v>8</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E117" s="2">
         <v>4910000</v>
@@ -18631,7 +18744,7 @@
         <v>8</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E118" s="2">
         <v>4550000</v>
@@ -18648,7 +18761,7 @@
         <v>8</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E119" s="2">
         <v>2080000</v>
@@ -18665,7 +18778,7 @@
         <v>8</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="E120" s="2">
         <v>2225000</v>
@@ -18682,7 +18795,7 @@
         <v>8</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E121" s="2">
         <v>2970000</v>
@@ -18699,7 +18812,7 @@
         <v>5</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="E122" s="2">
         <v>4350000</v>
@@ -18716,7 +18829,7 @@
         <v>5</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E123" s="2">
         <v>2999900</v>
@@ -18733,7 +18846,7 @@
         <v>8</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E124" s="2">
         <v>3479900</v>
@@ -18750,7 +18863,7 @@
         <v>5</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E125" s="2">
         <v>1990000</v>
@@ -18767,7 +18880,7 @@
         <v>5</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E126" s="2">
         <v>2149000</v>
@@ -18784,7 +18897,7 @@
         <v>8</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E127" s="2">
         <v>2115000</v>
@@ -18801,7 +18914,7 @@
         <v>8</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E128" s="2">
         <v>2238000</v>
@@ -18818,7 +18931,7 @@
         <v>8</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E129" s="2">
         <v>2514900</v>
@@ -18835,7 +18948,7 @@
         <v>8</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E130" s="2">
         <v>2997900</v>
@@ -18843,16 +18956,16 @@
     </row>
     <row r="131" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A131" s="1" t="s">
-        <v>1042</v>
+        <v>1048</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>1043</v>
+        <v>1049</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E131" s="2">
         <v>2549900</v>
@@ -18860,16 +18973,16 @@
     </row>
     <row r="132" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A132" s="1" t="s">
-        <v>1042</v>
+        <v>1048</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>1044</v>
+        <v>1050</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E132" s="2">
         <v>2629900</v>
@@ -18877,16 +18990,16 @@
     </row>
     <row r="133" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A133" s="1" t="s">
-        <v>1027</v>
+        <v>1033</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>1045</v>
+        <v>1051</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E133" s="2">
         <v>4100000</v>
@@ -18903,7 +19016,7 @@
         <v>8</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>1031</v>
+        <v>1037</v>
       </c>
       <c r="E134" s="2">
         <v>2219900</v>
@@ -18914,13 +19027,13 @@
         <v>22</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>1046</v>
+        <v>1052</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="E135" s="2">
         <v>2499900</v>
@@ -18928,7 +19041,7 @@
     </row>
     <row r="136" ht="27.15" customHeight="1" spans="1:5">
       <c r="A136" s="1" t="s">
-        <v>1024</v>
+        <v>1030</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>145</v>
@@ -18937,7 +19050,7 @@
         <v>8</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>1047</v>
+        <v>1053</v>
       </c>
       <c r="E136" s="2">
         <v>1602000</v>
@@ -18945,7 +19058,7 @@
     </row>
     <row r="137" ht="40.35" customHeight="1" spans="1:5">
       <c r="A137" s="1" t="s">
-        <v>1024</v>
+        <v>1030</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>146</v>
@@ -18954,7 +19067,7 @@
         <v>5</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>1013</v>
+        <v>1019</v>
       </c>
       <c r="E137" s="2">
         <v>1508000</v>
@@ -18971,7 +19084,7 @@
         <v>8</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E138" s="2">
         <v>4549990</v>
@@ -18988,7 +19101,7 @@
         <v>8</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E139" s="2">
         <v>2479990</v>
@@ -19005,7 +19118,7 @@
         <v>8</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>1048</v>
+        <v>1054</v>
       </c>
       <c r="E140" s="2">
         <v>2075990</v>
@@ -19022,7 +19135,7 @@
         <v>8</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="E141" s="2">
         <v>2080990</v>
@@ -19039,7 +19152,7 @@
         <v>380</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E142" s="2">
         <v>2273000</v>
@@ -19056,7 +19169,7 @@
         <v>380</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E143" s="2">
         <v>2443000</v>
@@ -19073,7 +19186,7 @@
         <v>5</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="E144" s="2">
         <v>1341000</v>
@@ -19084,13 +19197,13 @@
         <v>344</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>1049</v>
+        <v>1055</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="E145" s="2">
         <v>1381000</v>
@@ -19101,13 +19214,13 @@
         <v>344</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>1050</v>
+        <v>1056</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="E146" s="2">
         <v>1493000</v>
@@ -19118,13 +19231,13 @@
         <v>344</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>1051</v>
+        <v>1057</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="E147" s="2">
         <v>1533000</v>
@@ -19141,7 +19254,7 @@
         <v>5</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E148" s="2">
         <v>1670000</v>
@@ -19158,7 +19271,7 @@
         <v>8</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E149" s="2">
         <v>1487000</v>
@@ -19169,13 +19282,13 @@
         <v>54</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>1052</v>
+        <v>1058</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E150" s="2">
         <v>4850000</v>
@@ -19186,13 +19299,13 @@
         <v>54</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>1053</v>
+        <v>1059</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E151" s="2">
         <v>4000000</v>
@@ -19203,13 +19316,13 @@
         <v>54</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>1054</v>
+        <v>1060</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E152" s="2">
         <v>4930000</v>
@@ -19226,7 +19339,7 @@
         <v>5</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E153" s="2">
         <v>3692990</v>
@@ -19243,7 +19356,7 @@
         <v>270</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E154" s="2">
         <v>3979000</v>
@@ -19260,7 +19373,7 @@
         <v>8</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E155" s="2">
         <v>4099000</v>
@@ -19277,7 +19390,7 @@
         <v>8</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E156" s="2">
         <v>3449000</v>
@@ -19294,7 +19407,7 @@
         <v>8</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E157" s="2">
         <v>2799000</v>
@@ -19305,13 +19418,13 @@
         <v>200</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>1055</v>
+        <v>1061</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="E158" s="2">
         <v>3549000</v>
@@ -19322,13 +19435,13 @@
         <v>200</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>1056</v>
+        <v>1062</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E159" s="2">
         <v>3299000</v>
@@ -19345,7 +19458,7 @@
         <v>330</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E160" s="2">
         <v>7374900</v>
@@ -19362,7 +19475,7 @@
         <v>270</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E161" s="2">
         <v>3789900</v>
@@ -19379,7 +19492,7 @@
         <v>51</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="E162" s="2">
         <v>5829900</v>
@@ -19396,7 +19509,7 @@
         <v>270</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E163" s="2">
         <v>4144900</v>
@@ -19404,16 +19517,16 @@
     </row>
     <row r="164" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A164" s="1" t="s">
-        <v>1042</v>
+        <v>1048</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>1057</v>
+        <v>1063</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E164" s="2">
         <v>1672000</v>
@@ -19430,7 +19543,7 @@
         <v>8</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E165" s="2">
         <v>2040546</v>
@@ -19447,7 +19560,7 @@
         <v>8</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E166" s="2">
         <v>3100000</v>
@@ -19464,7 +19577,7 @@
         <v>8</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E167" s="2">
         <v>2990000</v>
@@ -19481,7 +19594,7 @@
         <v>312</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>1025</v>
+        <v>1031</v>
       </c>
       <c r="E168" s="2">
         <v>8669500</v>
@@ -19498,7 +19611,7 @@
         <v>677</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="E169" s="2">
         <v>4291000</v>
@@ -19515,7 +19628,7 @@
         <v>5</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E170" s="2">
         <v>6146500</v>
@@ -19523,7 +19636,7 @@
     </row>
     <row r="171" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A171" s="1" t="s">
-        <v>1018</v>
+        <v>1024</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>274</v>
@@ -19532,7 +19645,7 @@
         <v>8</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E171" s="2">
         <v>1889000</v>
@@ -19540,7 +19653,7 @@
     </row>
     <row r="172" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A172" s="1" t="s">
-        <v>1018</v>
+        <v>1024</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>276</v>
@@ -19549,7 +19662,7 @@
         <v>8</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E172" s="2">
         <v>2399000</v>
@@ -19557,7 +19670,7 @@
     </row>
     <row r="173" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A173" s="1" t="s">
-        <v>1018</v>
+        <v>1024</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>653</v>
@@ -19566,7 +19679,7 @@
         <v>8</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E173" s="2">
         <v>3059000</v>
@@ -19574,16 +19687,16 @@
     </row>
     <row r="174" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A174" s="1" t="s">
-        <v>1018</v>
+        <v>1024</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>1058</v>
+        <v>1064</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E174" s="2">
         <v>3279000</v>
@@ -19591,7 +19704,7 @@
     </row>
     <row r="175" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A175" s="1" t="s">
-        <v>1018</v>
+        <v>1024</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>654</v>
@@ -19600,7 +19713,7 @@
         <v>8</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E175" s="2">
         <v>3599000</v>
@@ -19608,7 +19721,7 @@
     </row>
     <row r="176" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A176" s="1" t="s">
-        <v>1059</v>
+        <v>1065</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>175</v>
@@ -19617,7 +19730,7 @@
         <v>8</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E176" s="2">
         <v>5499999</v>
@@ -19625,7 +19738,7 @@
     </row>
     <row r="177" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A177" s="1" t="s">
-        <v>1059</v>
+        <v>1065</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>172</v>
@@ -19634,7 +19747,7 @@
         <v>103</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E177" s="2">
         <v>4099000</v>
@@ -19642,7 +19755,7 @@
     </row>
     <row r="178" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A178" s="1" t="s">
-        <v>1059</v>
+        <v>1065</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>169</v>
@@ -19651,7 +19764,7 @@
         <v>8</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E178" s="2">
         <v>2449000</v>
@@ -19662,13 +19775,13 @@
         <v>22</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>1060</v>
+        <v>1066</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E179" s="2">
         <v>4529900</v>
@@ -19685,7 +19798,7 @@
         <v>8</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E180" s="2">
         <v>3739900</v>
@@ -19696,13 +19809,13 @@
         <v>22</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>1061</v>
+        <v>1067</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E181" s="2">
         <v>5219900</v>
@@ -19713,13 +19826,13 @@
         <v>54</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>1062</v>
+        <v>1068</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E182" s="2">
         <v>2780000</v>
@@ -19736,7 +19849,7 @@
         <v>8</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E183" s="2">
         <v>2020000</v>
@@ -19753,7 +19866,7 @@
         <v>8</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E184" s="2">
         <v>2650000</v>
@@ -19770,7 +19883,7 @@
         <v>8</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E185" s="2">
         <v>2080000</v>
@@ -19787,7 +19900,7 @@
         <v>8</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E186" s="2">
         <v>2181000</v>
@@ -19804,7 +19917,7 @@
         <v>5</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E187" s="2">
         <v>2279000</v>
@@ -19821,7 +19934,7 @@
         <v>103</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="E188" s="2">
         <v>2899000</v>
@@ -19838,7 +19951,7 @@
         <v>82</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="E189" s="2">
         <v>2379000</v>
@@ -19846,16 +19959,16 @@
     </row>
     <row r="190" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A190" s="1" t="s">
-        <v>1063</v>
+        <v>1069</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>1064</v>
+        <v>1070</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E190" s="2">
         <v>2499000</v>
@@ -19863,7 +19976,7 @@
     </row>
     <row r="191" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A191" s="1" t="s">
-        <v>1019</v>
+        <v>1025</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>473</v>
@@ -19872,7 +19985,7 @@
         <v>8</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E191" s="2">
         <v>2479900</v>
@@ -19889,7 +20002,7 @@
         <v>8</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E192" s="2">
         <v>3959000</v>
@@ -19900,13 +20013,13 @@
         <v>121</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>1065</v>
+        <v>1071</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E193" s="2">
         <v>2890000</v>
@@ -19917,13 +20030,13 @@
         <v>121</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>1066</v>
+        <v>1072</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E194" s="2">
         <v>4080000</v>
@@ -19934,13 +20047,13 @@
         <v>121</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>1067</v>
+        <v>1073</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E195" s="2">
         <v>6290000</v>
@@ -19948,7 +20061,7 @@
     </row>
     <row r="196" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A196" s="1" t="s">
-        <v>1027</v>
+        <v>1033</v>
       </c>
       <c r="B196" s="2">
         <v>6</v>
@@ -19957,7 +20070,7 @@
         <v>8</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E196" s="2">
         <v>2200000</v>
@@ -19965,7 +20078,7 @@
     </row>
     <row r="197" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A197" s="1" t="s">
-        <v>1026</v>
+        <v>1032</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>284</v>
@@ -19974,7 +20087,7 @@
         <v>8</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E197" s="2">
         <v>4599000</v>
@@ -19991,7 +20104,7 @@
         <v>8</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E198" s="2">
         <v>2199000</v>
@@ -20002,13 +20115,13 @@
         <v>215</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>1068</v>
+        <v>1074</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E199" s="2">
         <v>4599000</v>
@@ -20019,13 +20132,13 @@
         <v>105</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>1069</v>
+        <v>1075</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E200" s="2">
         <v>1990000</v>
@@ -20036,13 +20149,13 @@
         <v>105</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>1070</v>
+        <v>1076</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E201" s="2">
         <v>3590000</v>
@@ -20059,7 +20172,7 @@
         <v>8</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="E202" s="2">
         <v>2650000</v>
@@ -20070,13 +20183,13 @@
         <v>215</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>1071</v>
+        <v>1077</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E203" s="2">
         <v>2849000</v>
@@ -20084,7 +20197,7 @@
     </row>
     <row r="204" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A204" s="1" t="s">
-        <v>1059</v>
+        <v>1065</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>171</v>
@@ -20093,7 +20206,7 @@
         <v>8</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E204" s="2">
         <v>2099000</v>
@@ -20110,7 +20223,7 @@
         <v>8</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>1072</v>
+        <v>1078</v>
       </c>
       <c r="E205" s="2">
         <v>1263000</v>
@@ -20127,7 +20240,7 @@
         <v>8</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="E206" s="2">
         <v>1546500</v>
@@ -20144,7 +20257,7 @@
         <v>8</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>1073</v>
+        <v>1079</v>
       </c>
       <c r="E207" s="2">
         <v>883000</v>
@@ -20161,7 +20274,7 @@
         <v>8</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>1074</v>
+        <v>1080</v>
       </c>
       <c r="E208" s="2">
         <v>825000</v>
@@ -20178,7 +20291,7 @@
         <v>8</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>1073</v>
+        <v>1079</v>
       </c>
       <c r="E209" s="2">
         <v>851000</v>
@@ -20189,13 +20302,13 @@
         <v>176</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>1075</v>
+        <v>1081</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E210" s="2">
         <v>3357990</v>
@@ -20206,13 +20319,13 @@
         <v>215</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>1076</v>
+        <v>1082</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E211" s="2">
         <v>3899000</v>
@@ -20229,7 +20342,7 @@
         <v>8</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E212" s="2">
         <v>1990000</v>
@@ -20246,7 +20359,7 @@
         <v>8</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E213" s="2">
         <v>2199000</v>
@@ -20263,7 +20376,7 @@
         <v>8</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>1034</v>
+        <v>1040</v>
       </c>
       <c r="E214" s="2">
         <v>789900</v>
@@ -20280,7 +20393,7 @@
         <v>51</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>1077</v>
+        <v>1083</v>
       </c>
       <c r="E215" s="2">
         <v>869900</v>
@@ -20297,7 +20410,7 @@
         <v>8</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>1078</v>
+        <v>1084</v>
       </c>
       <c r="E216" s="2">
         <v>1089000</v>
@@ -20314,7 +20427,7 @@
         <v>8</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>1073</v>
+        <v>1079</v>
       </c>
       <c r="E217" s="2">
         <v>999900</v>
@@ -20331,7 +20444,7 @@
         <v>8</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>1074</v>
+        <v>1080</v>
       </c>
       <c r="E218" s="2">
         <v>1455000</v>
@@ -20348,7 +20461,7 @@
         <v>103</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>1077</v>
+        <v>1083</v>
       </c>
       <c r="E219" s="2">
         <v>809900</v>
@@ -20365,7 +20478,7 @@
         <v>8</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E220" s="2">
         <v>2000000</v>
@@ -20382,7 +20495,7 @@
         <v>8</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>1073</v>
+        <v>1079</v>
       </c>
       <c r="E221" s="2">
         <v>1229900</v>
@@ -20399,7 +20512,7 @@
         <v>8</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>1013</v>
+        <v>1019</v>
       </c>
       <c r="E222" s="2">
         <v>2656800</v>
@@ -20410,13 +20523,13 @@
         <v>344</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>1079</v>
+        <v>1085</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>1029</v>
+        <v>1035</v>
       </c>
       <c r="E223" s="2">
         <v>824000</v>
@@ -20427,13 +20540,13 @@
         <v>300</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>1080</v>
+        <v>1086</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>1033</v>
+        <v>1039</v>
       </c>
       <c r="E224" s="2">
         <v>1204900</v>
@@ -20450,7 +20563,7 @@
         <v>8</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>1005</v>
+        <v>1011</v>
       </c>
       <c r="E225" s="2">
         <v>2234900</v>
@@ -20458,7 +20571,7 @@
     </row>
     <row r="226" ht="40.35" customHeight="1" spans="1:5">
       <c r="A226" s="1" t="s">
-        <v>1024</v>
+        <v>1030</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>138</v>
@@ -20467,7 +20580,7 @@
         <v>5</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>1011</v>
+        <v>1017</v>
       </c>
       <c r="E226" s="2">
         <v>2673000</v>
@@ -20484,7 +20597,7 @@
         <v>8</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>1081</v>
+        <v>1087</v>
       </c>
       <c r="E227" s="2">
         <v>1419990</v>
@@ -20492,7 +20605,7 @@
     </row>
     <row r="228" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A228" s="1" t="s">
-        <v>1018</v>
+        <v>1024</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>277</v>
@@ -20501,7 +20614,7 @@
         <v>8</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>1082</v>
+        <v>1088</v>
       </c>
       <c r="E228" s="2">
         <v>1494000</v>
@@ -20518,7 +20631,7 @@
         <v>8</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E229" s="2">
         <v>2849990</v>
@@ -20532,10 +20645,10 @@
         <v>591</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>1083</v>
+        <v>1089</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="E230" s="2">
         <v>3173000</v>
@@ -20546,13 +20659,13 @@
         <v>54</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>1084</v>
+        <v>1090</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E231" s="2">
         <v>2380000</v>
@@ -20569,7 +20682,7 @@
         <v>8</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E232" s="2">
         <v>2599000</v>
@@ -20577,16 +20690,16 @@
     </row>
     <row r="233" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A233" s="1" t="s">
-        <v>1063</v>
+        <v>1069</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>1085</v>
+        <v>1091</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E233" s="2">
         <v>2999000</v>
@@ -20597,13 +20710,13 @@
         <v>22</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>1086</v>
+        <v>1092</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>312</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E234" s="2">
         <v>3590000</v>
@@ -20611,16 +20724,16 @@
     </row>
     <row r="235" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A235" s="1" t="s">
-        <v>1019</v>
+        <v>1025</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>1087</v>
+        <v>1093</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E235" s="2">
         <v>2569900</v>
@@ -20637,7 +20750,7 @@
         <v>8</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E236" s="2">
         <v>4750000</v>
@@ -20645,16 +20758,16 @@
     </row>
     <row r="237" ht="40.35" customHeight="1" spans="1:5">
       <c r="A237" s="1" t="s">
-        <v>1024</v>
+        <v>1030</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>1088</v>
+        <v>1094</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E237" s="2">
         <v>2499990</v>
@@ -20662,7 +20775,7 @@
     </row>
     <row r="238" ht="27.15" customHeight="1" spans="1:5">
       <c r="A238" s="1" t="s">
-        <v>1024</v>
+        <v>1030</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>793</v>
@@ -20671,7 +20784,7 @@
         <v>8</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E238" s="2">
         <v>2779990</v>
@@ -20688,7 +20801,7 @@
         <v>51</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E239" s="2">
         <v>2649000</v>
@@ -20705,7 +20818,7 @@
         <v>5</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="E240" s="2">
         <v>1899000</v>
@@ -20722,7 +20835,7 @@
         <v>8</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E241" s="2">
         <v>2825990</v>
@@ -20730,7 +20843,7 @@
     </row>
     <row r="242" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A242" s="1" t="s">
-        <v>1000</v>
+        <v>1006</v>
       </c>
       <c r="B242" s="2">
         <v>400</v>
@@ -20739,7 +20852,7 @@
         <v>8</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="E242" s="2">
         <v>5799000</v>
@@ -20747,7 +20860,7 @@
     </row>
     <row r="243" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A243" s="1" t="s">
-        <v>1018</v>
+        <v>1024</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>280</v>
@@ -20756,7 +20869,7 @@
         <v>8</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>1089</v>
+        <v>1095</v>
       </c>
       <c r="E243" s="2">
         <v>2899000</v>
@@ -20773,7 +20886,7 @@
         <v>8</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="E244" s="2">
         <v>1887500</v>
@@ -20790,7 +20903,7 @@
         <v>8</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="E245" s="2">
         <v>1805000</v>
@@ -20807,7 +20920,7 @@
         <v>8</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="E246" s="2">
         <v>1684500</v>
@@ -20815,7 +20928,7 @@
     </row>
     <row r="247" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A247" s="1" t="s">
-        <v>1090</v>
+        <v>1096</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>785</v>
@@ -20824,7 +20937,7 @@
         <v>8</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E247" s="2">
         <v>3899000</v>
@@ -20832,7 +20945,7 @@
     </row>
     <row r="248" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A248" s="1" t="s">
-        <v>1090</v>
+        <v>1096</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>784</v>
@@ -20841,7 +20954,7 @@
         <v>8</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E248" s="2">
         <v>3099000</v>
@@ -20849,7 +20962,7 @@
     </row>
     <row r="249" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A249" s="1" t="s">
-        <v>1091</v>
+        <v>1097</v>
       </c>
       <c r="B249" s="2">
         <v>1</v>
@@ -20858,7 +20971,7 @@
         <v>8</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="E249" s="2">
         <v>4162990</v>

</xml_diff>

<commit_message>
Add 6 cars (15 min)
</commit_message>
<xml_diff>
--- a/id.xlsx
+++ b/id.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$G$933</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$G$934</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Лист2!$A$1:$E$249</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3095" uniqueCount="1098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3105" uniqueCount="1103">
   <si>
     <t>Aito</t>
   </si>
@@ -2993,6 +2993,21 @@
   </si>
   <si>
     <t>Granta Active Cross Liftback</t>
+  </si>
+  <si>
+    <t>Corolla Cross</t>
+  </si>
+  <si>
+    <t>Xiaomi</t>
+  </si>
+  <si>
+    <t>YU7</t>
+  </si>
+  <si>
+    <t>UNI-V New</t>
+  </si>
+  <si>
+    <t>Niva Legend 3 двери Sport</t>
   </si>
   <si>
     <t>Марка</t>
@@ -4323,10 +4338,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G934"/>
+  <dimension ref="A1:G939"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A914" workbookViewId="0">
-      <selection activeCell="C934" sqref="C934"/>
+      <selection activeCell="G933" sqref="G933"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -16724,8 +16739,63 @@
         <v>986</v>
       </c>
     </row>
+    <row r="935" spans="1:3">
+      <c r="A935">
+        <v>1034</v>
+      </c>
+      <c r="B935" t="s">
+        <v>576</v>
+      </c>
+      <c r="C935" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="936" spans="1:3">
+      <c r="A936">
+        <v>1035</v>
+      </c>
+      <c r="B936" t="s">
+        <v>988</v>
+      </c>
+      <c r="C936" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="937" spans="1:3">
+      <c r="A937">
+        <v>1036</v>
+      </c>
+      <c r="B937" t="s">
+        <v>686</v>
+      </c>
+      <c r="C937" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="938" spans="1:3">
+      <c r="A938">
+        <v>1037</v>
+      </c>
+      <c r="B938" t="s">
+        <v>22</v>
+      </c>
+      <c r="C938" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="939" spans="1:3">
+      <c r="A939">
+        <v>1038</v>
+      </c>
+      <c r="B939" t="s">
+        <v>344</v>
+      </c>
+      <c r="C939" t="s">
+        <v>991</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G933" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G934" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -16746,19 +16816,19 @@
   <sheetData>
     <row r="1" ht="27.15" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>987</v>
+        <v>992</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>988</v>
+        <v>993</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>989</v>
+        <v>994</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>990</v>
+        <v>995</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>991</v>
+        <v>996</v>
       </c>
     </row>
     <row r="2" ht="40.35" hidden="1" customHeight="1" spans="1:5">
@@ -16766,13 +16836,13 @@
         <v>344</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>992</v>
+        <v>997</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>380</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E2" s="2">
         <v>1239900</v>
@@ -16789,7 +16859,7 @@
         <v>380</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E3" s="2">
         <v>1759000</v>
@@ -16806,7 +16876,7 @@
         <v>380</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E4" s="2">
         <v>1655000</v>
@@ -16823,7 +16893,7 @@
         <v>380</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E5" s="2">
         <v>1879000</v>
@@ -16834,13 +16904,13 @@
         <v>344</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>994</v>
+        <v>999</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="E6" s="2">
         <v>1077000</v>
@@ -16857,7 +16927,7 @@
         <v>82</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="E7" s="2">
         <v>1408000</v>
@@ -16868,13 +16938,13 @@
         <v>344</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>997</v>
+        <v>1002</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="E8" s="2">
         <v>749900</v>
@@ -16891,7 +16961,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="E9" s="2">
         <v>1175000</v>
@@ -16908,7 +16978,7 @@
         <v>252</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>998</v>
+        <v>1003</v>
       </c>
       <c r="E10" s="2">
         <v>2149000</v>
@@ -16925,7 +16995,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E11" s="2">
         <v>1660000</v>
@@ -16942,7 +17012,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E12" s="2">
         <v>2020000</v>
@@ -16959,7 +17029,7 @@
         <v>103</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1000</v>
+        <v>1005</v>
       </c>
       <c r="E13" s="2">
         <v>1859000</v>
@@ -16976,7 +17046,7 @@
         <v>303</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E14" s="2">
         <v>1334900</v>
@@ -16987,13 +17057,13 @@
         <v>176</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1001</v>
+        <v>1006</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E15" s="2">
         <v>3512990</v>
@@ -17010,7 +17080,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E16" s="2">
         <v>2836990</v>
@@ -17027,7 +17097,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>1003</v>
+        <v>1008</v>
       </c>
       <c r="E17" s="2">
         <v>1850000</v>
@@ -17044,7 +17114,7 @@
         <v>270</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1004</v>
+        <v>1009</v>
       </c>
       <c r="E18" s="2">
         <v>2749000</v>
@@ -17061,7 +17131,7 @@
         <v>103</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E19" s="2">
         <v>2179990</v>
@@ -17072,13 +17142,13 @@
         <v>176</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1005</v>
+        <v>1010</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E20" s="2">
         <v>2794990</v>
@@ -17095,7 +17165,7 @@
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E21" s="2">
         <v>3959990</v>
@@ -17103,7 +17173,7 @@
     </row>
     <row r="22" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>1006</v>
+        <v>1011</v>
       </c>
       <c r="B22" s="2">
         <v>300</v>
@@ -17112,7 +17182,7 @@
         <v>8</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E22" s="2">
         <v>4499000</v>
@@ -17120,7 +17190,7 @@
     </row>
     <row r="23" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>1006</v>
+        <v>1011</v>
       </c>
       <c r="B23" s="2">
         <v>500</v>
@@ -17129,7 +17199,7 @@
         <v>8</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E23" s="2">
         <v>6799000</v>
@@ -17140,13 +17210,13 @@
         <v>344</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1007</v>
+        <v>1012</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="E24" s="2">
         <v>778500</v>
@@ -17157,13 +17227,13 @@
         <v>344</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1008</v>
+        <v>1013</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="E25" s="2">
         <v>719300</v>
@@ -17174,13 +17244,13 @@
         <v>344</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1009</v>
+        <v>1014</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="E26" s="2">
         <v>950900</v>
@@ -17197,7 +17267,7 @@
         <v>380</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E27" s="2">
         <v>1316900</v>
@@ -17208,13 +17278,13 @@
         <v>242</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1010</v>
+        <v>1015</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>264</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1011</v>
+        <v>1016</v>
       </c>
       <c r="E28" s="2">
         <v>2769000</v>
@@ -17231,7 +17301,7 @@
         <v>303</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E29" s="2">
         <v>2244900</v>
@@ -17248,7 +17318,7 @@
         <v>259</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="E30" s="2">
         <v>1574900</v>
@@ -17265,7 +17335,7 @@
         <v>259</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="E31" s="2">
         <v>1434900</v>
@@ -17276,13 +17346,13 @@
         <v>344</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1012</v>
+        <v>1017</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E32" s="2">
         <v>1059000</v>
@@ -17299,7 +17369,7 @@
         <v>259</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>998</v>
+        <v>1003</v>
       </c>
       <c r="E33" s="2">
         <v>3969000</v>
@@ -17316,7 +17386,7 @@
         <v>8</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>1014</v>
+        <v>1019</v>
       </c>
       <c r="E34" s="2">
         <v>1314000</v>
@@ -17327,13 +17397,13 @@
         <v>215</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1015</v>
+        <v>1020</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E35" s="2">
         <v>2149000</v>
@@ -17350,7 +17420,7 @@
         <v>5</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>1017</v>
+        <v>1022</v>
       </c>
       <c r="E36" s="2">
         <v>2599000</v>
@@ -17361,13 +17431,13 @@
         <v>215</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1018</v>
+        <v>1023</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>1017</v>
+        <v>1022</v>
       </c>
       <c r="E37" s="2">
         <v>2599000</v>
@@ -17384,7 +17454,7 @@
         <v>8</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>1019</v>
+        <v>1024</v>
       </c>
       <c r="E38" s="2">
         <v>5269000</v>
@@ -17401,7 +17471,7 @@
         <v>303</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E39" s="2">
         <v>2314900</v>
@@ -17412,13 +17482,13 @@
         <v>344</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>1020</v>
+        <v>1025</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E40" s="2">
         <v>918900</v>
@@ -17435,7 +17505,7 @@
         <v>259</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E41" s="2">
         <v>2159900</v>
@@ -17452,7 +17522,7 @@
         <v>8</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>1021</v>
+        <v>1026</v>
       </c>
       <c r="E42" s="2">
         <v>1106900</v>
@@ -17469,7 +17539,7 @@
         <v>8</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>1021</v>
+        <v>1026</v>
       </c>
       <c r="E43" s="2">
         <v>1249900</v>
@@ -17486,7 +17556,7 @@
         <v>8</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E44" s="2">
         <v>2900000</v>
@@ -17497,13 +17567,13 @@
         <v>22</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>1022</v>
+        <v>1027</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E45" s="2">
         <v>2439900</v>
@@ -17520,7 +17590,7 @@
         <v>312</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
       <c r="E46" s="2">
         <v>2734900</v>
@@ -17537,7 +17607,7 @@
         <v>312</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
       <c r="E47" s="2">
         <v>1934900</v>
@@ -17554,7 +17624,7 @@
         <v>8</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
       <c r="E48" s="2">
         <v>2064900</v>
@@ -17571,7 +17641,7 @@
         <v>334</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E49" s="2">
         <v>2849900</v>
@@ -17579,7 +17649,7 @@
     </row>
     <row r="50" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A50" s="1" t="s">
-        <v>1024</v>
+        <v>1029</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>279</v>
@@ -17588,7 +17658,7 @@
         <v>8</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E50" s="2">
         <v>1779000</v>
@@ -17596,7 +17666,7 @@
     </row>
     <row r="51" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>1024</v>
+        <v>1029</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>273</v>
@@ -17605,7 +17675,7 @@
         <v>8</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E51" s="2">
         <v>2150000</v>
@@ -17613,7 +17683,7 @@
     </row>
     <row r="52" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A52" s="1" t="s">
-        <v>1025</v>
+        <v>1030</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>278</v>
@@ -17622,7 +17692,7 @@
         <v>8</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E52" s="2">
         <v>2129900</v>
@@ -17630,7 +17700,7 @@
     </row>
     <row r="53" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>1025</v>
+        <v>1030</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>472</v>
@@ -17639,7 +17709,7 @@
         <v>8</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E53" s="2">
         <v>2369900</v>
@@ -17656,7 +17726,7 @@
         <v>8</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
       <c r="E54" s="2">
         <v>1690000</v>
@@ -17673,7 +17743,7 @@
         <v>8</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E55" s="2">
         <v>2869900</v>
@@ -17684,13 +17754,13 @@
         <v>22</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1026</v>
+        <v>1031</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E56" s="2">
         <v>2569900</v>
@@ -17701,13 +17771,13 @@
         <v>22</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1027</v>
+        <v>1032</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E57" s="2">
         <v>2839900</v>
@@ -17724,7 +17794,7 @@
         <v>26</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E58" s="2">
         <v>3969900</v>
@@ -17741,7 +17811,7 @@
         <v>26</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E59" s="2">
         <v>3069900</v>
@@ -17758,7 +17828,7 @@
         <v>26</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E60" s="2">
         <v>3069900</v>
@@ -17769,13 +17839,13 @@
         <v>22</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>1028</v>
+        <v>1033</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>1029</v>
+        <v>1034</v>
       </c>
       <c r="E61" s="2">
         <v>2899900</v>
@@ -17783,7 +17853,7 @@
     </row>
     <row r="62" ht="40.35" customHeight="1" spans="1:5">
       <c r="A62" s="1" t="s">
-        <v>1030</v>
+        <v>1035</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>135</v>
@@ -17792,7 +17862,7 @@
         <v>26</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E62" s="2">
         <v>2374000</v>
@@ -17800,7 +17870,7 @@
     </row>
     <row r="63" ht="40.35" customHeight="1" spans="1:5">
       <c r="A63" s="1" t="s">
-        <v>1030</v>
+        <v>1035</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>136</v>
@@ -17809,7 +17879,7 @@
         <v>26</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E63" s="2">
         <v>2411000</v>
@@ -17817,7 +17887,7 @@
     </row>
     <row r="64" ht="40.35" customHeight="1" spans="1:5">
       <c r="A64" s="1" t="s">
-        <v>1030</v>
+        <v>1035</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>137</v>
@@ -17826,7 +17896,7 @@
         <v>26</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="E64" s="2">
         <v>2024000</v>
@@ -17843,7 +17913,7 @@
         <v>82</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>1019</v>
+        <v>1024</v>
       </c>
       <c r="E65" s="2">
         <v>1124000</v>
@@ -17860,7 +17930,7 @@
         <v>103</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E66" s="2">
         <v>1051000</v>
@@ -17877,7 +17947,7 @@
         <v>534</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
       <c r="E67" s="2">
         <v>1657000</v>
@@ -17894,7 +17964,7 @@
         <v>5</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E68" s="2">
         <v>1705000</v>
@@ -17911,7 +17981,7 @@
         <v>5</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1031</v>
+        <v>1036</v>
       </c>
       <c r="E69" s="2">
         <v>1699900</v>
@@ -17928,7 +17998,7 @@
         <v>26</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E70" s="2">
         <v>2489900</v>
@@ -17936,7 +18006,7 @@
     </row>
     <row r="71" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A71" s="1" t="s">
-        <v>1032</v>
+        <v>1037</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>273</v>
@@ -17945,7 +18015,7 @@
         <v>26</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E71" s="2">
         <v>2959900</v>
@@ -17953,7 +18023,7 @@
     </row>
     <row r="72" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A72" s="1" t="s">
-        <v>1033</v>
+        <v>1038</v>
       </c>
       <c r="B72" s="2">
         <v>3</v>
@@ -17962,7 +18032,7 @@
         <v>26</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E72" s="2">
         <v>1765000</v>
@@ -17979,7 +18049,7 @@
         <v>226</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1034</v>
+        <v>1039</v>
       </c>
       <c r="E73" s="2">
         <v>4409000</v>
@@ -17996,7 +18066,7 @@
         <v>226</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>1034</v>
+        <v>1039</v>
       </c>
       <c r="E74" s="2">
         <v>1690000</v>
@@ -18013,7 +18083,7 @@
         <v>85</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E75" s="2">
         <v>950900</v>
@@ -18030,7 +18100,7 @@
         <v>8</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>1014</v>
+        <v>1019</v>
       </c>
       <c r="E76" s="2">
         <v>880900</v>
@@ -18047,7 +18117,7 @@
         <v>82</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E77" s="2">
         <v>953900</v>
@@ -18064,7 +18134,7 @@
         <v>103</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E78" s="2">
         <v>2179000</v>
@@ -18081,7 +18151,7 @@
         <v>8</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>1035</v>
+        <v>1040</v>
       </c>
       <c r="E79" s="2">
         <v>1579000</v>
@@ -18098,7 +18168,7 @@
         <v>5</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>1014</v>
+        <v>1019</v>
       </c>
       <c r="E80" s="2">
         <v>4299000</v>
@@ -18115,7 +18185,7 @@
         <v>8</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>1036</v>
+        <v>1041</v>
       </c>
       <c r="E81" s="2">
         <v>2049000</v>
@@ -18132,7 +18202,7 @@
         <v>8</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E82" s="2">
         <v>3149000</v>
@@ -18149,7 +18219,7 @@
         <v>82</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>1037</v>
+        <v>1042</v>
       </c>
       <c r="E83" s="2">
         <v>2337000</v>
@@ -18160,13 +18230,13 @@
         <v>457</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>1038</v>
+        <v>1043</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>303</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>1037</v>
+        <v>1042</v>
       </c>
       <c r="E84" s="2">
         <v>2762000</v>
@@ -18183,7 +18253,7 @@
         <v>103</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E85" s="2">
         <v>1618000</v>
@@ -18200,7 +18270,7 @@
         <v>82</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>1019</v>
+        <v>1024</v>
       </c>
       <c r="E86" s="2">
         <v>1301000</v>
@@ -18217,7 +18287,7 @@
         <v>82</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>1019</v>
+        <v>1024</v>
       </c>
       <c r="E87" s="2">
         <v>1258000</v>
@@ -18234,7 +18304,7 @@
         <v>82</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>1019</v>
+        <v>1024</v>
       </c>
       <c r="E88" s="2">
         <v>1373000</v>
@@ -18251,7 +18321,7 @@
         <v>5</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="E89" s="2">
         <v>1724000</v>
@@ -18268,7 +18338,7 @@
         <v>8</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
       <c r="E90" s="2">
         <v>1874000</v>
@@ -18285,7 +18355,7 @@
         <v>5</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E91" s="2">
         <v>2057000</v>
@@ -18302,7 +18372,7 @@
         <v>5</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E92" s="2">
         <v>2118900</v>
@@ -18319,7 +18389,7 @@
         <v>5</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E93" s="2">
         <v>3248000</v>
@@ -18336,7 +18406,7 @@
         <v>5</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E94" s="2">
         <v>5378000</v>
@@ -18353,7 +18423,7 @@
         <v>5</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E95" s="2">
         <v>5806000</v>
@@ -18370,7 +18440,7 @@
         <v>303</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
       <c r="E96" s="2">
         <v>2388000</v>
@@ -18387,7 +18457,7 @@
         <v>303</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
       <c r="E97" s="2">
         <v>2681000</v>
@@ -18404,7 +18474,7 @@
         <v>617</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="E98" s="2">
         <v>1385900</v>
@@ -18421,7 +18491,7 @@
         <v>608</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>1039</v>
+        <v>1044</v>
       </c>
       <c r="E99" s="2">
         <v>1518000</v>
@@ -18438,7 +18508,7 @@
         <v>82</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E100" s="2">
         <v>3375900</v>
@@ -18455,7 +18525,7 @@
         <v>8</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E101" s="2">
         <v>2828900</v>
@@ -18472,7 +18542,7 @@
         <v>5</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
       <c r="E102" s="2">
         <v>4449900</v>
@@ -18489,7 +18559,7 @@
         <v>8</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>1040</v>
+        <v>1045</v>
       </c>
       <c r="E103" s="2">
         <v>1229000</v>
@@ -18506,7 +18576,7 @@
         <v>103</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E104" s="2">
         <v>2499000</v>
@@ -18514,7 +18584,7 @@
     </row>
     <row r="105" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A105" s="1" t="s">
-        <v>1041</v>
+        <v>1046</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>595</v>
@@ -18523,7 +18593,7 @@
         <v>596</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>1042</v>
+        <v>1047</v>
       </c>
       <c r="E105" s="2">
         <v>1680000</v>
@@ -18531,16 +18601,16 @@
     </row>
     <row r="106" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A106" s="1" t="s">
-        <v>1041</v>
+        <v>1046</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>1043</v>
+        <v>1048</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>596</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>1042</v>
+        <v>1047</v>
       </c>
       <c r="E106" s="2">
         <v>1705000</v>
@@ -18548,7 +18618,7 @@
     </row>
     <row r="107" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A107" s="1" t="s">
-        <v>1041</v>
+        <v>1046</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>39</v>
@@ -18557,7 +18627,7 @@
         <v>8</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>1044</v>
+        <v>1049</v>
       </c>
       <c r="E107" s="2">
         <v>1510000</v>
@@ -18574,7 +18644,7 @@
         <v>8</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E108" s="2">
         <v>2570000</v>
@@ -18591,7 +18661,7 @@
         <v>8</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E109" s="2">
         <v>3430000</v>
@@ -18602,13 +18672,13 @@
         <v>54</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>1045</v>
+        <v>1050</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E110" s="2">
         <v>2770000</v>
@@ -18625,7 +18695,7 @@
         <v>5</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E111" s="2">
         <v>1970000</v>
@@ -18636,13 +18706,13 @@
         <v>54</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>1046</v>
+        <v>1051</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E112" s="2">
         <v>3250000</v>
@@ -18653,13 +18723,13 @@
         <v>54</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>1047</v>
+        <v>1052</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E113" s="2">
         <v>3370000</v>
@@ -18676,7 +18746,7 @@
         <v>8</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
       <c r="E114" s="2">
         <v>3759900</v>
@@ -18693,7 +18763,7 @@
         <v>5</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E115" s="2">
         <v>3380000</v>
@@ -18710,7 +18780,7 @@
         <v>5</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E116" s="2">
         <v>3810000</v>
@@ -18727,7 +18797,7 @@
         <v>8</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E117" s="2">
         <v>4910000</v>
@@ -18744,7 +18814,7 @@
         <v>8</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E118" s="2">
         <v>4550000</v>
@@ -18761,7 +18831,7 @@
         <v>8</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E119" s="2">
         <v>2080000</v>
@@ -18778,7 +18848,7 @@
         <v>8</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
       <c r="E120" s="2">
         <v>2225000</v>
@@ -18795,7 +18865,7 @@
         <v>8</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E121" s="2">
         <v>2970000</v>
@@ -18812,7 +18882,7 @@
         <v>5</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
       <c r="E122" s="2">
         <v>4350000</v>
@@ -18829,7 +18899,7 @@
         <v>5</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E123" s="2">
         <v>2999900</v>
@@ -18846,7 +18916,7 @@
         <v>8</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E124" s="2">
         <v>3479900</v>
@@ -18863,7 +18933,7 @@
         <v>5</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E125" s="2">
         <v>1990000</v>
@@ -18880,7 +18950,7 @@
         <v>5</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E126" s="2">
         <v>2149000</v>
@@ -18897,7 +18967,7 @@
         <v>8</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E127" s="2">
         <v>2115000</v>
@@ -18914,7 +18984,7 @@
         <v>8</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E128" s="2">
         <v>2238000</v>
@@ -18931,7 +19001,7 @@
         <v>8</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E129" s="2">
         <v>2514900</v>
@@ -18948,7 +19018,7 @@
         <v>8</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E130" s="2">
         <v>2997900</v>
@@ -18956,16 +19026,16 @@
     </row>
     <row r="131" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A131" s="1" t="s">
-        <v>1048</v>
+        <v>1053</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>1049</v>
+        <v>1054</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E131" s="2">
         <v>2549900</v>
@@ -18973,16 +19043,16 @@
     </row>
     <row r="132" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A132" s="1" t="s">
-        <v>1048</v>
+        <v>1053</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>1050</v>
+        <v>1055</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E132" s="2">
         <v>2629900</v>
@@ -18990,16 +19060,16 @@
     </row>
     <row r="133" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A133" s="1" t="s">
-        <v>1033</v>
+        <v>1038</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>1051</v>
+        <v>1056</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E133" s="2">
         <v>4100000</v>
@@ -19016,7 +19086,7 @@
         <v>8</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>1037</v>
+        <v>1042</v>
       </c>
       <c r="E134" s="2">
         <v>2219900</v>
@@ -19027,13 +19097,13 @@
         <v>22</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>1052</v>
+        <v>1057</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="E135" s="2">
         <v>2499900</v>
@@ -19041,7 +19111,7 @@
     </row>
     <row r="136" ht="27.15" customHeight="1" spans="1:5">
       <c r="A136" s="1" t="s">
-        <v>1030</v>
+        <v>1035</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>145</v>
@@ -19050,7 +19120,7 @@
         <v>8</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>1053</v>
+        <v>1058</v>
       </c>
       <c r="E136" s="2">
         <v>1602000</v>
@@ -19058,7 +19128,7 @@
     </row>
     <row r="137" ht="40.35" customHeight="1" spans="1:5">
       <c r="A137" s="1" t="s">
-        <v>1030</v>
+        <v>1035</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>146</v>
@@ -19067,7 +19137,7 @@
         <v>5</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>1019</v>
+        <v>1024</v>
       </c>
       <c r="E137" s="2">
         <v>1508000</v>
@@ -19084,7 +19154,7 @@
         <v>8</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E138" s="2">
         <v>4549990</v>
@@ -19101,7 +19171,7 @@
         <v>8</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E139" s="2">
         <v>2479990</v>
@@ -19118,7 +19188,7 @@
         <v>8</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>1054</v>
+        <v>1059</v>
       </c>
       <c r="E140" s="2">
         <v>2075990</v>
@@ -19135,7 +19205,7 @@
         <v>8</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
       <c r="E141" s="2">
         <v>2080990</v>
@@ -19152,7 +19222,7 @@
         <v>380</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E142" s="2">
         <v>2273000</v>
@@ -19169,7 +19239,7 @@
         <v>380</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E143" s="2">
         <v>2443000</v>
@@ -19186,7 +19256,7 @@
         <v>5</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="E144" s="2">
         <v>1341000</v>
@@ -19197,13 +19267,13 @@
         <v>344</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>1055</v>
+        <v>1060</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="E145" s="2">
         <v>1381000</v>
@@ -19214,13 +19284,13 @@
         <v>344</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>1056</v>
+        <v>1061</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="E146" s="2">
         <v>1493000</v>
@@ -19231,13 +19301,13 @@
         <v>344</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>1057</v>
+        <v>1062</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="E147" s="2">
         <v>1533000</v>
@@ -19254,7 +19324,7 @@
         <v>5</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E148" s="2">
         <v>1670000</v>
@@ -19271,7 +19341,7 @@
         <v>8</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E149" s="2">
         <v>1487000</v>
@@ -19282,13 +19352,13 @@
         <v>54</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>1058</v>
+        <v>1063</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E150" s="2">
         <v>4850000</v>
@@ -19299,13 +19369,13 @@
         <v>54</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>1059</v>
+        <v>1064</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E151" s="2">
         <v>4000000</v>
@@ -19316,13 +19386,13 @@
         <v>54</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>1060</v>
+        <v>1065</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E152" s="2">
         <v>4930000</v>
@@ -19339,7 +19409,7 @@
         <v>5</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E153" s="2">
         <v>3692990</v>
@@ -19356,7 +19426,7 @@
         <v>270</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>1004</v>
+        <v>1009</v>
       </c>
       <c r="E154" s="2">
         <v>3979000</v>
@@ -19373,7 +19443,7 @@
         <v>8</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E155" s="2">
         <v>4099000</v>
@@ -19390,7 +19460,7 @@
         <v>8</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E156" s="2">
         <v>3449000</v>
@@ -19407,7 +19477,7 @@
         <v>8</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E157" s="2">
         <v>2799000</v>
@@ -19418,13 +19488,13 @@
         <v>200</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>1061</v>
+        <v>1066</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
       <c r="E158" s="2">
         <v>3549000</v>
@@ -19435,13 +19505,13 @@
         <v>200</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>1062</v>
+        <v>1067</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E159" s="2">
         <v>3299000</v>
@@ -19458,7 +19528,7 @@
         <v>330</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E160" s="2">
         <v>7374900</v>
@@ -19475,7 +19545,7 @@
         <v>270</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E161" s="2">
         <v>3789900</v>
@@ -19492,7 +19562,7 @@
         <v>51</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
       <c r="E162" s="2">
         <v>5829900</v>
@@ -19509,7 +19579,7 @@
         <v>270</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E163" s="2">
         <v>4144900</v>
@@ -19517,16 +19587,16 @@
     </row>
     <row r="164" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A164" s="1" t="s">
-        <v>1048</v>
+        <v>1053</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>1063</v>
+        <v>1068</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E164" s="2">
         <v>1672000</v>
@@ -19543,7 +19613,7 @@
         <v>8</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E165" s="2">
         <v>2040546</v>
@@ -19560,7 +19630,7 @@
         <v>8</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E166" s="2">
         <v>3100000</v>
@@ -19577,7 +19647,7 @@
         <v>8</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E167" s="2">
         <v>2990000</v>
@@ -19594,7 +19664,7 @@
         <v>312</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>1031</v>
+        <v>1036</v>
       </c>
       <c r="E168" s="2">
         <v>8669500</v>
@@ -19611,7 +19681,7 @@
         <v>677</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
       <c r="E169" s="2">
         <v>4291000</v>
@@ -19628,7 +19698,7 @@
         <v>5</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E170" s="2">
         <v>6146500</v>
@@ -19636,7 +19706,7 @@
     </row>
     <row r="171" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A171" s="1" t="s">
-        <v>1024</v>
+        <v>1029</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>274</v>
@@ -19645,7 +19715,7 @@
         <v>8</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E171" s="2">
         <v>1889000</v>
@@ -19653,7 +19723,7 @@
     </row>
     <row r="172" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A172" s="1" t="s">
-        <v>1024</v>
+        <v>1029</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>276</v>
@@ -19662,7 +19732,7 @@
         <v>8</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E172" s="2">
         <v>2399000</v>
@@ -19670,7 +19740,7 @@
     </row>
     <row r="173" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A173" s="1" t="s">
-        <v>1024</v>
+        <v>1029</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>653</v>
@@ -19679,7 +19749,7 @@
         <v>8</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E173" s="2">
         <v>3059000</v>
@@ -19687,16 +19757,16 @@
     </row>
     <row r="174" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A174" s="1" t="s">
-        <v>1024</v>
+        <v>1029</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>1064</v>
+        <v>1069</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E174" s="2">
         <v>3279000</v>
@@ -19704,7 +19774,7 @@
     </row>
     <row r="175" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A175" s="1" t="s">
-        <v>1024</v>
+        <v>1029</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>654</v>
@@ -19713,7 +19783,7 @@
         <v>8</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E175" s="2">
         <v>3599000</v>
@@ -19721,7 +19791,7 @@
     </row>
     <row r="176" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A176" s="1" t="s">
-        <v>1065</v>
+        <v>1070</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>175</v>
@@ -19730,7 +19800,7 @@
         <v>8</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E176" s="2">
         <v>5499999</v>
@@ -19738,7 +19808,7 @@
     </row>
     <row r="177" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A177" s="1" t="s">
-        <v>1065</v>
+        <v>1070</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>172</v>
@@ -19747,7 +19817,7 @@
         <v>103</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E177" s="2">
         <v>4099000</v>
@@ -19755,7 +19825,7 @@
     </row>
     <row r="178" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A178" s="1" t="s">
-        <v>1065</v>
+        <v>1070</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>169</v>
@@ -19764,7 +19834,7 @@
         <v>8</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E178" s="2">
         <v>2449000</v>
@@ -19775,13 +19845,13 @@
         <v>22</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>1066</v>
+        <v>1071</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E179" s="2">
         <v>4529900</v>
@@ -19798,7 +19868,7 @@
         <v>8</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E180" s="2">
         <v>3739900</v>
@@ -19809,13 +19879,13 @@
         <v>22</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>1067</v>
+        <v>1072</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E181" s="2">
         <v>5219900</v>
@@ -19826,13 +19896,13 @@
         <v>54</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>1068</v>
+        <v>1073</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E182" s="2">
         <v>2780000</v>
@@ -19849,7 +19919,7 @@
         <v>8</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E183" s="2">
         <v>2020000</v>
@@ -19866,7 +19936,7 @@
         <v>8</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E184" s="2">
         <v>2650000</v>
@@ -19883,7 +19953,7 @@
         <v>8</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E185" s="2">
         <v>2080000</v>
@@ -19900,7 +19970,7 @@
         <v>8</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E186" s="2">
         <v>2181000</v>
@@ -19917,7 +19987,7 @@
         <v>5</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>1014</v>
+        <v>1019</v>
       </c>
       <c r="E187" s="2">
         <v>2279000</v>
@@ -19934,7 +20004,7 @@
         <v>103</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>1014</v>
+        <v>1019</v>
       </c>
       <c r="E188" s="2">
         <v>2899000</v>
@@ -19951,7 +20021,7 @@
         <v>82</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
       <c r="E189" s="2">
         <v>2379000</v>
@@ -19959,16 +20029,16 @@
     </row>
     <row r="190" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A190" s="1" t="s">
-        <v>1069</v>
+        <v>1074</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>1070</v>
+        <v>1075</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E190" s="2">
         <v>2499000</v>
@@ -19976,7 +20046,7 @@
     </row>
     <row r="191" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A191" s="1" t="s">
-        <v>1025</v>
+        <v>1030</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>473</v>
@@ -19985,7 +20055,7 @@
         <v>8</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E191" s="2">
         <v>2479900</v>
@@ -20002,7 +20072,7 @@
         <v>8</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E192" s="2">
         <v>3959000</v>
@@ -20013,13 +20083,13 @@
         <v>121</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>1071</v>
+        <v>1076</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E193" s="2">
         <v>2890000</v>
@@ -20030,13 +20100,13 @@
         <v>121</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>1072</v>
+        <v>1077</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E194" s="2">
         <v>4080000</v>
@@ -20047,13 +20117,13 @@
         <v>121</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>1073</v>
+        <v>1078</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E195" s="2">
         <v>6290000</v>
@@ -20061,7 +20131,7 @@
     </row>
     <row r="196" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A196" s="1" t="s">
-        <v>1033</v>
+        <v>1038</v>
       </c>
       <c r="B196" s="2">
         <v>6</v>
@@ -20070,7 +20140,7 @@
         <v>8</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E196" s="2">
         <v>2200000</v>
@@ -20078,7 +20148,7 @@
     </row>
     <row r="197" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A197" s="1" t="s">
-        <v>1032</v>
+        <v>1037</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>284</v>
@@ -20087,7 +20157,7 @@
         <v>8</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E197" s="2">
         <v>4599000</v>
@@ -20104,7 +20174,7 @@
         <v>8</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E198" s="2">
         <v>2199000</v>
@@ -20115,13 +20185,13 @@
         <v>215</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>1074</v>
+        <v>1079</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E199" s="2">
         <v>4599000</v>
@@ -20132,13 +20202,13 @@
         <v>105</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>1075</v>
+        <v>1080</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E200" s="2">
         <v>1990000</v>
@@ -20149,13 +20219,13 @@
         <v>105</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>1076</v>
+        <v>1081</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E201" s="2">
         <v>3590000</v>
@@ -20172,7 +20242,7 @@
         <v>8</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="E202" s="2">
         <v>2650000</v>
@@ -20183,13 +20253,13 @@
         <v>215</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>1077</v>
+        <v>1082</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E203" s="2">
         <v>2849000</v>
@@ -20197,7 +20267,7 @@
     </row>
     <row r="204" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A204" s="1" t="s">
-        <v>1065</v>
+        <v>1070</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>171</v>
@@ -20206,7 +20276,7 @@
         <v>8</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E204" s="2">
         <v>2099000</v>
@@ -20223,7 +20293,7 @@
         <v>8</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>1078</v>
+        <v>1083</v>
       </c>
       <c r="E205" s="2">
         <v>1263000</v>
@@ -20240,7 +20310,7 @@
         <v>8</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="E206" s="2">
         <v>1546500</v>
@@ -20257,7 +20327,7 @@
         <v>8</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>1079</v>
+        <v>1084</v>
       </c>
       <c r="E207" s="2">
         <v>883000</v>
@@ -20274,7 +20344,7 @@
         <v>8</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>1080</v>
+        <v>1085</v>
       </c>
       <c r="E208" s="2">
         <v>825000</v>
@@ -20291,7 +20361,7 @@
         <v>8</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>1079</v>
+        <v>1084</v>
       </c>
       <c r="E209" s="2">
         <v>851000</v>
@@ -20302,13 +20372,13 @@
         <v>176</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>1081</v>
+        <v>1086</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E210" s="2">
         <v>3357990</v>
@@ -20319,13 +20389,13 @@
         <v>215</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>1082</v>
+        <v>1087</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E211" s="2">
         <v>3899000</v>
@@ -20342,7 +20412,7 @@
         <v>8</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E212" s="2">
         <v>1990000</v>
@@ -20359,7 +20429,7 @@
         <v>8</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E213" s="2">
         <v>2199000</v>
@@ -20376,7 +20446,7 @@
         <v>8</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>1040</v>
+        <v>1045</v>
       </c>
       <c r="E214" s="2">
         <v>789900</v>
@@ -20393,7 +20463,7 @@
         <v>51</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>1083</v>
+        <v>1088</v>
       </c>
       <c r="E215" s="2">
         <v>869900</v>
@@ -20410,7 +20480,7 @@
         <v>8</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>1084</v>
+        <v>1089</v>
       </c>
       <c r="E216" s="2">
         <v>1089000</v>
@@ -20427,7 +20497,7 @@
         <v>8</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>1079</v>
+        <v>1084</v>
       </c>
       <c r="E217" s="2">
         <v>999900</v>
@@ -20444,7 +20514,7 @@
         <v>8</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>1080</v>
+        <v>1085</v>
       </c>
       <c r="E218" s="2">
         <v>1455000</v>
@@ -20461,7 +20531,7 @@
         <v>103</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>1083</v>
+        <v>1088</v>
       </c>
       <c r="E219" s="2">
         <v>809900</v>
@@ -20478,7 +20548,7 @@
         <v>8</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>1004</v>
+        <v>1009</v>
       </c>
       <c r="E220" s="2">
         <v>2000000</v>
@@ -20495,7 +20565,7 @@
         <v>8</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>1079</v>
+        <v>1084</v>
       </c>
       <c r="E221" s="2">
         <v>1229900</v>
@@ -20512,7 +20582,7 @@
         <v>8</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>1019</v>
+        <v>1024</v>
       </c>
       <c r="E222" s="2">
         <v>2656800</v>
@@ -20523,13 +20593,13 @@
         <v>344</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>1085</v>
+        <v>1090</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>1035</v>
+        <v>1040</v>
       </c>
       <c r="E223" s="2">
         <v>824000</v>
@@ -20540,13 +20610,13 @@
         <v>300</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>1086</v>
+        <v>1091</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>1039</v>
+        <v>1044</v>
       </c>
       <c r="E224" s="2">
         <v>1204900</v>
@@ -20563,7 +20633,7 @@
         <v>8</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>1011</v>
+        <v>1016</v>
       </c>
       <c r="E225" s="2">
         <v>2234900</v>
@@ -20571,7 +20641,7 @@
     </row>
     <row r="226" ht="40.35" customHeight="1" spans="1:5">
       <c r="A226" s="1" t="s">
-        <v>1030</v>
+        <v>1035</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>138</v>
@@ -20580,7 +20650,7 @@
         <v>5</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>1017</v>
+        <v>1022</v>
       </c>
       <c r="E226" s="2">
         <v>2673000</v>
@@ -20597,7 +20667,7 @@
         <v>8</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>1087</v>
+        <v>1092</v>
       </c>
       <c r="E227" s="2">
         <v>1419990</v>
@@ -20605,7 +20675,7 @@
     </row>
     <row r="228" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A228" s="1" t="s">
-        <v>1024</v>
+        <v>1029</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>277</v>
@@ -20614,7 +20684,7 @@
         <v>8</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>1088</v>
+        <v>1093</v>
       </c>
       <c r="E228" s="2">
         <v>1494000</v>
@@ -20631,7 +20701,7 @@
         <v>8</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E229" s="2">
         <v>2849990</v>
@@ -20645,10 +20715,10 @@
         <v>591</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>1089</v>
+        <v>1094</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="E230" s="2">
         <v>3173000</v>
@@ -20659,13 +20729,13 @@
         <v>54</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>1090</v>
+        <v>1095</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E231" s="2">
         <v>2380000</v>
@@ -20682,7 +20752,7 @@
         <v>8</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E232" s="2">
         <v>2599000</v>
@@ -20690,16 +20760,16 @@
     </row>
     <row r="233" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A233" s="1" t="s">
-        <v>1069</v>
+        <v>1074</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>1091</v>
+        <v>1096</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E233" s="2">
         <v>2999000</v>
@@ -20710,13 +20780,13 @@
         <v>22</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>1092</v>
+        <v>1097</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>312</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E234" s="2">
         <v>3590000</v>
@@ -20724,16 +20794,16 @@
     </row>
     <row r="235" ht="40.35" hidden="1" customHeight="1" spans="1:5">
       <c r="A235" s="1" t="s">
-        <v>1025</v>
+        <v>1030</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>1093</v>
+        <v>1098</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E235" s="2">
         <v>2569900</v>
@@ -20750,7 +20820,7 @@
         <v>8</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E236" s="2">
         <v>4750000</v>
@@ -20758,16 +20828,16 @@
     </row>
     <row r="237" ht="40.35" customHeight="1" spans="1:5">
       <c r="A237" s="1" t="s">
-        <v>1030</v>
+        <v>1035</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>1094</v>
+        <v>1099</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E237" s="2">
         <v>2499990</v>
@@ -20775,7 +20845,7 @@
     </row>
     <row r="238" ht="27.15" customHeight="1" spans="1:5">
       <c r="A238" s="1" t="s">
-        <v>1030</v>
+        <v>1035</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>793</v>
@@ -20784,7 +20854,7 @@
         <v>8</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E238" s="2">
         <v>2779990</v>
@@ -20801,7 +20871,7 @@
         <v>51</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E239" s="2">
         <v>2649000</v>
@@ -20818,7 +20888,7 @@
         <v>5</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="E240" s="2">
         <v>1899000</v>
@@ -20835,7 +20905,7 @@
         <v>8</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E241" s="2">
         <v>2825990</v>
@@ -20843,7 +20913,7 @@
     </row>
     <row r="242" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A242" s="1" t="s">
-        <v>1006</v>
+        <v>1011</v>
       </c>
       <c r="B242" s="2">
         <v>400</v>
@@ -20852,7 +20922,7 @@
         <v>8</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E242" s="2">
         <v>5799000</v>
@@ -20860,7 +20930,7 @@
     </row>
     <row r="243" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A243" s="1" t="s">
-        <v>1024</v>
+        <v>1029</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>280</v>
@@ -20869,7 +20939,7 @@
         <v>8</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>1095</v>
+        <v>1100</v>
       </c>
       <c r="E243" s="2">
         <v>2899000</v>
@@ -20886,7 +20956,7 @@
         <v>8</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="E244" s="2">
         <v>1887500</v>
@@ -20903,7 +20973,7 @@
         <v>8</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="E245" s="2">
         <v>1805000</v>
@@ -20920,7 +20990,7 @@
         <v>8</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="E246" s="2">
         <v>1684500</v>
@@ -20928,7 +20998,7 @@
     </row>
     <row r="247" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A247" s="1" t="s">
-        <v>1096</v>
+        <v>1101</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>785</v>
@@ -20937,7 +21007,7 @@
         <v>8</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E247" s="2">
         <v>3899000</v>
@@ -20945,7 +21015,7 @@
     </row>
     <row r="248" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A248" s="1" t="s">
-        <v>1096</v>
+        <v>1101</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>784</v>
@@ -20954,7 +21024,7 @@
         <v>8</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E248" s="2">
         <v>3099000</v>
@@ -20962,7 +21032,7 @@
     </row>
     <row r="249" ht="27.15" hidden="1" customHeight="1" spans="1:5">
       <c r="A249" s="1" t="s">
-        <v>1097</v>
+        <v>1102</v>
       </c>
       <c r="B249" s="2">
         <v>1</v>
@@ -20971,7 +21041,7 @@
         <v>8</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="E249" s="2">
         <v>4162990</v>

</xml_diff>